<commit_message>
Standardizing x axes across figures
</commit_message>
<xml_diff>
--- a/Data/Summary.xlsx
+++ b/Data/Summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="360" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="220" yWindow="700" windowWidth="25360" windowHeight="15720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MasterData" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="57">
   <si>
     <t>Month</t>
   </si>
@@ -194,9 +194,6 @@
   <si>
     <t>HCO3(Meq)</t>
   </si>
-  <si>
-    <t>n.a.</t>
-  </si>
 </sst>
 </file>
 
@@ -206,7 +203,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -251,6 +248,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -269,7 +271,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -303,8 +305,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -318,8 +322,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -336,6 +341,7 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -352,6 +358,7 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -681,11 +688,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U110"/>
+  <dimension ref="A1:U109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q49" sqref="Q49:U49"/>
+      <selection pane="topRight" activeCell="S109" sqref="S102:S109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -889,9 +896,7 @@
       <c r="R3" s="10">
         <v>1.3325</v>
       </c>
-      <c r="S3" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S3" s="10"/>
       <c r="T3" s="10">
         <v>20.985499999999998</v>
       </c>
@@ -958,9 +963,7 @@
       <c r="R4" s="10">
         <v>1.3341000000000001</v>
       </c>
-      <c r="S4" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S4" s="10"/>
       <c r="T4" s="10">
         <v>22.053699999999999</v>
       </c>
@@ -1027,9 +1030,7 @@
       <c r="R5" s="10">
         <v>1.4133</v>
       </c>
-      <c r="S5" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S5" s="10"/>
       <c r="T5" s="10">
         <v>21.180199999999999</v>
       </c>
@@ -1096,9 +1097,7 @@
       <c r="R6" s="10">
         <v>1.8131999999999999</v>
       </c>
-      <c r="S6" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S6" s="10"/>
       <c r="T6" s="10">
         <v>24.563199999999998</v>
       </c>
@@ -1165,9 +1164,7 @@
       <c r="R7" s="10">
         <v>1.3553999999999999</v>
       </c>
-      <c r="S7" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S7" s="10"/>
       <c r="T7" s="10">
         <v>22.490600000000001</v>
       </c>
@@ -1234,9 +1231,7 @@
       <c r="R8" s="10">
         <v>1.3132999999999999</v>
       </c>
-      <c r="S8" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S8" s="10"/>
       <c r="T8" s="10">
         <v>20.820900000000002</v>
       </c>
@@ -1303,9 +1298,7 @@
       <c r="R9" s="10">
         <v>1.0549999999999999</v>
       </c>
-      <c r="S9" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S9" s="10"/>
       <c r="T9" s="10">
         <v>22.1935</v>
       </c>
@@ -1413,9 +1406,7 @@
       <c r="R12" s="10">
         <v>1.7073</v>
       </c>
-      <c r="S12" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S12" s="10"/>
       <c r="T12" s="10">
         <v>21.306799999999999</v>
       </c>
@@ -1482,9 +1473,7 @@
       <c r="R13" s="10">
         <v>1.2054</v>
       </c>
-      <c r="S13" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S13" s="10"/>
       <c r="T13" s="10">
         <v>20.903500000000001</v>
       </c>
@@ -1620,9 +1609,7 @@
       <c r="R15" s="10">
         <v>1.6662999999999999</v>
       </c>
-      <c r="S15" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S15" s="10"/>
       <c r="T15" s="10">
         <v>21.716100000000001</v>
       </c>
@@ -1689,9 +1676,7 @@
       <c r="R16" s="10">
         <v>1.1845000000000001</v>
       </c>
-      <c r="S16" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S16" s="10"/>
       <c r="T16" s="10">
         <v>22.2394</v>
       </c>
@@ -1758,9 +1743,7 @@
       <c r="R17" s="10">
         <v>1.1606000000000001</v>
       </c>
-      <c r="S17" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S17" s="10"/>
       <c r="T17" s="10">
         <v>21.356200000000001</v>
       </c>
@@ -1827,9 +1810,7 @@
       <c r="R18" s="10">
         <v>1.3104</v>
       </c>
-      <c r="S18" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S18" s="10"/>
       <c r="T18" s="10">
         <v>20.741900000000001</v>
       </c>
@@ -1896,9 +1877,7 @@
       <c r="R19" s="10">
         <v>1.0569999999999999</v>
       </c>
-      <c r="S19" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S19" s="10"/>
       <c r="T19" s="10">
         <v>22.616299999999999</v>
       </c>
@@ -2003,9 +1982,7 @@
       <c r="R22" s="10">
         <v>1.391</v>
       </c>
-      <c r="S22" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S22" s="10"/>
       <c r="T22" s="10">
         <v>21.552199999999999</v>
       </c>
@@ -2060,9 +2037,7 @@
       <c r="R23" s="10">
         <v>1.2885</v>
       </c>
-      <c r="S23" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S23" s="10"/>
       <c r="T23" s="10">
         <v>21.4282</v>
       </c>
@@ -2117,9 +2092,7 @@
       <c r="R24" s="10">
         <v>1.2214</v>
       </c>
-      <c r="S24" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S24" s="10"/>
       <c r="T24" s="10">
         <v>22.1905</v>
       </c>
@@ -2174,9 +2147,7 @@
       <c r="R25" s="10">
         <v>1.4151</v>
       </c>
-      <c r="S25" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S25" s="10"/>
       <c r="T25" s="10">
         <v>21.304200000000002</v>
       </c>
@@ -2231,9 +2202,7 @@
       <c r="R26" s="10">
         <v>1.4085000000000001</v>
       </c>
-      <c r="S26" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S26" s="10"/>
       <c r="T26" s="10">
         <v>23.2822</v>
       </c>
@@ -2288,9 +2257,7 @@
       <c r="R27" s="10">
         <v>1.2061999999999999</v>
       </c>
-      <c r="S27" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S27" s="10"/>
       <c r="T27" s="10">
         <v>21.0503</v>
       </c>
@@ -2345,9 +2312,7 @@
       <c r="R28" s="10">
         <v>1.2672000000000001</v>
       </c>
-      <c r="S28" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S28" s="10"/>
       <c r="T28" s="10">
         <v>20.343299999999999</v>
       </c>
@@ -2402,9 +2367,7 @@
       <c r="R29" s="10">
         <v>1.0686</v>
       </c>
-      <c r="S29" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S29" s="10"/>
       <c r="T29" s="10">
         <v>21.330300000000001</v>
       </c>
@@ -2520,9 +2483,7 @@
       <c r="R32" s="10">
         <v>1.2793000000000001</v>
       </c>
-      <c r="S32" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S32" s="10"/>
       <c r="T32" s="10">
         <v>20.879300000000001</v>
       </c>
@@ -2589,9 +2550,7 @@
       <c r="R33" s="10">
         <v>1.5025999999999999</v>
       </c>
-      <c r="S33" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S33" s="10"/>
       <c r="T33" s="10">
         <v>21.090900000000001</v>
       </c>
@@ -2658,9 +2617,7 @@
       <c r="R34" s="10">
         <v>1.1229</v>
       </c>
-      <c r="S34" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S34" s="10"/>
       <c r="T34" s="10">
         <v>21.686399999999999</v>
       </c>
@@ -2796,9 +2753,7 @@
       <c r="R36" s="10">
         <v>1.3782000000000001</v>
       </c>
-      <c r="S36" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S36" s="10"/>
       <c r="T36" s="10">
         <v>22.765799999999999</v>
       </c>
@@ -2865,9 +2820,7 @@
       <c r="R37" s="10">
         <v>1.1166</v>
       </c>
-      <c r="S37" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S37" s="10"/>
       <c r="T37" s="10">
         <v>20.706800000000001</v>
       </c>
@@ -2934,9 +2887,7 @@
       <c r="R38" s="10">
         <v>1.2663</v>
       </c>
-      <c r="S38" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S38" s="10"/>
       <c r="T38" s="10">
         <v>20.4665</v>
       </c>
@@ -3003,9 +2954,7 @@
       <c r="R39" s="10">
         <v>1.0226999999999999</v>
       </c>
-      <c r="S39" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S39" s="10"/>
       <c r="T39" s="10">
         <v>21.6953</v>
       </c>
@@ -3122,9 +3071,7 @@
       <c r="R42" s="10">
         <v>1.2153</v>
       </c>
-      <c r="S42" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S42" s="10"/>
       <c r="T42" s="10">
         <v>22.919899999999998</v>
       </c>
@@ -3191,9 +3138,7 @@
       <c r="R43" s="10">
         <v>1.4762</v>
       </c>
-      <c r="S43" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S43" s="10"/>
       <c r="T43" s="10">
         <v>21.790299999999998</v>
       </c>
@@ -3260,9 +3205,7 @@
       <c r="R44" s="10">
         <v>1.0885</v>
       </c>
-      <c r="S44" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S44" s="10"/>
       <c r="T44" s="10">
         <v>21.7605</v>
       </c>
@@ -3329,9 +3272,7 @@
       <c r="R45" s="10">
         <v>1.4092</v>
       </c>
-      <c r="S45" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S45" s="10"/>
       <c r="T45" s="10">
         <v>21.2181</v>
       </c>
@@ -3398,9 +3339,7 @@
       <c r="R46" s="10">
         <v>1.3514999999999999</v>
       </c>
-      <c r="S46" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S46" s="10"/>
       <c r="T46" s="10">
         <v>22.4437</v>
       </c>
@@ -3467,9 +3406,7 @@
       <c r="R47" s="10">
         <v>1.228</v>
       </c>
-      <c r="S47" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S47" s="10"/>
       <c r="T47" s="10">
         <v>20.766300000000001</v>
       </c>
@@ -3536,9 +3473,7 @@
       <c r="R48" s="10">
         <v>1.3180000000000001</v>
       </c>
-      <c r="S48" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S48" s="10"/>
       <c r="T48" s="10">
         <v>21.396599999999999</v>
       </c>
@@ -3605,9 +3540,7 @@
       <c r="R49" s="10">
         <v>1.0055000000000001</v>
       </c>
-      <c r="S49" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="S49" s="10"/>
       <c r="T49" s="10">
         <v>21.2286</v>
       </c>
@@ -3696,20 +3629,36 @@
         <f t="shared" ref="J52:J59" si="28">I52/61</f>
         <v>6.0375409836065579</v>
       </c>
+      <c r="K52">
+        <v>3.0030000000000001</v>
+      </c>
       <c r="L52" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.4710860366713672E-2</v>
+      </c>
+      <c r="M52">
+        <v>38.354700000000001</v>
       </c>
       <c r="N52" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.89196976744186052</v>
       </c>
       <c r="P52" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S52">
-        <v>0</v>
+      <c r="Q52">
+        <v>111.38</v>
+      </c>
+      <c r="R52">
+        <v>1.29</v>
+      </c>
+      <c r="S52" s="10"/>
+      <c r="T52">
+        <v>22.02</v>
+      </c>
+      <c r="U52">
+        <v>5.63</v>
       </c>
     </row>
     <row r="53" spans="1:21">
@@ -3744,20 +3693,36 @@
         <f t="shared" si="28"/>
         <v>5.3532786885245907</v>
       </c>
+      <c r="K53">
+        <v>3.4365000000000001</v>
+      </c>
       <c r="L53" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.6939351198871648E-2</v>
+      </c>
+      <c r="M53">
+        <v>39.512900000000002</v>
       </c>
       <c r="N53" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.91890465116279074</v>
       </c>
       <c r="P53" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S53">
-        <v>0</v>
+      <c r="Q53">
+        <v>108.82</v>
+      </c>
+      <c r="R53">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="S53" s="10"/>
+      <c r="T53">
+        <v>20.87</v>
+      </c>
+      <c r="U53">
+        <v>5.4</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -3793,9 +3758,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S54">
-        <v>0</v>
-      </c>
+      <c r="R54" s="10"/>
+      <c r="S54" s="10"/>
     </row>
     <row r="55" spans="1:21">
       <c r="A55" t="s">
@@ -3829,20 +3793,36 @@
         <f t="shared" si="28"/>
         <v>5.4873770491803278</v>
       </c>
+      <c r="K55">
+        <v>2.9516</v>
+      </c>
       <c r="L55" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.3260930888575446E-2</v>
+      </c>
+      <c r="M55">
+        <v>37.333500000000001</v>
       </c>
       <c r="N55" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.8682209302325582</v>
       </c>
       <c r="P55" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S55">
-        <v>0</v>
+      <c r="Q55">
+        <v>123.71</v>
+      </c>
+      <c r="R55">
+        <v>1.22</v>
+      </c>
+      <c r="S55" s="10"/>
+      <c r="T55">
+        <v>23.11</v>
+      </c>
+      <c r="U55">
+        <v>5.8</v>
       </c>
     </row>
     <row r="56" spans="1:21">
@@ -3877,20 +3857,36 @@
         <f t="shared" si="28"/>
         <v>5.4829508196721308</v>
       </c>
+      <c r="K56">
+        <v>3.0781999999999998</v>
+      </c>
       <c r="L56" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.6832157968970369E-2</v>
+      </c>
+      <c r="M56">
+        <v>37.541400000000003</v>
       </c>
       <c r="N56" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.87305581395348841</v>
       </c>
       <c r="P56" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S56">
-        <v>0</v>
+      <c r="Q56">
+        <v>120.91</v>
+      </c>
+      <c r="R56">
+        <v>0.86</v>
+      </c>
+      <c r="S56" s="10"/>
+      <c r="T56">
+        <v>22.96</v>
+      </c>
+      <c r="U56">
+        <v>5.34</v>
       </c>
     </row>
     <row r="57" spans="1:21">
@@ -3925,20 +3921,36 @@
         <f t="shared" si="28"/>
         <v>5.3999999999999995</v>
       </c>
+      <c r="K57">
+        <v>3.0173000000000001</v>
+      </c>
       <c r="L57" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.5114245416078982E-2</v>
+      </c>
+      <c r="M57">
+        <v>36.258499999999998</v>
       </c>
       <c r="N57" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.84322093023255806</v>
       </c>
       <c r="P57" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S57">
-        <v>0</v>
+      <c r="Q57">
+        <v>115.12</v>
+      </c>
+      <c r="R57">
+        <v>1.03</v>
+      </c>
+      <c r="S57" s="10"/>
+      <c r="T57">
+        <v>20.65</v>
+      </c>
+      <c r="U57">
+        <v>5.97</v>
       </c>
     </row>
     <row r="58" spans="1:21">
@@ -3973,20 +3985,36 @@
         <f t="shared" si="28"/>
         <v>5.4455737704918032</v>
       </c>
+      <c r="K58">
+        <v>3.1680999999999999</v>
+      </c>
       <c r="L58" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.9368124118476722E-2</v>
+      </c>
+      <c r="M58">
+        <v>36.617899999999999</v>
       </c>
       <c r="N58" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.8515790697674418</v>
       </c>
       <c r="P58" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S58">
-        <v>0</v>
+      <c r="Q58">
+        <v>149.85</v>
+      </c>
+      <c r="R58">
+        <v>1.08</v>
+      </c>
+      <c r="S58" s="10"/>
+      <c r="T58">
+        <v>20.86</v>
+      </c>
+      <c r="U58">
+        <v>5.37</v>
       </c>
     </row>
     <row r="59" spans="1:21">
@@ -4021,20 +4049,36 @@
         <f t="shared" si="28"/>
         <v>5.4013114754098366</v>
       </c>
+      <c r="K59">
+        <v>3.0899000000000001</v>
+      </c>
       <c r="L59" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.7162200282087446E-2</v>
+      </c>
+      <c r="M59">
+        <v>38.158099999999997</v>
       </c>
       <c r="N59" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.88739767441860462</v>
       </c>
       <c r="P59" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S59">
-        <v>0</v>
+      <c r="Q59">
+        <v>120.86</v>
+      </c>
+      <c r="R59">
+        <v>0.86</v>
+      </c>
+      <c r="S59" s="10"/>
+      <c r="T59">
+        <v>22.18</v>
+      </c>
+      <c r="U59">
+        <v>5.48</v>
       </c>
     </row>
     <row r="60" spans="1:21">
@@ -4048,19 +4092,19 @@
       </c>
       <c r="K60" s="5">
         <f t="shared" ref="K60" si="29">SUM(K52:K59)</f>
-        <v>0</v>
+        <v>21.744600000000002</v>
       </c>
       <c r="L60" s="5">
         <f t="shared" ref="L60" si="30">SUM(L52:L59)</f>
-        <v>0</v>
+        <v>0.61338787023977426</v>
       </c>
       <c r="M60" s="5">
         <f t="shared" ref="M60" si="31">SUM(M52:M59)</f>
-        <v>0</v>
+        <v>263.77699999999999</v>
       </c>
       <c r="N60" s="5">
         <f t="shared" ref="N60" si="32">SUM(N52:N59)</f>
-        <v>0</v>
+        <v>6.134348837209302</v>
       </c>
       <c r="O60" s="5">
         <f t="shared" ref="O60" si="33">SUM(O52:O59)</f>
@@ -4116,20 +4160,36 @@
         <f t="shared" ref="J62:J69" si="35">I62/61</f>
         <v>5.86672131147541</v>
       </c>
+      <c r="K62">
+        <v>2.3873000000000002</v>
+      </c>
       <c r="L62" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.7342736248236959E-2</v>
+      </c>
+      <c r="M62">
+        <v>45.106000000000002</v>
       </c>
       <c r="N62" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.0489767441860465</v>
       </c>
       <c r="P62" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S62">
-        <v>0</v>
+      <c r="Q62">
+        <v>142.71</v>
+      </c>
+      <c r="R62">
+        <v>1</v>
+      </c>
+      <c r="S62" s="10"/>
+      <c r="T62">
+        <v>25.5</v>
+      </c>
+      <c r="U62">
+        <v>4.49</v>
       </c>
     </row>
     <row r="63" spans="1:21">
@@ -4164,20 +4224,36 @@
         <f t="shared" si="35"/>
         <v>5.518196721311476</v>
       </c>
+      <c r="K63">
+        <v>2.2913999999999999</v>
+      </c>
       <c r="L63" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.4637517630465435E-2</v>
+      </c>
+      <c r="M63">
+        <v>50.9696</v>
       </c>
       <c r="N63" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.185339534883721</v>
       </c>
       <c r="P63" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S63">
-        <v>0</v>
+      <c r="Q63">
+        <v>133.63999999999999</v>
+      </c>
+      <c r="R63">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="S63" s="10"/>
+      <c r="T63">
+        <v>23.37</v>
+      </c>
+      <c r="U63">
+        <v>5.57</v>
       </c>
     </row>
     <row r="64" spans="1:21">
@@ -4207,9 +4283,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S64">
-        <v>0</v>
-      </c>
+      <c r="Q64" s="10"/>
+      <c r="R64" s="10"/>
+      <c r="S64" s="10"/>
+      <c r="T64" s="10"/>
+      <c r="U64" s="10"/>
     </row>
     <row r="65" spans="1:21">
       <c r="A65" t="s">
@@ -4243,20 +4321,36 @@
         <f t="shared" si="35"/>
         <v>5.6742622950819674</v>
       </c>
+      <c r="K65">
+        <v>1.9777</v>
+      </c>
       <c r="L65" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.578843441466854E-2</v>
+      </c>
+      <c r="M65">
+        <v>47.9328</v>
       </c>
       <c r="N65" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.1147162790697676</v>
       </c>
       <c r="P65" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S65">
-        <v>0</v>
+      <c r="Q65">
+        <v>127.41</v>
+      </c>
+      <c r="R65">
+        <v>1.18</v>
+      </c>
+      <c r="S65" s="10"/>
+      <c r="T65">
+        <v>21.5</v>
+      </c>
+      <c r="U65">
+        <v>5.61</v>
       </c>
     </row>
     <row r="66" spans="1:21">
@@ -4291,20 +4385,36 @@
         <f t="shared" si="35"/>
         <v>5.5009836065573774</v>
       </c>
+      <c r="K66">
+        <v>2.1665000000000001</v>
+      </c>
       <c r="L66" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.1114245416078981E-2</v>
+      </c>
+      <c r="M66">
+        <v>47.983800000000002</v>
       </c>
       <c r="N66" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.1159023255813953</v>
       </c>
       <c r="P66" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S66">
-        <v>0</v>
+      <c r="Q66">
+        <v>121.06</v>
+      </c>
+      <c r="R66">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S66" s="10"/>
+      <c r="T66">
+        <v>24.47</v>
+      </c>
+      <c r="U66">
+        <v>4.59</v>
       </c>
     </row>
     <row r="67" spans="1:21">
@@ -4339,20 +4449,36 @@
         <f t="shared" si="35"/>
         <v>5.4096721311475413</v>
       </c>
+      <c r="K67">
+        <v>2.1861000000000002</v>
+      </c>
       <c r="L67" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.166713681241185E-2</v>
+      </c>
+      <c r="M67">
+        <v>47.686700000000002</v>
       </c>
       <c r="N67" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.1089930232558141</v>
       </c>
       <c r="P67" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S67">
-        <v>0</v>
+      <c r="Q67">
+        <v>115.34</v>
+      </c>
+      <c r="R67">
+        <v>1.08</v>
+      </c>
+      <c r="S67" s="10"/>
+      <c r="T67">
+        <v>21.18</v>
+      </c>
+      <c r="U67">
+        <v>5.86</v>
       </c>
     </row>
     <row r="68" spans="1:21">
@@ -4387,20 +4513,36 @@
         <f t="shared" si="35"/>
         <v>5.589672131147541</v>
       </c>
+      <c r="K68">
+        <v>2.1775000000000002</v>
+      </c>
       <c r="L68" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.1424541607898453E-2</v>
+      </c>
+      <c r="M68">
+        <v>47.455100000000002</v>
       </c>
       <c r="N68" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.1036069767441861</v>
       </c>
       <c r="P68" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S68">
-        <v>0</v>
+      <c r="Q68">
+        <v>114.72</v>
+      </c>
+      <c r="R68">
+        <v>0.98</v>
+      </c>
+      <c r="S68" s="10"/>
+      <c r="T68">
+        <v>22.14</v>
+      </c>
+      <c r="U68">
+        <v>5.37</v>
       </c>
     </row>
     <row r="69" spans="1:21">
@@ -4435,20 +4577,36 @@
         <f t="shared" si="35"/>
         <v>5.5496721311475401</v>
       </c>
+      <c r="K69">
+        <v>2.5712999999999999</v>
+      </c>
       <c r="L69" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.2533145275035252E-2</v>
+      </c>
+      <c r="M69">
+        <v>51.689900000000002</v>
       </c>
       <c r="N69" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.2020906976744186</v>
       </c>
       <c r="P69" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S69">
-        <v>0</v>
+      <c r="Q69">
+        <v>128.44999999999999</v>
+      </c>
+      <c r="R69">
+        <v>0.74</v>
+      </c>
+      <c r="S69" s="10"/>
+      <c r="T69">
+        <v>23.6</v>
+      </c>
+      <c r="U69">
+        <v>4.95</v>
       </c>
     </row>
     <row r="70" spans="1:21">
@@ -4463,19 +4621,19 @@
       </c>
       <c r="K70" s="5">
         <f t="shared" ref="K70" si="36">SUM(K62:K69)</f>
-        <v>0</v>
+        <v>15.7578</v>
       </c>
       <c r="L70" s="5">
         <f t="shared" ref="L70" si="37">SUM(L62:L69)</f>
-        <v>0</v>
+        <v>0.44450775740479548</v>
       </c>
       <c r="M70" s="5">
         <f t="shared" ref="M70" si="38">SUM(M62:M69)</f>
-        <v>0</v>
+        <v>338.82390000000004</v>
       </c>
       <c r="N70" s="5">
         <f t="shared" ref="N70" si="39">SUM(N62:N69)</f>
-        <v>0</v>
+        <v>7.8796255813953495</v>
       </c>
       <c r="O70" s="5">
         <f t="shared" ref="O70" si="40">SUM(O62:O69)</f>
@@ -4544,8 +4702,18 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S72">
-        <v>0</v>
+      <c r="Q72">
+        <v>125.77</v>
+      </c>
+      <c r="R72">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="S72" s="10"/>
+      <c r="T72">
+        <v>23.33</v>
+      </c>
+      <c r="U72">
+        <v>5.5</v>
       </c>
     </row>
     <row r="73" spans="1:21">
@@ -4592,8 +4760,18 @@
         <f t="shared" ref="P73:P109" si="45">O73/62</f>
         <v>0</v>
       </c>
-      <c r="S73">
-        <v>0</v>
+      <c r="Q73">
+        <v>91.94</v>
+      </c>
+      <c r="R73">
+        <v>0.64</v>
+      </c>
+      <c r="S73" s="10"/>
+      <c r="T73">
+        <v>23.63</v>
+      </c>
+      <c r="U73">
+        <v>4.6399999999999997</v>
       </c>
     </row>
     <row r="74" spans="1:21">
@@ -4626,9 +4804,11 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S74">
-        <v>0</v>
-      </c>
+      <c r="Q74" s="10"/>
+      <c r="R74" s="10"/>
+      <c r="S74" s="10"/>
+      <c r="T74" s="10"/>
+      <c r="U74" s="10"/>
     </row>
     <row r="75" spans="1:21">
       <c r="A75" t="s">
@@ -4674,8 +4854,18 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S75">
-        <v>0</v>
+      <c r="Q75">
+        <v>131.88</v>
+      </c>
+      <c r="R75">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="S75" s="10"/>
+      <c r="T75">
+        <v>23.1</v>
+      </c>
+      <c r="U75">
+        <v>5.82</v>
       </c>
     </row>
     <row r="76" spans="1:21">
@@ -4722,8 +4912,18 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S76">
-        <v>0</v>
+      <c r="Q76">
+        <v>115.92</v>
+      </c>
+      <c r="R76">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="S76" s="10"/>
+      <c r="T76">
+        <v>22.16</v>
+      </c>
+      <c r="U76">
+        <v>6.07</v>
       </c>
     </row>
     <row r="77" spans="1:21">
@@ -4770,8 +4970,20 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
+      <c r="Q77">
+        <v>121.74</v>
+      </c>
+      <c r="R77">
+        <v>0.88</v>
+      </c>
       <c r="S77">
         <v>0.91</v>
+      </c>
+      <c r="T77">
+        <v>22.04</v>
+      </c>
+      <c r="U77">
+        <v>5.94</v>
       </c>
     </row>
     <row r="78" spans="1:21">
@@ -4818,8 +5030,18 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S78">
-        <v>0</v>
+      <c r="Q78">
+        <v>117.42</v>
+      </c>
+      <c r="R78">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="S78" s="10"/>
+      <c r="T78">
+        <v>20.5</v>
+      </c>
+      <c r="U78">
+        <v>5.58</v>
       </c>
     </row>
     <row r="79" spans="1:21">
@@ -4866,8 +5088,18 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S79">
-        <v>0</v>
+      <c r="Q79">
+        <v>146.57</v>
+      </c>
+      <c r="R79">
+        <v>0.53</v>
+      </c>
+      <c r="S79" s="10"/>
+      <c r="T79">
+        <v>24.42</v>
+      </c>
+      <c r="U79">
+        <v>5.33</v>
       </c>
     </row>
     <row r="80" spans="1:21">
@@ -4949,20 +5181,39 @@
         <f t="shared" ref="J82:J89" si="52">I82/61</f>
         <v>5.8426229508196714</v>
       </c>
+      <c r="K82">
+        <v>2.4500000000000002</v>
+      </c>
       <c r="L82" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>6.9111424541607902E-2</v>
+      </c>
+      <c r="M82">
+        <v>54.1492</v>
       </c>
       <c r="N82" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.2592837209302326</v>
+      </c>
+      <c r="O82">
+        <v>1.6395</v>
       </c>
       <c r="P82" s="6">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S82" s="2">
-        <v>0</v>
+        <v>2.6443548387096772E-2</v>
+      </c>
+      <c r="Q82" s="11">
+        <v>118.6</v>
+      </c>
+      <c r="R82" s="11">
+        <v>1.39</v>
+      </c>
+      <c r="S82" s="10"/>
+      <c r="T82" s="11">
+        <v>24.26</v>
+      </c>
+      <c r="U82" s="11">
+        <v>5.8</v>
       </c>
     </row>
     <row r="83" spans="1:21">
@@ -4997,20 +5248,39 @@
         <f t="shared" si="52"/>
         <v>5.8147540983606554</v>
       </c>
+      <c r="K83">
+        <v>2.9519000000000002</v>
+      </c>
       <c r="L83" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>8.3269393511988712E-2</v>
+      </c>
+      <c r="M83">
+        <v>56.819899999999997</v>
       </c>
       <c r="N83" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.321393023255814</v>
+      </c>
+      <c r="O83">
+        <v>2.0198</v>
       </c>
       <c r="P83" s="6">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S83" s="2">
-        <v>0</v>
+        <v>3.257741935483871E-2</v>
+      </c>
+      <c r="Q83" s="11">
+        <v>124.18</v>
+      </c>
+      <c r="R83" s="11">
+        <v>1.45</v>
+      </c>
+      <c r="S83" s="10"/>
+      <c r="T83" s="11">
+        <v>22.61</v>
+      </c>
+      <c r="U83" s="11">
+        <v>6.15</v>
       </c>
     </row>
     <row r="84" spans="1:21">
@@ -5039,9 +5309,11 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S84" s="2">
-        <v>0</v>
-      </c>
+      <c r="Q84" s="10"/>
+      <c r="R84" s="10"/>
+      <c r="S84" s="10"/>
+      <c r="T84" s="10"/>
+      <c r="U84" s="10"/>
     </row>
     <row r="85" spans="1:21">
       <c r="A85" t="s">
@@ -5075,20 +5347,39 @@
         <f t="shared" si="52"/>
         <v>5.6786885245901635</v>
       </c>
+      <c r="K85">
+        <v>2.4131</v>
+      </c>
       <c r="L85" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>6.8070521861777145E-2</v>
+      </c>
+      <c r="M85">
+        <v>51.599400000000003</v>
       </c>
       <c r="N85" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.1999860465116279</v>
+      </c>
+      <c r="O85">
+        <v>3.5419</v>
       </c>
       <c r="P85" s="6">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S85" s="2">
-        <v>0</v>
+        <v>5.7127419354838713E-2</v>
+      </c>
+      <c r="Q85" s="11">
+        <v>143.4</v>
+      </c>
+      <c r="R85" s="11">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="S85" s="10"/>
+      <c r="T85" s="11">
+        <v>24.57</v>
+      </c>
+      <c r="U85" s="11">
+        <v>5.01</v>
       </c>
     </row>
     <row r="86" spans="1:21">
@@ -5123,20 +5414,36 @@
         <f t="shared" si="52"/>
         <v>5.5983606557377046</v>
       </c>
+      <c r="K86">
+        <v>2.2784</v>
+      </c>
       <c r="L86" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>6.4270803949224256E-2</v>
+      </c>
+      <c r="M86">
+        <v>52.341999999999999</v>
       </c>
       <c r="N86" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.2172558139534884</v>
       </c>
       <c r="P86" s="6">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S86" s="2">
-        <v>0</v>
+      <c r="Q86" s="11">
+        <v>109.85</v>
+      </c>
+      <c r="R86" s="11">
+        <v>1.03</v>
+      </c>
+      <c r="S86" s="10"/>
+      <c r="T86" s="11">
+        <v>22.2</v>
+      </c>
+      <c r="U86" s="11">
+        <v>5.37</v>
       </c>
     </row>
     <row r="87" spans="1:21">
@@ -5171,20 +5478,39 @@
         <f t="shared" si="52"/>
         <v>5.8622950819672131</v>
       </c>
+      <c r="K87">
+        <v>2.3043</v>
+      </c>
       <c r="L87" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>6.5001410437235535E-2</v>
+      </c>
+      <c r="M87">
+        <v>51.661499999999997</v>
       </c>
       <c r="N87" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.2014302325581394</v>
+      </c>
+      <c r="O87">
+        <v>1.0674999999999999</v>
       </c>
       <c r="P87" s="6">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S87" s="2">
-        <v>0</v>
+        <v>1.7217741935483869E-2</v>
+      </c>
+      <c r="Q87" s="11">
+        <v>129.36000000000001</v>
+      </c>
+      <c r="R87" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S87" s="10"/>
+      <c r="T87" s="11">
+        <v>23.14</v>
+      </c>
+      <c r="U87" s="11">
+        <v>5.8</v>
       </c>
     </row>
     <row r="88" spans="1:21">
@@ -5219,20 +5545,36 @@
         <f t="shared" si="52"/>
         <v>5.6163934426229511</v>
       </c>
+      <c r="K88">
+        <v>2.8698000000000001</v>
+      </c>
       <c r="L88" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>8.0953455571227073E-2</v>
+      </c>
+      <c r="M88">
+        <v>50.555</v>
       </c>
       <c r="N88" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.1756976744186047</v>
       </c>
       <c r="P88" s="6">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S88" s="2">
-        <v>0</v>
+      <c r="Q88" s="11">
+        <v>116.25</v>
+      </c>
+      <c r="R88" s="11">
+        <v>1.21</v>
+      </c>
+      <c r="S88" s="10"/>
+      <c r="T88" s="11">
+        <v>23.26</v>
+      </c>
+      <c r="U88" s="11">
+        <v>6.01</v>
       </c>
     </row>
     <row r="89" spans="1:21">
@@ -5267,68 +5609,61 @@
         <f t="shared" si="52"/>
         <v>5.7721311475409838</v>
       </c>
+      <c r="K89">
+        <v>2.9990000000000001</v>
+      </c>
       <c r="L89" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>8.4598025387870229E-2</v>
+      </c>
+      <c r="M89">
+        <v>53.045299999999997</v>
       </c>
       <c r="N89" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.2336116279069766</v>
       </c>
       <c r="P89" s="6">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S89" s="2">
-        <v>0</v>
+      <c r="Q89" s="11">
+        <v>118.52</v>
+      </c>
+      <c r="R89" s="11">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="S89" s="10"/>
+      <c r="T89" s="11">
+        <v>21.69</v>
+      </c>
+      <c r="U89" s="11">
+        <v>6.26</v>
       </c>
     </row>
     <row r="90" spans="1:21">
-      <c r="A90" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="B90" s="2"/>
-      <c r="J90" s="5">
-        <f>SUM(J82:J89)</f>
-        <v>40.185245901639341</v>
-      </c>
-      <c r="K90" s="5">
-        <f t="shared" ref="K90" si="53">SUM(K82:K89)</f>
-        <v>0</v>
-      </c>
-      <c r="L90" s="5">
-        <f t="shared" ref="L90" si="54">SUM(L82:L89)</f>
-        <v>0</v>
-      </c>
-      <c r="M90" s="5">
-        <f t="shared" ref="M90" si="55">SUM(M82:M89)</f>
-        <v>0</v>
-      </c>
-      <c r="N90" s="5">
-        <f t="shared" ref="N90" si="56">SUM(N82:N89)</f>
-        <v>0</v>
-      </c>
-      <c r="O90" s="5">
-        <f t="shared" ref="O90" si="57">SUM(O82:O89)</f>
-        <v>0</v>
-      </c>
-      <c r="P90" s="5">
-        <f t="shared" ref="P90" si="58">SUM(P82:P89)</f>
-        <v>0</v>
-      </c>
-      <c r="Q90" s="5"/>
-      <c r="R90" s="5"/>
-      <c r="S90" s="5"/>
-      <c r="T90" s="5"/>
-      <c r="U90" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="L90" s="6"/>
+      <c r="N90" s="6"/>
+      <c r="P90" s="6"/>
+      <c r="Q90" s="11"/>
+      <c r="R90" s="11"/>
+      <c r="S90" s="10"/>
+      <c r="T90" s="11"/>
+      <c r="U90" s="11"/>
     </row>
     <row r="91" spans="1:21">
-      <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="J91" s="5"/>
       <c r="L91" s="6"/>
       <c r="N91" s="6"/>
       <c r="P91" s="6"/>
+      <c r="Q91" s="11"/>
+      <c r="R91" s="11"/>
+      <c r="S91" s="10"/>
+      <c r="T91" s="11"/>
+      <c r="U91" s="11"/>
     </row>
     <row r="92" spans="1:21">
       <c r="A92" t="s">
@@ -5340,27 +5675,61 @@
       <c r="C92" t="s">
         <v>34</v>
       </c>
+      <c r="D92">
+        <v>637</v>
+      </c>
+      <c r="E92">
+        <v>14.7</v>
+      </c>
+      <c r="F92">
+        <v>588.4</v>
+      </c>
+      <c r="G92">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="H92">
+        <v>6.93</v>
+      </c>
       <c r="I92">
         <v>331.5</v>
       </c>
       <c r="J92" s="5">
-        <f t="shared" ref="J92:J99" si="59">I92/61</f>
+        <f t="shared" ref="J92:J99" si="53">I92/61</f>
         <v>5.4344262295081966</v>
+      </c>
+      <c r="K92">
+        <v>3.6242000000000001</v>
       </c>
       <c r="L92" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>0.10223413258110013</v>
+      </c>
+      <c r="M92">
+        <v>52.437600000000003</v>
       </c>
       <c r="N92" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.219479069767442</v>
+      </c>
+      <c r="O92">
+        <v>2.2021999999999999</v>
       </c>
       <c r="P92" s="6">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S92" s="2">
-        <v>0</v>
+        <v>3.5519354838709674E-2</v>
+      </c>
+      <c r="Q92" s="11">
+        <v>110.92</v>
+      </c>
+      <c r="R92" s="11">
+        <v>1.33</v>
+      </c>
+      <c r="S92" s="10"/>
+      <c r="T92" s="11">
+        <v>21.08</v>
+      </c>
+      <c r="U92" s="11">
+        <v>5.53</v>
       </c>
     </row>
     <row r="93" spans="1:21">
@@ -5373,27 +5742,61 @@
       <c r="C93" t="s">
         <v>35</v>
       </c>
+      <c r="D93">
+        <v>598</v>
+      </c>
+      <c r="E93">
+        <v>15.3</v>
+      </c>
+      <c r="F93">
+        <v>583.1</v>
+      </c>
+      <c r="G93">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="H93">
+        <v>6.97</v>
+      </c>
       <c r="I93">
         <v>348.6</v>
       </c>
       <c r="J93" s="5">
-        <f t="shared" si="59"/>
+        <f t="shared" si="53"/>
         <v>5.7147540983606557</v>
+      </c>
+      <c r="K93">
+        <v>2.2852999999999999</v>
       </c>
       <c r="L93" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>6.4465444287729184E-2</v>
+      </c>
+      <c r="M93">
+        <v>50.705300000000001</v>
       </c>
       <c r="N93" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.1791930232558139</v>
+      </c>
+      <c r="O93">
+        <v>1.0262</v>
       </c>
       <c r="P93" s="6">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S93" s="2">
-        <v>0</v>
+        <v>1.6551612903225807E-2</v>
+      </c>
+      <c r="Q93" s="11">
+        <v>114.77</v>
+      </c>
+      <c r="R93" s="11">
+        <v>0.73</v>
+      </c>
+      <c r="S93" s="10"/>
+      <c r="T93" s="11">
+        <v>23.18</v>
+      </c>
+      <c r="U93" s="11">
+        <v>4.4400000000000004</v>
       </c>
     </row>
     <row r="94" spans="1:21">
@@ -5407,7 +5810,7 @@
         <v>35</v>
       </c>
       <c r="J94" s="5">
-        <f t="shared" si="59"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="L94" s="6">
@@ -5422,9 +5825,11 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S94" s="2">
-        <v>0</v>
-      </c>
+      <c r="Q94" s="11"/>
+      <c r="R94" s="10"/>
+      <c r="S94" s="10"/>
+      <c r="T94" s="10"/>
+      <c r="U94" s="10"/>
     </row>
     <row r="95" spans="1:21">
       <c r="A95" t="s">
@@ -5436,27 +5841,61 @@
       <c r="C95" t="s">
         <v>34</v>
       </c>
+      <c r="D95">
+        <v>576</v>
+      </c>
+      <c r="E95">
+        <v>14.8</v>
+      </c>
+      <c r="F95">
+        <v>586.29999999999995</v>
+      </c>
+      <c r="G95">
+        <v>31.9</v>
+      </c>
+      <c r="H95">
+        <v>6.82</v>
+      </c>
       <c r="I95">
         <v>336.7</v>
       </c>
       <c r="J95" s="5">
-        <f t="shared" si="59"/>
+        <f t="shared" si="53"/>
         <v>5.5196721311475407</v>
+      </c>
+      <c r="K95">
+        <v>2.5106999999999999</v>
       </c>
       <c r="L95" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>7.0823695345557117E-2</v>
+      </c>
+      <c r="M95">
+        <v>51.929400000000001</v>
       </c>
       <c r="N95" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.207660465116279</v>
+      </c>
+      <c r="O95">
+        <v>3.0528</v>
       </c>
       <c r="P95" s="6">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S95" s="2">
-        <v>0</v>
+        <v>4.9238709677419355E-2</v>
+      </c>
+      <c r="Q95" s="11">
+        <v>111.89</v>
+      </c>
+      <c r="R95" s="11">
+        <v>0.76</v>
+      </c>
+      <c r="S95" s="10"/>
+      <c r="T95" s="11">
+        <v>22.52</v>
+      </c>
+      <c r="U95" s="11">
+        <v>4.6900000000000004</v>
       </c>
     </row>
     <row r="96" spans="1:21">
@@ -5469,27 +5908,58 @@
       <c r="C96" t="s">
         <v>35</v>
       </c>
+      <c r="D96">
+        <v>571</v>
+      </c>
+      <c r="E96">
+        <v>15</v>
+      </c>
+      <c r="F96">
+        <v>589.29999999999995</v>
+      </c>
+      <c r="G96">
+        <v>41</v>
+      </c>
+      <c r="H96">
+        <v>6.96</v>
+      </c>
       <c r="I96">
         <v>332.1</v>
       </c>
       <c r="J96" s="5">
-        <f t="shared" si="59"/>
+        <f t="shared" si="53"/>
         <v>5.4442622950819679</v>
+      </c>
+      <c r="K96">
+        <v>2.2568999999999999</v>
       </c>
       <c r="L96" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>6.3664315937940752E-2</v>
+      </c>
+      <c r="M96">
+        <v>50.792000000000002</v>
       </c>
       <c r="N96" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.1812093023255814</v>
       </c>
       <c r="P96" s="6">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S96" s="2">
-        <v>0</v>
+      <c r="Q96" s="11">
+        <v>116.92</v>
+      </c>
+      <c r="R96" s="11">
+        <v>0.53</v>
+      </c>
+      <c r="S96" s="10"/>
+      <c r="T96" s="11">
+        <v>23.97</v>
+      </c>
+      <c r="U96" s="11">
+        <v>4.63</v>
       </c>
     </row>
     <row r="97" spans="1:21">
@@ -5502,27 +5972,61 @@
       <c r="C97" t="s">
         <v>34</v>
       </c>
+      <c r="D97">
+        <v>599</v>
+      </c>
+      <c r="E97">
+        <v>15.6</v>
+      </c>
+      <c r="F97">
+        <v>584.29999999999995</v>
+      </c>
+      <c r="G97">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="H97">
+        <v>6.99</v>
+      </c>
       <c r="I97">
         <v>327.60000000000002</v>
       </c>
       <c r="J97" s="5">
-        <f t="shared" si="59"/>
+        <f t="shared" si="53"/>
         <v>5.3704918032786892</v>
+      </c>
+      <c r="K97">
+        <v>2.4434</v>
       </c>
       <c r="L97" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>6.8925246826516212E-2</v>
+      </c>
+      <c r="M97">
+        <v>54.710599999999999</v>
       </c>
       <c r="N97" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.272339534883721</v>
+      </c>
+      <c r="O97">
+        <v>3.0112000000000001</v>
       </c>
       <c r="P97" s="6">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S97" s="2">
-        <v>0</v>
+        <v>4.8567741935483875E-2</v>
+      </c>
+      <c r="Q97" s="11">
+        <v>114.88</v>
+      </c>
+      <c r="R97" s="11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S97" s="10"/>
+      <c r="T97" s="11">
+        <v>23.02</v>
+      </c>
+      <c r="U97" s="11">
+        <v>4.8</v>
       </c>
     </row>
     <row r="98" spans="1:21">
@@ -5535,27 +6039,61 @@
       <c r="C98" t="s">
         <v>34</v>
       </c>
+      <c r="D98">
+        <v>502</v>
+      </c>
+      <c r="E98">
+        <v>14.2</v>
+      </c>
+      <c r="F98">
+        <v>593.4</v>
+      </c>
+      <c r="G98">
+        <v>26.8</v>
+      </c>
+      <c r="H98">
+        <v>6.81</v>
+      </c>
       <c r="I98">
         <v>347.5</v>
       </c>
       <c r="J98" s="5">
-        <f t="shared" si="59"/>
+        <f t="shared" si="53"/>
         <v>5.6967213114754101</v>
+      </c>
+      <c r="K98">
+        <v>2.5190000000000001</v>
       </c>
       <c r="L98" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>7.1057827926657255E-2</v>
+      </c>
+      <c r="M98">
+        <v>48.082500000000003</v>
       </c>
       <c r="N98" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.1181976744186046</v>
+      </c>
+      <c r="O98">
+        <v>3.5583999999999998</v>
       </c>
       <c r="P98" s="6">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S98" s="2">
-        <v>0</v>
+        <v>5.7393548387096774E-2</v>
+      </c>
+      <c r="Q98" s="11">
+        <v>151.76</v>
+      </c>
+      <c r="R98" s="11">
+        <v>1.2</v>
+      </c>
+      <c r="S98" s="10"/>
+      <c r="T98" s="11">
+        <v>22.73</v>
+      </c>
+      <c r="U98" s="11">
+        <v>5.93</v>
       </c>
     </row>
     <row r="99" spans="1:21">
@@ -5568,75 +6106,83 @@
       <c r="C99" t="s">
         <v>35</v>
       </c>
+      <c r="D99">
+        <v>539</v>
+      </c>
+      <c r="E99">
+        <v>14.6</v>
+      </c>
+      <c r="F99">
+        <v>599.20000000000005</v>
+      </c>
+      <c r="G99">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="H99">
+        <v>6.9</v>
+      </c>
       <c r="I99">
         <v>337.7</v>
       </c>
       <c r="J99" s="5">
-        <f t="shared" si="59"/>
+        <f t="shared" si="53"/>
         <v>5.5360655737704914</v>
+      </c>
+      <c r="K99">
+        <v>2.3052000000000001</v>
       </c>
       <c r="L99" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>6.502679830747532E-2</v>
+      </c>
+      <c r="M99">
+        <v>54.148499999999999</v>
       </c>
       <c r="N99" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.259267441860465</v>
       </c>
       <c r="P99" s="6">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S99" s="2">
-        <v>0</v>
+      <c r="Q99" s="11">
+        <v>111.38</v>
+      </c>
+      <c r="R99" s="11">
+        <v>1.29</v>
+      </c>
+      <c r="S99" s="10"/>
+      <c r="T99" s="11">
+        <v>22.02</v>
+      </c>
+      <c r="U99" s="11">
+        <v>5.63</v>
       </c>
     </row>
     <row r="100" spans="1:21">
-      <c r="A100" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="B100" s="2"/>
-      <c r="J100" s="5">
-        <f>SUM(J92:J99)</f>
-        <v>38.716393442622952</v>
-      </c>
-      <c r="K100" s="5">
-        <f t="shared" ref="K100" si="60">SUM(K92:K99)</f>
-        <v>0</v>
-      </c>
-      <c r="L100" s="5">
-        <f t="shared" ref="L100" si="61">SUM(L92:L99)</f>
-        <v>0</v>
-      </c>
-      <c r="M100" s="5">
-        <f t="shared" ref="M100" si="62">SUM(M92:M99)</f>
-        <v>0</v>
-      </c>
-      <c r="N100" s="5">
-        <f t="shared" ref="N100" si="63">SUM(N92:N99)</f>
-        <v>0</v>
-      </c>
-      <c r="O100" s="5">
-        <f t="shared" ref="O100" si="64">SUM(O92:O99)</f>
-        <v>0</v>
-      </c>
-      <c r="P100" s="5">
-        <f t="shared" ref="P100" si="65">SUM(P92:P99)</f>
-        <v>0</v>
-      </c>
-      <c r="Q100" s="5"/>
-      <c r="R100" s="5"/>
-      <c r="S100" s="5"/>
-      <c r="T100" s="5"/>
-      <c r="U100" s="5"/>
+      <c r="J100" s="5"/>
+      <c r="L100" s="6"/>
+      <c r="N100" s="6"/>
+      <c r="P100" s="6"/>
+      <c r="Q100" s="11"/>
+      <c r="R100" s="11"/>
+      <c r="S100" s="10"/>
+      <c r="T100" s="11"/>
+      <c r="U100" s="11"/>
     </row>
     <row r="101" spans="1:21">
-      <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="J101" s="5"/>
       <c r="L101" s="6"/>
       <c r="N101" s="6"/>
       <c r="P101" s="6"/>
+      <c r="Q101" s="11"/>
+      <c r="R101" s="11"/>
+      <c r="S101" s="10"/>
+      <c r="T101" s="11"/>
+      <c r="U101" s="11"/>
     </row>
     <row r="102" spans="1:21">
       <c r="A102" t="s">
@@ -5648,24 +6194,55 @@
       <c r="C102" t="s">
         <v>34</v>
       </c>
+      <c r="D102">
+        <v>419</v>
+      </c>
+      <c r="E102">
+        <v>9.9</v>
+      </c>
+      <c r="F102">
+        <v>538.70000000000005</v>
+      </c>
+      <c r="G102">
+        <v>40.9</v>
+      </c>
+      <c r="H102">
+        <v>6.91</v>
+      </c>
       <c r="J102" s="5">
-        <f t="shared" ref="J102:J109" si="66">I102/61</f>
+        <f t="shared" ref="J102:J109" si="54">I102/61</f>
         <v>0</v>
+      </c>
+      <c r="K102">
+        <v>2.0566</v>
       </c>
       <c r="L102" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>5.8014104372355428E-2</v>
+      </c>
+      <c r="M102">
+        <v>43.161499999999997</v>
       </c>
       <c r="N102" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.0037558139534883</v>
       </c>
       <c r="P102" s="6">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S102" s="2">
-        <v>0</v>
+      <c r="Q102" s="11">
+        <v>105.88</v>
+      </c>
+      <c r="R102" s="11">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="S102" s="10"/>
+      <c r="T102" s="11">
+        <v>19.11</v>
+      </c>
+      <c r="U102" s="11">
+        <v>4.6900000000000004</v>
       </c>
     </row>
     <row r="103" spans="1:21">
@@ -5678,24 +6255,55 @@
       <c r="C103" t="s">
         <v>35</v>
       </c>
+      <c r="D103">
+        <v>381</v>
+      </c>
+      <c r="E103">
+        <v>13.8</v>
+      </c>
+      <c r="F103">
+        <v>605.29999999999995</v>
+      </c>
+      <c r="G103">
+        <v>35.1</v>
+      </c>
+      <c r="H103">
+        <v>6.85</v>
+      </c>
       <c r="J103" s="5">
-        <f t="shared" si="66"/>
+        <f t="shared" si="54"/>
         <v>0</v>
+      </c>
+      <c r="K103">
+        <v>1.8793</v>
       </c>
       <c r="L103" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>5.3012693935119884E-2</v>
+      </c>
+      <c r="M103">
+        <v>45.767299999999999</v>
       </c>
       <c r="N103" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.0643558139534883</v>
       </c>
       <c r="P103" s="6">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S103" s="2">
-        <v>0</v>
+      <c r="Q103" s="11">
+        <v>112.97</v>
+      </c>
+      <c r="R103" s="11">
+        <v>1.28</v>
+      </c>
+      <c r="S103" s="10"/>
+      <c r="T103" s="11">
+        <v>22.02</v>
+      </c>
+      <c r="U103" s="11">
+        <v>5.52</v>
       </c>
     </row>
     <row r="104" spans="1:21">
@@ -5708,24 +6316,58 @@
       <c r="C104" t="s">
         <v>35</v>
       </c>
+      <c r="D104">
+        <v>515</v>
+      </c>
+      <c r="E104">
+        <v>13.8</v>
+      </c>
+      <c r="F104">
+        <v>636.4</v>
+      </c>
+      <c r="G104">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="H104">
+        <v>6.82</v>
+      </c>
       <c r="J104" s="5">
-        <f t="shared" si="66"/>
+        <f t="shared" si="54"/>
         <v>0</v>
+      </c>
+      <c r="K104">
+        <v>1.8940999999999999</v>
       </c>
       <c r="L104" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>5.3430183356840612E-2</v>
+      </c>
+      <c r="M104">
+        <v>42.325699999999998</v>
       </c>
       <c r="N104" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>0.98431860465116272</v>
+      </c>
+      <c r="O104">
+        <v>0.61660000000000004</v>
       </c>
       <c r="P104" s="6">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S104" s="2">
-        <v>0</v>
+        <v>9.9451612903225812E-3</v>
+      </c>
+      <c r="Q104" s="11">
+        <v>127.34</v>
+      </c>
+      <c r="R104" s="11">
+        <v>1.28</v>
+      </c>
+      <c r="S104" s="10"/>
+      <c r="T104" s="11">
+        <v>23.52</v>
+      </c>
+      <c r="U104" s="11">
+        <v>5.81</v>
       </c>
     </row>
     <row r="105" spans="1:21">
@@ -5738,24 +6380,58 @@
       <c r="C105" t="s">
         <v>34</v>
       </c>
+      <c r="D105">
+        <v>378</v>
+      </c>
+      <c r="E105">
+        <v>13.9</v>
+      </c>
+      <c r="F105">
+        <v>604.4</v>
+      </c>
+      <c r="G105">
+        <v>32.4</v>
+      </c>
+      <c r="H105">
+        <v>6.64</v>
+      </c>
       <c r="J105" s="5">
-        <f t="shared" si="66"/>
+        <f t="shared" si="54"/>
         <v>0</v>
+      </c>
+      <c r="K105">
+        <v>2.0468000000000002</v>
       </c>
       <c r="L105" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>5.7737658674189E-2</v>
+      </c>
+      <c r="M105">
+        <v>46.565300000000001</v>
       </c>
       <c r="N105" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.082913953488372</v>
+      </c>
+      <c r="O105">
+        <v>0.73609999999999998</v>
       </c>
       <c r="P105" s="6">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S105" s="2">
-        <v>0</v>
+        <v>1.187258064516129E-2</v>
+      </c>
+      <c r="Q105" s="11">
+        <v>142.61000000000001</v>
+      </c>
+      <c r="R105" s="11">
+        <v>1.51</v>
+      </c>
+      <c r="S105" s="10"/>
+      <c r="T105" s="11">
+        <v>21.69</v>
+      </c>
+      <c r="U105" s="11">
+        <v>6.33</v>
       </c>
     </row>
     <row r="106" spans="1:21">
@@ -5768,24 +6444,55 @@
       <c r="C106" t="s">
         <v>35</v>
       </c>
+      <c r="D106">
+        <v>368</v>
+      </c>
+      <c r="E106">
+        <v>13.7</v>
+      </c>
+      <c r="F106">
+        <v>612.20000000000005</v>
+      </c>
+      <c r="G106">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="H106">
+        <v>6.82</v>
+      </c>
       <c r="J106" s="5">
-        <f t="shared" si="66"/>
+        <f t="shared" si="54"/>
         <v>0</v>
+      </c>
+      <c r="K106">
+        <v>1.6537999999999999</v>
       </c>
       <c r="L106" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>4.6651622002820872E-2</v>
+      </c>
+      <c r="M106">
+        <v>40.464500000000001</v>
       </c>
       <c r="N106" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>0.94103488372093025</v>
       </c>
       <c r="P106" s="6">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S106" s="2">
-        <v>0</v>
+      <c r="Q106" s="11">
+        <v>118.12</v>
+      </c>
+      <c r="R106" s="11">
+        <v>1.33</v>
+      </c>
+      <c r="S106" s="10"/>
+      <c r="T106" s="11">
+        <v>23.72</v>
+      </c>
+      <c r="U106" s="11">
+        <v>6.25</v>
       </c>
     </row>
     <row r="107" spans="1:21">
@@ -5798,24 +6505,55 @@
       <c r="C107" t="s">
         <v>34</v>
       </c>
+      <c r="D107">
+        <v>367</v>
+      </c>
+      <c r="E107">
+        <v>14</v>
+      </c>
+      <c r="F107">
+        <v>662.7</v>
+      </c>
+      <c r="G107">
+        <v>34.1</v>
+      </c>
+      <c r="H107">
+        <v>6.84</v>
+      </c>
       <c r="J107" s="5">
-        <f t="shared" si="66"/>
+        <f t="shared" si="54"/>
         <v>0</v>
+      </c>
+      <c r="K107">
+        <v>3.8464999999999998</v>
       </c>
       <c r="L107" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>0.10850493653032439</v>
+      </c>
+      <c r="M107">
+        <v>53.490699999999997</v>
       </c>
       <c r="N107" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.2439697674418604</v>
       </c>
       <c r="P107" s="6">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S107" s="2">
-        <v>0</v>
+      <c r="Q107" s="11">
+        <v>118.04</v>
+      </c>
+      <c r="R107" s="11">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="S107" s="10"/>
+      <c r="T107" s="11">
+        <v>22.11</v>
+      </c>
+      <c r="U107" s="11">
+        <v>6.97</v>
       </c>
     </row>
     <row r="108" spans="1:21">
@@ -5828,24 +6566,58 @@
       <c r="C108" t="s">
         <v>34</v>
       </c>
+      <c r="D108">
+        <v>323</v>
+      </c>
+      <c r="E108">
+        <v>13.5</v>
+      </c>
+      <c r="F108">
+        <v>582.5</v>
+      </c>
+      <c r="G108">
+        <v>26.2</v>
+      </c>
+      <c r="H108">
+        <v>6.63</v>
+      </c>
       <c r="J108" s="5">
-        <f t="shared" si="66"/>
+        <f t="shared" si="54"/>
         <v>0</v>
+      </c>
+      <c r="K108">
+        <v>2.5438000000000001</v>
       </c>
       <c r="L108" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>7.175740479548659E-2</v>
+      </c>
+      <c r="M108">
+        <v>46.504800000000003</v>
       </c>
       <c r="N108" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.0815069767441861</v>
+      </c>
+      <c r="O108">
+        <v>1.7306999999999999</v>
       </c>
       <c r="P108" s="6">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="S108" s="2">
-        <v>0</v>
+        <v>2.7914516129032257E-2</v>
+      </c>
+      <c r="Q108" s="11">
+        <v>113.98</v>
+      </c>
+      <c r="R108" s="11">
+        <v>1.55</v>
+      </c>
+      <c r="S108" s="10"/>
+      <c r="T108" s="11">
+        <v>21.68</v>
+      </c>
+      <c r="U108" s="11">
+        <v>6.33</v>
       </c>
     </row>
     <row r="109" spans="1:21">
@@ -5858,63 +6630,56 @@
       <c r="C109" t="s">
         <v>35</v>
       </c>
+      <c r="D109">
+        <v>348</v>
+      </c>
+      <c r="E109">
+        <v>13.9</v>
+      </c>
+      <c r="F109">
+        <v>630.20000000000005</v>
+      </c>
+      <c r="G109">
+        <v>33.4</v>
+      </c>
+      <c r="H109">
+        <v>6.8</v>
+      </c>
       <c r="J109" s="5">
-        <f t="shared" si="66"/>
+        <f t="shared" si="54"/>
         <v>0</v>
+      </c>
+      <c r="K109">
+        <v>2.2713999999999999</v>
       </c>
       <c r="L109" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>6.4073342736248234E-2</v>
+      </c>
+      <c r="M109">
+        <v>47.848199999999999</v>
       </c>
       <c r="N109" s="6">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1.1127488372093024</v>
       </c>
       <c r="P109" s="6">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="S109" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:21">
-      <c r="A110" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J110" s="5">
-        <f>SUM(J102:J109)</f>
-        <v>0</v>
-      </c>
-      <c r="K110" s="5">
-        <f t="shared" ref="K110" si="67">SUM(K102:K109)</f>
-        <v>0</v>
-      </c>
-      <c r="L110" s="5">
-        <f t="shared" ref="L110" si="68">SUM(L102:L109)</f>
-        <v>0</v>
-      </c>
-      <c r="M110" s="5">
-        <f t="shared" ref="M110" si="69">SUM(M102:M109)</f>
-        <v>0</v>
-      </c>
-      <c r="N110" s="5">
-        <f t="shared" ref="N110" si="70">SUM(N102:N109)</f>
-        <v>0</v>
-      </c>
-      <c r="O110" s="5">
-        <f t="shared" ref="O110" si="71">SUM(O102:O109)</f>
-        <v>0</v>
-      </c>
-      <c r="P110" s="5">
-        <f t="shared" ref="P110" si="72">SUM(P102:P109)</f>
-        <v>0</v>
-      </c>
-      <c r="Q110" s="5"/>
-      <c r="R110" s="5"/>
-      <c r="S110" s="5"/>
-      <c r="T110" s="5"/>
-      <c r="U110" s="5"/>
+      <c r="Q109" s="11">
+        <v>120.45</v>
+      </c>
+      <c r="R109" s="11">
+        <v>1.31</v>
+      </c>
+      <c r="S109" s="10"/>
+      <c r="T109" s="11">
+        <v>24.06</v>
+      </c>
+      <c r="U109" s="11">
+        <v>6.37</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -5933,7 +6698,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:N31"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6467,37 +7232,37 @@
         <f>AVERAGE(MasterData!I52:I59)</f>
         <v>336.44142857142862</v>
       </c>
-      <c r="G11" t="e">
+      <c r="G11">
         <f>AVERAGE(MasterData!K52:K59)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H11" t="e">
+        <v>3.1063714285714288</v>
+      </c>
+      <c r="H11">
         <f>AVERAGE(MasterData!M52:M59)</f>
-        <v>#DIV/0!</v>
+        <v>37.682428571428566</v>
       </c>
       <c r="I11" t="e">
         <f>AVERAGE(MasterData!O52:O59)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J11" t="e">
+      <c r="J11">
         <f>AVERAGE(MasterData!Q52:Q59)</f>
+        <v>121.52142857142857</v>
+      </c>
+      <c r="K11">
+        <f>AVERAGE(MasterData!R52:R59)</f>
+        <v>1.0714285714285716</v>
+      </c>
+      <c r="L11" t="e">
+        <f>AVERAGE(MasterData!S52:S59)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K11" t="e">
-        <f>AVERAGE(MasterData!R52:R59)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L11">
-        <f>AVERAGE(MasterData!S52:S59)</f>
-        <v>0</v>
-      </c>
-      <c r="M11" t="e">
+      <c r="M11">
         <f>AVERAGE(MasterData!T52:T59)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N11" t="e">
+        <v>21.80714285714286</v>
+      </c>
+      <c r="N11">
         <f>AVERAGE(MasterData!U52:U59)</f>
-        <v>#DIV/0!</v>
+        <v>5.5699999999999994</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -6524,37 +7289,37 @@
         <f>STDEV(MasterData!I52:I59)</f>
         <v>14.348228030633182</v>
       </c>
-      <c r="G12" t="e">
+      <c r="G12">
         <f>STDEV(MasterData!K52:K59)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H12" t="e">
+        <v>0.16146918915885797</v>
+      </c>
+      <c r="H12">
         <f>STDEV(MasterData!M52:M59)</f>
-        <v>#DIV/0!</v>
+        <v>1.1053861839711439</v>
       </c>
       <c r="I12" t="e">
         <f>STDEV(MasterData!O52:O59)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J12" t="e">
+      <c r="J12">
         <f>STDEV(MasterData!Q52:Q59)</f>
+        <v>13.621443179256527</v>
+      </c>
+      <c r="K12">
+        <f>STDEV(MasterData!R52:R59)</f>
+        <v>0.1677725217299269</v>
+      </c>
+      <c r="L12" t="e">
+        <f>STDEV(MasterData!S52:S59)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K12" t="e">
-        <f>STDEV(MasterData!R52:R59)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L12">
-        <f>STDEV(MasterData!S52:S59)</f>
-        <v>0</v>
-      </c>
-      <c r="M12" t="e">
+      <c r="M12">
         <f>STDEV(MasterData!T52:T59)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N12" t="e">
+        <v>1.0267377835603777</v>
+      </c>
+      <c r="N12">
         <f>STDEV(MasterData!U52:U59)</f>
-        <v>#DIV/0!</v>
+        <v>0.24027761721253449</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -6581,37 +7346,37 @@
         <f>AVERAGE(MasterData!I62:I69)</f>
         <v>340.80857142857138</v>
       </c>
-      <c r="G13" t="e">
+      <c r="G13">
         <f>AVERAGE(MasterData!K62:K69)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H13" t="e">
+        <v>2.2511142857142858</v>
+      </c>
+      <c r="H13">
         <f>AVERAGE(MasterData!M62:M69)</f>
-        <v>#DIV/0!</v>
+        <v>48.403414285714291</v>
       </c>
       <c r="I13" t="e">
         <f>AVERAGE(MasterData!O62:O69)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J13" t="e">
+      <c r="J13">
         <f>AVERAGE(MasterData!Q62:Q69)</f>
+        <v>126.18999999999998</v>
+      </c>
+      <c r="K13">
+        <f>AVERAGE(MasterData!R62:R69)</f>
+        <v>0.95571428571428563</v>
+      </c>
+      <c r="L13" t="e">
+        <f>AVERAGE(MasterData!S62:S69)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K13" t="e">
-        <f>AVERAGE(MasterData!R62:R69)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L13">
-        <f>AVERAGE(MasterData!S62:S69)</f>
-        <v>0</v>
-      </c>
-      <c r="M13" t="e">
+      <c r="M13">
         <f>AVERAGE(MasterData!T62:T69)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N13" t="e">
+        <v>23.10857142857143</v>
+      </c>
+      <c r="N13">
         <f>AVERAGE(MasterData!U62:U69)</f>
-        <v>#DIV/0!</v>
+        <v>5.2057142857142864</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -6638,37 +7403,37 @@
         <f>STDEV(MasterData!I62:I69)</f>
         <v>9.0078196188486306</v>
       </c>
-      <c r="G14" t="e">
+      <c r="G14">
         <f>STDEV(MasterData!K62:K69)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14" t="e">
+        <v>0.18896615595190075</v>
+      </c>
+      <c r="H14">
         <f>STDEV(MasterData!M62:M69)</f>
-        <v>#DIV/0!</v>
+        <v>2.2386667069400712</v>
       </c>
       <c r="I14" t="e">
         <f>STDEV(MasterData!O62:O69)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J14" t="e">
+      <c r="J14">
         <f>STDEV(MasterData!Q62:Q69)</f>
+        <v>10.088022601084912</v>
+      </c>
+      <c r="K14">
+        <f>STDEV(MasterData!R62:R69)</f>
+        <v>0.2313624244093487</v>
+      </c>
+      <c r="L14" t="e">
+        <f>STDEV(MasterData!S62:S69)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K14" t="e">
-        <f>STDEV(MasterData!R62:R69)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L14">
-        <f>STDEV(MasterData!S62:S69)</f>
-        <v>0</v>
-      </c>
-      <c r="M14" t="e">
+      <c r="M14">
         <f>STDEV(MasterData!T62:T69)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N14" t="e">
+        <v>1.5878332046264449</v>
+      </c>
+      <c r="N14">
         <f>STDEV(MasterData!U62:U69)</f>
-        <v>#DIV/0!</v>
+        <v>0.53353716343091306</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -6707,25 +7472,25 @@
         <f>AVERAGE(MasterData!O72:O79)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J15" t="e">
+      <c r="J15">
         <f>AVERAGE(MasterData!Q72:Q79)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K15" t="e">
+        <v>121.60571428571428</v>
+      </c>
+      <c r="K15">
         <f>AVERAGE(MasterData!R72:R79)</f>
-        <v>#DIV/0!</v>
+        <v>0.92428571428571427</v>
       </c>
       <c r="L15">
         <f>AVERAGE(MasterData!S72:S79)</f>
-        <v>0.11375</v>
-      </c>
-      <c r="M15" t="e">
+        <v>0.91</v>
+      </c>
+      <c r="M15">
         <f>AVERAGE(MasterData!T72:T79)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N15" t="e">
+        <v>22.740000000000002</v>
+      </c>
+      <c r="N15">
         <f>AVERAGE(MasterData!U72:U79)</f>
-        <v>#DIV/0!</v>
+        <v>5.5542857142857143</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -6764,25 +7529,25 @@
         <f>STDEV(MasterData!O72:O79)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J16" t="e">
+      <c r="J16">
         <f>STDEV(MasterData!Q72:Q79)</f>
+        <v>16.713457508988338</v>
+      </c>
+      <c r="K16">
+        <f>STDEV(MasterData!R72:R79)</f>
+        <v>0.2483181523004408</v>
+      </c>
+      <c r="L16" t="e">
+        <f>STDEV(MasterData!S72:S79)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K16" t="e">
-        <f>STDEV(MasterData!R72:R79)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16">
-        <f>STDEV(MasterData!S72:S79)</f>
-        <v>0.32173358543987912</v>
-      </c>
-      <c r="M16" t="e">
+      <c r="M16">
         <f>STDEV(MasterData!T72:T79)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N16" t="e">
+        <v>1.2868695867621296</v>
+      </c>
+      <c r="N16">
         <f>STDEV(MasterData!U72:U79)</f>
-        <v>#DIV/0!</v>
+        <v>0.47874339483196876</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -6814,37 +7579,37 @@
         <f>AVERAGE(MasterData!I82:I89)</f>
         <v>350.18571428571425</v>
       </c>
-      <c r="G18" t="e">
+      <c r="G18">
         <f>AVERAGE(MasterData!K82:K89)</f>
+        <v>2.6095000000000002</v>
+      </c>
+      <c r="H18">
+        <f>AVERAGE(MasterData!M82:M89)</f>
+        <v>52.881757142857147</v>
+      </c>
+      <c r="I18">
+        <f>AVERAGE(MasterData!O82:O89)</f>
+        <v>2.0671749999999998</v>
+      </c>
+      <c r="J18">
+        <f>AVERAGE(MasterData!Q82:Q89)</f>
+        <v>122.88</v>
+      </c>
+      <c r="K18">
+        <f>AVERAGE(MasterData!R82:R89)</f>
+        <v>1.2042857142857142</v>
+      </c>
+      <c r="L18" t="e">
+        <f>AVERAGE(MasterData!S82:S89)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H18" t="e">
-        <f>AVERAGE(MasterData!M82:M89)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" t="e">
-        <f>AVERAGE(MasterData!O82:O89)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" t="e">
-        <f>AVERAGE(MasterData!Q82:Q89)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K18" t="e">
-        <f>AVERAGE(MasterData!R82:R89)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L18">
-        <f>AVERAGE(MasterData!S82:S89)</f>
-        <v>0</v>
-      </c>
-      <c r="M18" t="e">
+      <c r="M18">
         <f>AVERAGE(MasterData!T82:T89)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N18" t="e">
+        <v>23.104285714285712</v>
+      </c>
+      <c r="N18">
         <f>AVERAGE(MasterData!U82:U89)</f>
-        <v>#DIV/0!</v>
+        <v>5.7714285714285714</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -6871,265 +7636,265 @@
         <f>STDEV(MasterData!I82:I89)</f>
         <v>6.6451557722972323</v>
       </c>
-      <c r="G19" t="e">
+      <c r="G19">
         <f>STDEV(MasterData!K82:K89)</f>
+        <v>0.31714653815967625</v>
+      </c>
+      <c r="H19">
+        <f>STDEV(MasterData!M82:M89)</f>
+        <v>2.080894468617716</v>
+      </c>
+      <c r="I19">
+        <f>STDEV(MasterData!O82:O89)</f>
+        <v>1.0581925198973328</v>
+      </c>
+      <c r="J19">
+        <f>STDEV(MasterData!Q82:Q89)</f>
+        <v>10.922580586412112</v>
+      </c>
+      <c r="K19">
+        <f>STDEV(MasterData!R82:R89)</f>
+        <v>0.15873007936505867</v>
+      </c>
+      <c r="L19" t="e">
+        <f>STDEV(MasterData!S82:S89)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H19" t="e">
-        <f>STDEV(MasterData!M82:M89)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" t="e">
-        <f>STDEV(MasterData!O82:O89)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J19" t="e">
-        <f>STDEV(MasterData!Q82:Q89)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K19" t="e">
-        <f>STDEV(MasterData!R82:R89)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L19">
-        <f>STDEV(MasterData!S82:S89)</f>
-        <v>0</v>
-      </c>
-      <c r="M19" t="e">
+      <c r="M19">
         <f>STDEV(MasterData!T82:T89)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N19" t="e">
+        <v>1.0465635375337892</v>
+      </c>
+      <c r="N19">
         <f>STDEV(MasterData!U82:U89)</f>
-        <v>#DIV/0!</v>
+        <v>0.44375025150898306</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="e">
+      <c r="B20">
         <f>AVERAGE(MasterData!E92:E99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C20" t="e">
+        <v>14.885714285714284</v>
+      </c>
+      <c r="C20">
         <f>AVERAGE(MasterData!F92:F99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D20" t="e">
+        <v>589.14285714285711</v>
+      </c>
+      <c r="D20">
         <f>AVERAGE(MasterData!G92:G99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E20" t="e">
+        <v>33.714285714285715</v>
+      </c>
+      <c r="E20">
         <f>AVERAGE(MasterData!H92:H99)</f>
-        <v>#DIV/0!</v>
+        <v>6.9114285714285719</v>
       </c>
       <c r="F20">
         <f>AVERAGE(MasterData!I92:I99)</f>
         <v>337.38571428571424</v>
       </c>
-      <c r="G20" t="e">
+      <c r="G20">
         <f>AVERAGE(MasterData!K92:K99)</f>
+        <v>2.5635285714285714</v>
+      </c>
+      <c r="H20">
+        <f>AVERAGE(MasterData!M92:M99)</f>
+        <v>51.829414285714279</v>
+      </c>
+      <c r="I20">
+        <f>AVERAGE(MasterData!O92:O99)</f>
+        <v>2.57016</v>
+      </c>
+      <c r="J20">
+        <f>AVERAGE(MasterData!Q92:Q99)</f>
+        <v>118.93142857142857</v>
+      </c>
+      <c r="K20">
+        <f>AVERAGE(MasterData!R92:R99)</f>
+        <v>0.91285714285714292</v>
+      </c>
+      <c r="L20" t="e">
+        <f>AVERAGE(MasterData!S92:S99)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H20" t="e">
-        <f>AVERAGE(MasterData!M92:M99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" t="e">
-        <f>AVERAGE(MasterData!O92:O99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J20" t="e">
-        <f>AVERAGE(MasterData!Q92:Q99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K20" t="e">
-        <f>AVERAGE(MasterData!R92:R99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L20">
-        <f>AVERAGE(MasterData!S92:S99)</f>
-        <v>0</v>
-      </c>
-      <c r="M20" t="e">
+      <c r="M20">
         <f>AVERAGE(MasterData!T92:T99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N20" t="e">
+        <v>22.645714285714288</v>
+      </c>
+      <c r="N20">
         <f>AVERAGE(MasterData!U92:U99)</f>
-        <v>#DIV/0!</v>
+        <v>5.0928571428571425</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="e">
+      <c r="B21">
         <f>STDEV(MasterData!E92:E99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C21" t="e">
+        <v>0.46342410895626152</v>
+      </c>
+      <c r="C21">
         <f>STDEV(MasterData!F92:F99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D21" t="e">
+        <v>5.5960870683175283</v>
+      </c>
+      <c r="D21">
         <f>STDEV(MasterData!G92:G99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E21" t="e">
+        <v>4.470059123929861</v>
+      </c>
+      <c r="E21">
         <f>STDEV(MasterData!H92:H99)</f>
-        <v>#DIV/0!</v>
+        <v>7.1978832867394996E-2</v>
       </c>
       <c r="F21">
         <f>STDEV(MasterData!I92:I99)</f>
         <v>8.0308630859180923</v>
       </c>
-      <c r="G21" t="e">
+      <c r="G21">
         <f>STDEV(MasterData!K92:K99)</f>
+        <v>0.47999900595135064</v>
+      </c>
+      <c r="H21">
+        <f>STDEV(MasterData!M92:M99)</f>
+        <v>2.2523507967074234</v>
+      </c>
+      <c r="I21">
+        <f>STDEV(MasterData!O92:O99)</f>
+        <v>0.99036394724363885</v>
+      </c>
+      <c r="J21">
+        <f>STDEV(MasterData!Q92:Q99)</f>
+        <v>14.64172852793401</v>
+      </c>
+      <c r="K21">
+        <f>STDEV(MasterData!R92:R99)</f>
+        <v>0.34970055217353618</v>
+      </c>
+      <c r="L21" t="e">
+        <f>STDEV(MasterData!S92:S99)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H21" t="e">
-        <f>STDEV(MasterData!M92:M99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" t="e">
-        <f>STDEV(MasterData!O92:O99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J21" t="e">
-        <f>STDEV(MasterData!Q92:Q99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K21" t="e">
-        <f>STDEV(MasterData!R92:R99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L21">
-        <f>STDEV(MasterData!S92:S99)</f>
-        <v>0</v>
-      </c>
-      <c r="M21" t="e">
+      <c r="M21">
         <f>STDEV(MasterData!T92:T99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N21" t="e">
+        <v>0.91698522603251642</v>
+      </c>
+      <c r="N21">
         <f>STDEV(MasterData!U92:U99)</f>
-        <v>#DIV/0!</v>
+        <v>0.58721700377612707</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="e">
+      <c r="B22">
         <f>AVERAGE(MasterData!E102:E109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C22" t="e">
+        <v>13.3125</v>
+      </c>
+      <c r="C22">
         <f>AVERAGE(MasterData!F102:F109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D22" t="e">
+        <v>609.04999999999995</v>
+      </c>
+      <c r="D22">
         <f>AVERAGE(MasterData!G102:G109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E22" t="e">
+        <v>34.0625</v>
+      </c>
+      <c r="E22">
         <f>AVERAGE(MasterData!H102:H109)</f>
-        <v>#DIV/0!</v>
+        <v>6.7887499999999994</v>
       </c>
       <c r="F22" t="e">
         <f>AVERAGE(MasterData!I102:I109)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G22" t="e">
+      <c r="G22">
         <f>AVERAGE(MasterData!K102:K109)</f>
+        <v>2.2740374999999999</v>
+      </c>
+      <c r="H22">
+        <f>AVERAGE(MasterData!M102:M109)</f>
+        <v>45.766000000000005</v>
+      </c>
+      <c r="I22">
+        <f>AVERAGE(MasterData!O102:O109)</f>
+        <v>1.0278</v>
+      </c>
+      <c r="J22">
+        <f>AVERAGE(MasterData!Q102:Q109)</f>
+        <v>119.92375000000001</v>
+      </c>
+      <c r="K22">
+        <f>AVERAGE(MasterData!R102:R109)</f>
+        <v>1.3137500000000002</v>
+      </c>
+      <c r="L22" t="e">
+        <f>AVERAGE(MasterData!S102:S109)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H22" t="e">
-        <f>AVERAGE(MasterData!M102:M109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" t="e">
-        <f>AVERAGE(MasterData!O102:O109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J22" t="e">
-        <f>AVERAGE(MasterData!Q102:Q109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K22" t="e">
-        <f>AVERAGE(MasterData!R102:R109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L22">
-        <f>AVERAGE(MasterData!S102:S109)</f>
-        <v>0</v>
-      </c>
-      <c r="M22" t="e">
+      <c r="M22">
         <f>AVERAGE(MasterData!T102:T109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N22" t="e">
+        <v>22.23875</v>
+      </c>
+      <c r="N22">
         <f>AVERAGE(MasterData!U102:U109)</f>
-        <v>#DIV/0!</v>
+        <v>6.0337499999999995</v>
       </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>42</v>
       </c>
-      <c r="B23" t="e">
+      <c r="B23">
         <f>STDEV(MasterData!E102:E109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C23" t="e">
+        <v>1.3871218918527466</v>
+      </c>
+      <c r="C23">
         <f>STDEV(MasterData!F102:F109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D23" t="e">
+        <v>37.365568566338105</v>
+      </c>
+      <c r="D23">
         <f>STDEV(MasterData!G102:G109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E23" t="e">
+        <v>4.0609420089432335</v>
+      </c>
+      <c r="E23">
         <f>STDEV(MasterData!H102:H109)</f>
-        <v>#DIV/0!</v>
+        <v>0.10034761012173073</v>
       </c>
       <c r="F23" t="e">
         <f>STDEV(MasterData!I102:I109)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G23" t="e">
+      <c r="G23">
         <f>STDEV(MasterData!K102:K109)</f>
+        <v>0.68963735591872588</v>
+      </c>
+      <c r="H23">
+        <f>STDEV(MasterData!M102:M109)</f>
+        <v>3.9985040263292753</v>
+      </c>
+      <c r="I23">
+        <f>STDEV(MasterData!O102:O109)</f>
+        <v>0.61165461659338427</v>
+      </c>
+      <c r="J23">
+        <f>STDEV(MasterData!Q102:Q109)</f>
+        <v>11.068974578265406</v>
+      </c>
+      <c r="K23">
+        <f>STDEV(MasterData!R102:R109)</f>
+        <v>0.1561077924292765</v>
+      </c>
+      <c r="L23" t="e">
+        <f>STDEV(MasterData!S102:S109)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H23" t="e">
-        <f>STDEV(MasterData!M102:M109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I23" t="e">
-        <f>STDEV(MasterData!O102:O109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J23" t="e">
-        <f>STDEV(MasterData!Q102:Q109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K23" t="e">
-        <f>STDEV(MasterData!R102:R109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L23">
-        <f>STDEV(MasterData!S102:S109)</f>
-        <v>0</v>
-      </c>
-      <c r="M23" t="e">
+      <c r="M23">
         <f>STDEV(MasterData!T102:T109)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N23" t="e">
+        <v>1.5865275424199676</v>
+      </c>
+      <c r="N23">
         <f>STDEV(MasterData!U102:U109)</f>
-        <v>#DIV/0!</v>
+        <v>0.68988482475596835</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -7138,19 +7903,19 @@
       </c>
       <c r="B25">
         <f>AVERAGE(MasterData!E2:E109)</f>
-        <v>14.620000000000001</v>
+        <v>14.505333333333335</v>
       </c>
       <c r="C25">
         <f>AVERAGE(MasterData!F2:F109)</f>
-        <v>646.73333333333335</v>
+        <v>637.33866666666665</v>
       </c>
       <c r="D25">
         <f>AVERAGE(MasterData!G2:G109)</f>
-        <v>29.161666666666672</v>
+        <v>30.109333333333336</v>
       </c>
       <c r="E25">
         <f>AVERAGE(MasterData!H2:H109)</f>
-        <v>6.8237288135593221</v>
+        <v>6.8282432432432438</v>
       </c>
       <c r="F25">
         <f>AVERAGE(MasterData!I2:I109)</f>
@@ -7158,35 +7923,35 @@
       </c>
       <c r="G25">
         <f>AVERAGE(MasterData!K2:K109)</f>
-        <v>3.079780758666717</v>
+        <v>3.3773199659598703</v>
       </c>
       <c r="H25">
         <f>AVERAGE(MasterData!M2:M109)</f>
-        <v>52.394730594447076</v>
+        <v>58.694575893107356</v>
       </c>
       <c r="I25">
         <f>AVERAGE(MasterData!O2:O109)</f>
-        <v>1.1103692443899904</v>
+        <v>1.3323897114425345</v>
       </c>
       <c r="J25">
         <f>AVERAGE(MasterData!Q2:Q109)</f>
-        <v>112.171575</v>
+        <v>117.15846987951809</v>
       </c>
       <c r="K25">
         <f>AVERAGE(MasterData!R2:R109)</f>
-        <v>1.3103474999999998</v>
+        <v>1.185589156626506</v>
       </c>
       <c r="L25">
         <f>AVERAGE(MasterData!S2:S109)</f>
-        <v>4.414313725490196E-2</v>
+        <v>0.56282500000000002</v>
       </c>
       <c r="M25">
         <f>AVERAGE(MasterData!T2:T109)</f>
-        <v>21.593625000000007</v>
+        <v>22.114397590361449</v>
       </c>
       <c r="N25">
         <f>AVERAGE(MasterData!U2:U109)</f>
-        <v>5.8946975000000004</v>
+        <v>5.7158783132530111</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -7195,19 +7960,19 @@
       </c>
       <c r="B26">
         <f>STDEV(MasterData!E2:E109)</f>
-        <v>1.1967186775597427</v>
+        <v>1.2326518691952855</v>
       </c>
       <c r="C26">
         <f>STDEV(MasterData!F2:F109)</f>
-        <v>31.218674695084577</v>
+        <v>35.909111594350193</v>
       </c>
       <c r="D26">
         <f>STDEV(MasterData!G2:G109)</f>
-        <v>8.1386312859742791</v>
+        <v>7.7225568748105697</v>
       </c>
       <c r="E26">
         <f>STDEV(MasterData!H2:H109)</f>
-        <v>0.23134463249241569</v>
+        <v>0.21157827081188713</v>
       </c>
       <c r="F26">
         <f>STDEV(MasterData!I2:I109)</f>
@@ -7215,35 +7980,35 @@
       </c>
       <c r="G26">
         <f>STDEV(MasterData!K2:K109)</f>
-        <v>4.2161472487647291</v>
+        <v>4.0366728249444854</v>
       </c>
       <c r="H26">
         <f>STDEV(MasterData!M2:M109)</f>
-        <v>71.286843306894156</v>
+        <v>66.1266429518313</v>
       </c>
       <c r="I26">
         <f>STDEV(MasterData!O2:O109)</f>
-        <v>1.5696118618123815</v>
+        <v>1.5270589402890959</v>
       </c>
       <c r="J26">
         <f>STDEV(MasterData!Q2:Q109)</f>
-        <v>6.9139809894471016</v>
+        <v>11.193286564087824</v>
       </c>
       <c r="K26">
         <f>STDEV(MasterData!R2:R109)</f>
-        <v>0.18439934922225432</v>
+        <v>0.25799053915913761</v>
       </c>
       <c r="L26">
         <f>STDEV(MasterData!S2:S109)</f>
-        <v>0.19481862360144317</v>
+        <v>0.49329042409112306</v>
       </c>
       <c r="M26">
         <f>STDEV(MasterData!T2:T109)</f>
-        <v>0.84661365291831403</v>
+        <v>1.2031703695000566</v>
       </c>
       <c r="N26">
         <f>STDEV(MasterData!U2:U109)</f>
-        <v>0.45105166767973126</v>
+        <v>0.5513366828142604</v>
       </c>
     </row>
   </sheetData>
@@ -7261,9 +8026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -7510,7 +8273,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updating file pathways, fixing cation labeling error
</commit_message>
<xml_diff>
--- a/Data/Summary.xlsx
+++ b/Data/Summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joe/Desktop/R_Scripts/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joe/R_Scripts/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB8EAC1-C03F-E346-AFEB-5A26A9E070F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C952FBFE-018F-EB47-B513-E8F5BD2AAF26}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="25600" windowHeight="15960" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29260" yWindow="1400" windowWidth="25600" windowHeight="15960" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterData" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="53">
   <si>
     <t>Month</t>
   </si>
@@ -185,6 +186,12 @@
   </si>
   <si>
     <t>Charge balance</t>
+  </si>
+  <si>
+    <t>Ag Mean</t>
+  </si>
+  <si>
+    <t>Prairie Mean</t>
   </si>
 </sst>
 </file>
@@ -690,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q109"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
@@ -5098,11 +5105,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J9" sqref="J9"/>
+      <selection pane="topRight" activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7693,6 +7700,234 @@
       <c r="O46" s="6">
         <f>STDEV(MasterData!Q102,MasterData!Q105,MasterData!Q107,MasterData!Q108)</f>
         <v>0.97454262776613942</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="6">
+        <f>AVERAGE(C3,C7,C15,C19,C23,C27,C31,C35,C39,C43)</f>
+        <v>14.445000000000002</v>
+      </c>
+      <c r="D50" s="6">
+        <f>AVERAGE(D3,D7,D15,D19,D23,D27,D31,D35,D39,D43)</f>
+        <v>638.83916666666664</v>
+      </c>
+      <c r="E50" s="6">
+        <f>AVERAGE(E3,E7,E15,E19,E23,E27,E31,E35,E39,E43)</f>
+        <v>31.772500000000001</v>
+      </c>
+      <c r="F50" s="6">
+        <f>AVERAGE(F3,F7,F15,F19,F23,F27,F31,F35,F39,F43)</f>
+        <v>6.8778333333333332</v>
+      </c>
+      <c r="G50" s="6">
+        <f>AVERAGE(G3,G7,G11,G15,G19,G23,G27,G31,G35,G39)</f>
+        <v>339.82291666666669</v>
+      </c>
+      <c r="H50" s="6">
+        <f>AVERAGE(H3,H7,H11,H15,H19,H23,H27,H35,H39,H43)</f>
+        <v>2.2681804146595281</v>
+      </c>
+      <c r="I50" s="6">
+        <f>AVERAGE(I3,I7,I11,I15,I19,I23,I27,I35,I39,I43)</f>
+        <v>41.558382751948457</v>
+      </c>
+      <c r="J50" s="6">
+        <f>AVERAGE(J3,J7,J11,J15,J19,J35,J39,J43)</f>
+        <v>0.83965206511880164</v>
+      </c>
+      <c r="K50" s="6">
+        <f>AVERAGE(K3,K7,K11,K15,K19,K23,K27,K31,K35,K39,K43)</f>
+        <v>116.07990151515151</v>
+      </c>
+      <c r="L50" s="6">
+        <f>AVERAGE(L3,L7,L11,L15,L19,L23,L27,L31,L35,L39,L43)</f>
+        <v>1.1139378787878789</v>
+      </c>
+      <c r="M50" s="6" t="e">
+        <f>AVERAGE(M3,M7,M11,M15,M19,M23,M27,M31,M35,M39,M43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N50" s="6">
+        <f>AVERAGE(N3,N7,N11,N15,N19,N23,N27,N31,N35,N39,N43)</f>
+        <v>22.509100757575755</v>
+      </c>
+      <c r="O50" s="6">
+        <f>AVERAGE(O3,O7,O11,O15,O19,O23,O27,O31,O35,O39,O43)</f>
+        <v>5.5710128787878785</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="6">
+        <f>AVERAGE(C4,C8,C16,C20,C24,C28,C32,C36,C40,C44)</f>
+        <v>0.30000969249146625</v>
+      </c>
+      <c r="D51" s="6">
+        <f>AVERAGE(D4,D8,D16,D20,D24,D28,D32,D36,D40,D44)</f>
+        <v>7.5870957282340425</v>
+      </c>
+      <c r="E51" s="6">
+        <f>AVERAGE(E4,E8,E16,E20,E24,E28,E32,E36,E40,E44)</f>
+        <v>3.2815243088606332</v>
+      </c>
+      <c r="F51" s="6">
+        <f>AVERAGE(F4,F8,F16,F20,F24,F28,F32,F36,F40,F44)</f>
+        <v>5.247865207987943E-2</v>
+      </c>
+      <c r="G51" s="6">
+        <f>AVERAGE(G4,G8,G12,G16,G20,G24,G28,G32,G36,G40)</f>
+        <v>6.9148050649372719</v>
+      </c>
+      <c r="H51" s="6">
+        <f>AVERAGE(H4,H8,H12,H16,H20,H24,H28,H36,H40,H44)</f>
+        <v>0.15055190029363763</v>
+      </c>
+      <c r="I51" s="6">
+        <f>AVERAGE(I4,I8,I12,I16,I20,I24,I28,I36,I40,I44)</f>
+        <v>1.3455148551585014</v>
+      </c>
+      <c r="J51" s="6">
+        <f>AVERAGE(J4,J8,J12,J16,J20)</f>
+        <v>0.11796722679571951</v>
+      </c>
+      <c r="K51" s="6">
+        <f>AVERAGE(K4,K8,K12,K16,K20,K24,K28,K32,K36,K40,K44)</f>
+        <v>8.6571466910815893</v>
+      </c>
+      <c r="L51" s="6">
+        <f>AVERAGE(L4,L8,L12,L16,L20,L24,L28,L32,L36,L40,L44)</f>
+        <v>0.22824962348669156</v>
+      </c>
+      <c r="M51" s="6" t="e">
+        <f>AVERAGE(M4,M8,M12,M16,M20,M24,M28,M32,M36,M40,M44)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N51" s="6">
+        <f>AVERAGE(N4,N8,N12,N16,N20,N24,N28,N32,N36,N40,N44)</f>
+        <v>0.87129466991843896</v>
+      </c>
+      <c r="O51" s="6">
+        <f>AVERAGE(O4,O8,O12,O16,O20,O24,O28,O32,O36,O40,O44)</f>
+        <v>0.40937575872007875</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="6">
+        <f>AVERAGE(C5,C9,C17,C21,C25,C29,C33,C37,C41,C45)</f>
+        <v>14.584999999999999</v>
+      </c>
+      <c r="D52" s="6">
+        <f>AVERAGE(D5,D9,D17,D21,D25,D29,D33,D37,D41,D45)</f>
+        <v>633.79250000000002</v>
+      </c>
+      <c r="E52" s="6">
+        <f>AVERAGE(E5,E9,E17,E21,E25,E29,E33,E37,E41,E45)</f>
+        <v>28.2925</v>
+      </c>
+      <c r="F52" s="6">
+        <f>AVERAGE(F5,F9,F17,F21,F25,F29,F33,F37,F41,F45)</f>
+        <v>6.7896666666666663</v>
+      </c>
+      <c r="G52" s="6">
+        <f>AVERAGE(G5,G9,G13,G17,G21,G25,G29,G33,G37,G41)</f>
+        <v>342.72974999999997</v>
+      </c>
+      <c r="H52" s="6">
+        <f>AVERAGE(H5,H9,H13,H17,H21,H25,H29,H37,H41,H45)</f>
+        <v>2.3770038280002606</v>
+      </c>
+      <c r="I52" s="6">
+        <f>AVERAGE(I5,I9,I13,I17,I21,I25,I29,I37,I41,I45)</f>
+        <v>41.412580632368282</v>
+      </c>
+      <c r="J52" s="6">
+        <f>AVERAGE(J5,J9,J13,J17,J21,J37,J41,J45)</f>
+        <v>1.3358224223994233</v>
+      </c>
+      <c r="K52" s="6">
+        <f>AVERAGE(K5,K9,K13,K17,K21,K25,K29,K33,K37,K41,K45)</f>
+        <v>118.43713636363636</v>
+      </c>
+      <c r="L52" s="6">
+        <f>AVERAGE(L5,L9,L13,L17,L21,L25,L29,L33,L37,L41,L45)</f>
+        <v>1.227211363636364</v>
+      </c>
+      <c r="M52" s="6" t="e">
+        <f>AVERAGE(M5,M9,M13,M17,M21,M25,M29,M33,M37,M41,M45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N52" s="6">
+        <f>AVERAGE(N5,N9,N13,N17,N21,N25,N29,N33,N37,N41,N45)</f>
+        <v>21.807679545454548</v>
+      </c>
+      <c r="O52" s="6">
+        <f>AVERAGE(O5,O9,O13,O17,O21,O25,O29,O33,O37,O41,O45)</f>
+        <v>5.8161363636363639</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="6">
+        <f>AVERAGE(C6,C10,C18,C22,C26,C30,C34,C38,C42,C46)</f>
+        <v>0.75966375550034204</v>
+      </c>
+      <c r="D53" s="6">
+        <f>AVERAGE(D6,D10,D18,D22,D26,D30,D34,D38,D42,D46)</f>
+        <v>19.253439105781748</v>
+      </c>
+      <c r="E53" s="6">
+        <f>AVERAGE(E6,E10,E18,E22,E26,E30,E34,E38,E42,E46)</f>
+        <v>3.5463388830997515</v>
+      </c>
+      <c r="F53" s="6">
+        <f>AVERAGE(F6,F10,F18,F22,F26,F30,F34,F38,F42,F46)</f>
+        <v>0.11370416870136835</v>
+      </c>
+      <c r="G53" s="6">
+        <f>AVERAGE(G6,G10,G14,G18,G22,G26,G30,G34,G38,G42)</f>
+        <v>13.156755877405407</v>
+      </c>
+      <c r="H53" s="6">
+        <f>AVERAGE(H6,H10,H14,H18,H22,H26,H30,H38,H42,H46)</f>
+        <v>0.25134488622937445</v>
+      </c>
+      <c r="I53" s="6">
+        <f>AVERAGE(I6,I10,I14,I18,I22,I26,I30,I38,I42,I46)</f>
+        <v>1.6536224169239564</v>
+      </c>
+      <c r="J53" s="6">
+        <f>AVERAGE(J6,J10,J14,J18,J22,J38,J42,J46)</f>
+        <v>0.38887673083033336</v>
+      </c>
+      <c r="K53" s="6">
+        <f>AVERAGE(K6,K10,K14,K18,K22,K26,K30,K34,K38,K42,K46)</f>
+        <v>9.7081405781464589</v>
+      </c>
+      <c r="L53" s="6">
+        <f>AVERAGE(L6,L10,L14,L18,L22,L26,L30,L34,L38,L42,L46)</f>
+        <v>0.15946162531564642</v>
+      </c>
+      <c r="M53" s="6" t="e">
+        <f>AVERAGE(M6,M10,M14,M18,M22,M26,M30,M34,M38,M42,M46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N53" s="6">
+        <f>AVERAGE(N6,N10,N14,N18,N22,N26,N30,N34,N38,N42,N46)</f>
+        <v>0.92474577139431036</v>
+      </c>
+      <c r="O53" s="6">
+        <f>AVERAGE(O6,O10,O14,O18,O22,O26,O30,O34,O38,O42,O46)</f>
+        <v>0.51248071237121295</v>
       </c>
     </row>
   </sheetData>
@@ -7710,8 +7945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Transferring PHREEQC caturation data to master file
</commit_message>
<xml_diff>
--- a/Data/Summary.xlsx
+++ b/Data/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joe/R_Scripts/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C952FBFE-018F-EB47-B513-E8F5BD2AAF26}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D1CCAD-8BB5-E841-A840-A9DF515B629C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29260" yWindow="1400" windowWidth="25600" windowHeight="15960" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-720" yWindow="460" windowWidth="19800" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="57">
   <si>
     <t>Month</t>
   </si>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>Prairie Mean</t>
+  </si>
+  <si>
+    <t>Aragonite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Calcite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dolomite</t>
   </si>
 </sst>
 </file>
@@ -695,11 +707,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q109"/>
+  <dimension ref="A1:U109"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R1" sqref="R1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,7 +724,7 @@
     <col min="10" max="10" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -764,8 +776,20 @@
       <c r="Q1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -814,8 +838,20 @@
       <c r="Q2">
         <v>5.53</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R2">
+        <v>-6.7299999999999999E-2</v>
+      </c>
+      <c r="S2">
+        <v>8.2699999999999996E-2</v>
+      </c>
+      <c r="T2">
+        <v>-1.3968</v>
+      </c>
+      <c r="U2">
+        <v>-0.31130000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -865,8 +901,20 @@
       <c r="Q3" s="10">
         <v>5.3906000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R3">
+        <v>-0.20250000000000001</v>
+      </c>
+      <c r="S3">
+        <v>-5.0900000000000001E-2</v>
+      </c>
+      <c r="T3">
+        <v>-1.4384999999999999</v>
+      </c>
+      <c r="U3">
+        <v>-0.64190000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -916,8 +964,20 @@
       <c r="Q4" s="10">
         <v>6.1277999999999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R4">
+        <v>-0.2102</v>
+      </c>
+      <c r="S4">
+        <v>-5.8200000000000002E-2</v>
+      </c>
+      <c r="T4">
+        <v>-1.3806</v>
+      </c>
+      <c r="U4">
+        <v>-0.64349999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -967,8 +1027,20 @@
       <c r="Q5" s="10">
         <v>5.8407999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R5">
+        <v>-4.9700000000000001E-2</v>
+      </c>
+      <c r="S5">
+        <v>0.1007</v>
+      </c>
+      <c r="T5">
+        <v>-1.5624</v>
+      </c>
+      <c r="U5">
+        <v>-0.2656</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1018,8 +1090,20 @@
       <c r="Q6" s="10">
         <v>6.0766999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R6">
+        <v>-0.16259999999999999</v>
+      </c>
+      <c r="S6">
+        <v>-1.09E-2</v>
+      </c>
+      <c r="T6">
+        <v>-1.3701000000000001</v>
+      </c>
+      <c r="U6">
+        <v>-0.53300000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1069,8 +1153,20 @@
       <c r="Q7" s="10">
         <v>7.3661000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R7">
+        <v>-0.2535</v>
+      </c>
+      <c r="S7">
+        <v>-0.1027</v>
+      </c>
+      <c r="T7">
+        <v>-1.2857000000000001</v>
+      </c>
+      <c r="U7">
+        <v>-0.70899999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1120,8 +1216,20 @@
       <c r="Q8" s="10">
         <v>5.8030999999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R8">
+        <v>-5.9200000000000003E-2</v>
+      </c>
+      <c r="S8">
+        <v>9.1399999999999995E-2</v>
+      </c>
+      <c r="T8">
+        <v>-1.5533999999999999</v>
+      </c>
+      <c r="U8">
+        <v>-0.32140000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1171,8 +1279,20 @@
       <c r="Q9" s="10">
         <v>5.4602000000000004</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R9">
+        <v>-0.23100000000000001</v>
+      </c>
+      <c r="S9">
+        <v>-7.9600000000000004E-2</v>
+      </c>
+      <c r="T9">
+        <v>-1.3197000000000001</v>
+      </c>
+      <c r="U9">
+        <v>-0.66379999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
@@ -1186,14 +1306,14 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="I11" s="5"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1243,8 +1363,20 @@
       <c r="Q12" s="10">
         <v>6.2778</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R12">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="S12">
+        <v>0.1699</v>
+      </c>
+      <c r="T12">
+        <v>-1.5316000000000001</v>
+      </c>
+      <c r="U12">
+        <v>-0.16930000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1294,8 +1426,20 @@
       <c r="Q13" s="10">
         <v>5.2759999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R13">
+        <v>-0.19819999999999999</v>
+      </c>
+      <c r="S13">
+        <v>-4.6600000000000003E-2</v>
+      </c>
+      <c r="T13">
+        <v>-1.4379999999999999</v>
+      </c>
+      <c r="U13">
+        <v>-0.59560000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1347,8 +1491,20 @@
       <c r="Q14" s="10">
         <v>6.1856999999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R14">
+        <v>-0.21429999999999999</v>
+      </c>
+      <c r="S14">
+        <v>-6.2399999999999997E-2</v>
+      </c>
+      <c r="T14">
+        <v>-1.3801000000000001</v>
+      </c>
+      <c r="U14">
+        <v>-0.68169999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1398,8 +1554,20 @@
       <c r="Q15" s="10">
         <v>6.5944000000000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R15">
+        <v>-1.49E-2</v>
+      </c>
+      <c r="S15">
+        <v>0.1356</v>
+      </c>
+      <c r="T15">
+        <v>-1.5446</v>
+      </c>
+      <c r="U15">
+        <v>-0.24940000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1449,8 +1617,20 @@
       <c r="Q16" s="10">
         <v>5.6196999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R16">
+        <v>-0.29270000000000002</v>
+      </c>
+      <c r="S16">
+        <v>-0.1411</v>
+      </c>
+      <c r="T16">
+        <v>-1.3371</v>
+      </c>
+      <c r="U16">
+        <v>-0.76280000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1500,8 +1680,20 @@
       <c r="Q17" s="10">
         <v>6.4991000000000003</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R17">
+        <v>-0.28749999999999998</v>
+      </c>
+      <c r="S17">
+        <v>-0.13650000000000001</v>
+      </c>
+      <c r="T17">
+        <v>-1.3203</v>
+      </c>
+      <c r="U17">
+        <v>-0.77769999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1551,8 +1743,20 @@
       <c r="Q18" s="10">
         <v>5.8525999999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R18">
+        <v>-5.3600000000000002E-2</v>
+      </c>
+      <c r="S18">
+        <v>9.8299999999999998E-2</v>
+      </c>
+      <c r="T18">
+        <v>-1.5731999999999999</v>
+      </c>
+      <c r="U18">
+        <v>-0.3412</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1602,8 +1806,20 @@
       <c r="Q19" s="10">
         <v>5.7286000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R19">
+        <v>-0.31259999999999999</v>
+      </c>
+      <c r="S19">
+        <v>-0.16109999999999999</v>
+      </c>
+      <c r="T19">
+        <v>-1.3062</v>
+      </c>
+      <c r="U19">
+        <v>-0.80310000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1626,14 +1842,14 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1671,8 +1887,20 @@
       <c r="Q22" s="10">
         <v>5.5218999999999996</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R22">
+        <v>5.8599999999999999E-2</v>
+      </c>
+      <c r="S22">
+        <v>0.2024</v>
+      </c>
+      <c r="T22">
+        <v>-1.3599000000000001</v>
+      </c>
+      <c r="U22">
+        <v>3.5200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1710,8 +1938,20 @@
       <c r="Q23" s="10">
         <v>5.4311999999999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R23">
+        <v>-7.3000000000000001E-3</v>
+      </c>
+      <c r="S23">
+        <v>0.13650000000000001</v>
+      </c>
+      <c r="T23">
+        <v>-1.4402999999999999</v>
+      </c>
+      <c r="U23">
+        <v>-0.1066</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1749,8 +1989,20 @@
       <c r="Q24" s="10">
         <v>5.5679999999999996</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R24">
+        <v>2.8899999999999999E-2</v>
+      </c>
+      <c r="S24">
+        <v>0.17269999999999999</v>
+      </c>
+      <c r="T24">
+        <v>-1.4047000000000001</v>
+      </c>
+      <c r="U24">
+        <v>-2.3199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1788,8 +2040,20 @@
       <c r="Q25" s="10">
         <v>5.8174000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R25">
+        <v>1.49E-2</v>
+      </c>
+      <c r="S25">
+        <v>0.15870000000000001</v>
+      </c>
+      <c r="T25">
+        <v>-1.3979999999999999</v>
+      </c>
+      <c r="U25">
+        <v>-4.7100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1827,8 +2091,20 @@
       <c r="Q26" s="10">
         <v>6.1433999999999997</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R26">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="S26">
+        <v>0.20810000000000001</v>
+      </c>
+      <c r="T26">
+        <v>-1.4125000000000001</v>
+      </c>
+      <c r="U26">
+        <v>2.1899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1866,8 +2142,20 @@
       <c r="Q27" s="10">
         <v>6.4687000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R27">
+        <v>1.17E-2</v>
+      </c>
+      <c r="S27">
+        <v>0.15540000000000001</v>
+      </c>
+      <c r="T27">
+        <v>-1.3976</v>
+      </c>
+      <c r="U27">
+        <v>-5.5800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1905,8 +2193,20 @@
       <c r="Q28" s="10">
         <v>5.7138</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R28">
+        <v>-1.95E-2</v>
+      </c>
+      <c r="S28">
+        <v>0.12429999999999999</v>
+      </c>
+      <c r="T28">
+        <v>-1.4165000000000001</v>
+      </c>
+      <c r="U28">
+        <v>-0.1166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1944,8 +2244,20 @@
       <c r="Q29" s="10">
         <v>5.5807000000000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R29">
+        <v>1.47E-2</v>
+      </c>
+      <c r="S29">
+        <v>0.1585</v>
+      </c>
+      <c r="T29">
+        <v>-1.4016</v>
+      </c>
+      <c r="U29">
+        <v>-5.0200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>50</v>
       </c>
@@ -1968,13 +2280,13 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="I31" s="5"/>
       <c r="J31" s="6"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -2024,8 +2336,20 @@
       <c r="Q32" s="10">
         <v>5.2262000000000004</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R32">
+        <v>-0.5615</v>
+      </c>
+      <c r="S32">
+        <v>-0.40960000000000002</v>
+      </c>
+      <c r="T32">
+        <v>-1.0874999999999999</v>
+      </c>
+      <c r="U32">
+        <v>-1.3594999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -2075,8 +2399,20 @@
       <c r="Q33" s="10">
         <v>5.7843999999999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R33">
+        <v>-0.23089999999999999</v>
+      </c>
+      <c r="S33">
+        <v>-7.8899999999999998E-2</v>
+      </c>
+      <c r="T33">
+        <v>-1.4370000000000001</v>
+      </c>
+      <c r="U33">
+        <v>-0.67869999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -2126,8 +2462,20 @@
       <c r="Q34" s="10">
         <v>5.4188999999999998</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R34">
+        <v>-0.39279999999999998</v>
+      </c>
+      <c r="S34">
+        <v>-0.24060000000000001</v>
+      </c>
+      <c r="T34">
+        <v>-1.2735000000000001</v>
+      </c>
+      <c r="U34">
+        <v>-0.9899</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -2179,8 +2527,20 @@
       <c r="Q35" s="10">
         <v>6.9112</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R35">
+        <v>-0.56920000000000004</v>
+      </c>
+      <c r="S35">
+        <v>-0.4178</v>
+      </c>
+      <c r="T35">
+        <v>-1.042</v>
+      </c>
+      <c r="U35">
+        <v>-1.3434999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -2230,8 +2590,20 @@
       <c r="Q36" s="10">
         <v>6.1120000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R36">
+        <v>-0.34710000000000002</v>
+      </c>
+      <c r="S36">
+        <v>-0.1948</v>
+      </c>
+      <c r="T36">
+        <v>-1.2599</v>
+      </c>
+      <c r="U36">
+        <v>-0.91390000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -2281,8 +2653,20 @@
       <c r="Q37" s="10">
         <v>6.0846999999999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R37">
+        <v>-0.47010000000000002</v>
+      </c>
+      <c r="S37">
+        <v>-0.31819999999999998</v>
+      </c>
+      <c r="T37">
+        <v>-1.1924999999999999</v>
+      </c>
+      <c r="U37">
+        <v>-1.1532</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -2332,8 +2716,20 @@
       <c r="Q38" s="10">
         <v>6.0003000000000002</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R38">
+        <v>-0.85589999999999999</v>
+      </c>
+      <c r="S38">
+        <v>-0.70379999999999998</v>
+      </c>
+      <c r="T38">
+        <v>-0.77190000000000003</v>
+      </c>
+      <c r="U38">
+        <v>-1.9557</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -2383,8 +2779,20 @@
       <c r="Q39" s="10">
         <v>5.6623000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R39">
+        <v>-0.42020000000000002</v>
+      </c>
+      <c r="S39">
+        <v>-0.2681</v>
+      </c>
+      <c r="T39">
+        <v>-1.2024999999999999</v>
+      </c>
+      <c r="U39">
+        <v>-1.046</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>50</v>
       </c>
@@ -2407,14 +2815,14 @@
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="I41" s="5"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -2464,8 +2872,20 @@
       <c r="Q42" s="10">
         <v>5.4579000000000004</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R42">
+        <v>-0.41599999999999998</v>
+      </c>
+      <c r="S42">
+        <v>-0.26440000000000002</v>
+      </c>
+      <c r="T42">
+        <v>-1.1571</v>
+      </c>
+      <c r="U42">
+        <v>-1.0559000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -2515,8 +2935,20 @@
       <c r="Q43" s="10">
         <v>6.0738000000000003</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R43">
+        <v>-0.13159999999999999</v>
+      </c>
+      <c r="S43">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="T43">
+        <v>-1.4388000000000001</v>
+      </c>
+      <c r="U43">
+        <v>-0.48159999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -2566,8 +2998,20 @@
       <c r="Q44" s="10">
         <v>5.492</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R44">
+        <v>-0.1132</v>
+      </c>
+      <c r="S44">
+        <v>3.8199999999999998E-2</v>
+      </c>
+      <c r="T44">
+        <v>-1.5011000000000001</v>
+      </c>
+      <c r="U44">
+        <v>-0.43380000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -2617,8 +3061,20 @@
       <c r="Q45" s="10">
         <v>5.9353999999999996</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R45">
+        <v>-0.50929999999999997</v>
+      </c>
+      <c r="S45">
+        <v>-0.3579</v>
+      </c>
+      <c r="T45">
+        <v>-1.1034999999999999</v>
+      </c>
+      <c r="U45">
+        <v>-1.2197</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -2668,8 +3124,20 @@
       <c r="Q46" s="10">
         <v>6.0716999999999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R46">
+        <v>-0.2487</v>
+      </c>
+      <c r="S46">
+        <v>-9.74E-2</v>
+      </c>
+      <c r="T46">
+        <v>-1.3486</v>
+      </c>
+      <c r="U46">
+        <v>-0.69940000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -2719,8 +3187,20 @@
       <c r="Q47" s="10">
         <v>6.1843000000000004</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R47">
+        <v>-0.39850000000000002</v>
+      </c>
+      <c r="S47">
+        <v>-0.24740000000000001</v>
+      </c>
+      <c r="T47">
+        <v>-1.1857</v>
+      </c>
+      <c r="U47">
+        <v>-1.0348999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -2770,8 +3250,20 @@
       <c r="Q48" s="10">
         <v>5.9943</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R48">
+        <v>-0.62419999999999998</v>
+      </c>
+      <c r="S48">
+        <v>-0.47210000000000002</v>
+      </c>
+      <c r="T48">
+        <v>-1.0414000000000001</v>
+      </c>
+      <c r="U48">
+        <v>-1.4703999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -2821,8 +3313,20 @@
       <c r="Q49" s="10">
         <v>5.5042</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R49">
+        <v>-0.4461</v>
+      </c>
+      <c r="S49">
+        <v>-0.29430000000000001</v>
+      </c>
+      <c r="T49">
+        <v>-1.2422</v>
+      </c>
+      <c r="U49">
+        <v>-1.0029999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
@@ -2845,13 +3349,13 @@
       <c r="P50" s="5"/>
       <c r="Q50" s="5"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="I51" s="5"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -2898,8 +3402,20 @@
       <c r="Q52">
         <v>5.63</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R52">
+        <v>-0.56340000000000001</v>
+      </c>
+      <c r="S52">
+        <v>-0.4098</v>
+      </c>
+      <c r="T52">
+        <v>-1.0351999999999999</v>
+      </c>
+      <c r="U52">
+        <v>-1.3696999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -2946,8 +3462,20 @@
       <c r="Q53">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R53">
+        <v>-0.4516</v>
+      </c>
+      <c r="S53">
+        <v>-0.29830000000000001</v>
+      </c>
+      <c r="T53">
+        <v>-1.2439</v>
+      </c>
+      <c r="U53">
+        <v>-1.1508</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -2967,7 +3495,7 @@
       <c r="N54" s="10"/>
       <c r="O54" s="10"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -3014,8 +3542,20 @@
       <c r="Q55">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R55">
+        <v>-0.65810000000000002</v>
+      </c>
+      <c r="S55">
+        <v>-0.50509999999999999</v>
+      </c>
+      <c r="T55">
+        <v>-0.96409999999999996</v>
+      </c>
+      <c r="U55">
+        <v>-1.5703</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -3062,8 +3602,20 @@
       <c r="Q56">
         <v>5.34</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R56">
+        <v>-0.43519999999999998</v>
+      </c>
+      <c r="S56">
+        <v>-0.28179999999999999</v>
+      </c>
+      <c r="T56">
+        <v>-1.2068000000000001</v>
+      </c>
+      <c r="U56">
+        <v>-1.1254999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -3110,8 +3662,20 @@
       <c r="Q57">
         <v>5.97</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R57">
+        <v>-0.56240000000000001</v>
+      </c>
+      <c r="S57">
+        <v>-0.4098</v>
+      </c>
+      <c r="T57">
+        <v>-1.0867</v>
+      </c>
+      <c r="U57">
+        <v>-1.3888</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -3158,8 +3722,20 @@
       <c r="Q58">
         <v>5.37</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R58">
+        <v>-0.71870000000000001</v>
+      </c>
+      <c r="S58">
+        <v>-0.56510000000000005</v>
+      </c>
+      <c r="T58">
+        <v>-0.85419999999999996</v>
+      </c>
+      <c r="U58">
+        <v>-1.8320000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -3206,8 +3782,20 @@
       <c r="Q59">
         <v>5.48</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R59">
+        <v>-0.52610000000000001</v>
+      </c>
+      <c r="S59">
+        <v>-0.373</v>
+      </c>
+      <c r="T59">
+        <v>-1.1214</v>
+      </c>
+      <c r="U59">
+        <v>-1.3172999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>50</v>
       </c>
@@ -3230,11 +3818,11 @@
       <c r="P60" s="5"/>
       <c r="Q60" s="5"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="I61" s="9"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -3281,8 +3869,20 @@
       <c r="Q62">
         <v>4.49</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R62">
+        <v>-0.44629999999999997</v>
+      </c>
+      <c r="S62">
+        <v>-0.29449999999999998</v>
+      </c>
+      <c r="T62">
+        <v>-1.0402</v>
+      </c>
+      <c r="U62">
+        <v>-1.141</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -3329,8 +3929,20 @@
       <c r="Q63">
         <v>5.57</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R63">
+        <v>-0.34389999999999998</v>
+      </c>
+      <c r="S63">
+        <v>-0.1928</v>
+      </c>
+      <c r="T63">
+        <v>-1.2009000000000001</v>
+      </c>
+      <c r="U63">
+        <v>-0.93369999999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -3347,7 +3959,7 @@
       <c r="P64" s="10"/>
       <c r="Q64" s="10"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -3394,8 +4006,20 @@
       <c r="Q65">
         <v>5.61</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R65">
+        <v>-0.62419999999999998</v>
+      </c>
+      <c r="S65">
+        <v>-0.4733</v>
+      </c>
+      <c r="T65">
+        <v>-0.90569999999999995</v>
+      </c>
+      <c r="U65">
+        <v>-1.5056</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -3442,8 +4066,20 @@
       <c r="Q66">
         <v>4.59</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R66">
+        <v>-0.48089999999999999</v>
+      </c>
+      <c r="S66">
+        <v>-0.32979999999999998</v>
+      </c>
+      <c r="T66">
+        <v>-1.0999000000000001</v>
+      </c>
+      <c r="U66">
+        <v>-1.1434</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -3490,8 +4126,20 @@
       <c r="Q67">
         <v>5.86</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R67">
+        <v>-0.47349999999999998</v>
+      </c>
+      <c r="S67">
+        <v>-0.32300000000000001</v>
+      </c>
+      <c r="T67">
+        <v>-1.1218999999999999</v>
+      </c>
+      <c r="U67">
+        <v>-1.1603000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -3538,8 +4186,20 @@
       <c r="Q68">
         <v>5.37</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R68">
+        <v>-0.76270000000000004</v>
+      </c>
+      <c r="S68">
+        <v>-0.61119999999999997</v>
+      </c>
+      <c r="T68">
+        <v>-0.83460000000000001</v>
+      </c>
+      <c r="U68">
+        <v>-1.7363</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -3586,8 +4246,20 @@
       <c r="Q69">
         <v>4.95</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R69">
+        <v>-0.45619999999999999</v>
+      </c>
+      <c r="S69">
+        <v>-0.30459999999999998</v>
+      </c>
+      <c r="T69">
+        <v>-1.1109</v>
+      </c>
+      <c r="U69">
+        <v>-1.1457999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>50</v>
       </c>
@@ -3611,12 +4283,12 @@
       <c r="P70" s="5"/>
       <c r="Q70" s="5"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="I71" s="9"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>9</v>
       </c>
@@ -3657,8 +4329,20 @@
       <c r="Q72">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R72">
+        <v>0.1411</v>
+      </c>
+      <c r="S72">
+        <v>0.29310000000000003</v>
+      </c>
+      <c r="T72">
+        <v>-1.6935</v>
+      </c>
+      <c r="U72">
+        <v>4.4699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>9</v>
       </c>
@@ -3699,8 +4383,20 @@
       <c r="Q73">
         <v>4.6399999999999997</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R73">
+        <v>2.58E-2</v>
+      </c>
+      <c r="S73">
+        <v>0.17710000000000001</v>
+      </c>
+      <c r="T73">
+        <v>-1.6735</v>
+      </c>
+      <c r="U73">
+        <v>-2.92E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>9</v>
       </c>
@@ -3720,7 +4416,7 @@
       <c r="P74" s="10"/>
       <c r="Q74" s="10"/>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>9</v>
       </c>
@@ -3761,8 +4457,20 @@
       <c r="Q75">
         <v>5.82</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R75">
+        <v>0.16320000000000001</v>
+      </c>
+      <c r="S75">
+        <v>0.31509999999999999</v>
+      </c>
+      <c r="T75">
+        <v>-1.6933</v>
+      </c>
+      <c r="U75">
+        <v>6.8900000000000003E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>9</v>
       </c>
@@ -3803,8 +4511,20 @@
       <c r="Q76">
         <v>6.07</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R76">
+        <v>4.6100000000000002E-2</v>
+      </c>
+      <c r="S76">
+        <v>0.19769999999999999</v>
+      </c>
+      <c r="T76">
+        <v>-1.6233</v>
+      </c>
+      <c r="U76">
+        <v>-0.1231</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>9</v>
       </c>
@@ -3847,8 +4567,20 @@
       <c r="Q77">
         <v>5.94</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R77">
+        <v>9.6799999999999997E-2</v>
+      </c>
+      <c r="S77">
+        <v>0.248</v>
+      </c>
+      <c r="T77">
+        <v>-1.6795</v>
+      </c>
+      <c r="U77">
+        <v>-3.5900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>9</v>
       </c>
@@ -3889,8 +4621,20 @@
       <c r="Q78">
         <v>5.58</v>
       </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R78">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="S78">
+        <v>0.184</v>
+      </c>
+      <c r="T78">
+        <v>-1.6142000000000001</v>
+      </c>
+      <c r="U78">
+        <v>-0.20530000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -3931,8 +4675,20 @@
       <c r="Q79">
         <v>5.33</v>
       </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R79">
+        <v>0.1497</v>
+      </c>
+      <c r="S79">
+        <v>0.30149999999999999</v>
+      </c>
+      <c r="T79">
+        <v>-1.6494</v>
+      </c>
+      <c r="U79">
+        <v>2.18E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>50</v>
       </c>
@@ -3956,10 +4712,10 @@
       <c r="P80" s="5"/>
       <c r="Q80" s="5"/>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -4009,8 +4765,20 @@
       <c r="Q82" s="11">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R82">
+        <v>-0.20480000000000001</v>
+      </c>
+      <c r="S82">
+        <v>-5.4399999999999997E-2</v>
+      </c>
+      <c r="T82">
+        <v>-1.3194999999999999</v>
+      </c>
+      <c r="U82">
+        <v>-0.57299999999999995</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -4060,8 +4828,20 @@
       <c r="Q83" s="11">
         <v>6.15</v>
       </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R83">
+        <v>-0.1095</v>
+      </c>
+      <c r="S83">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="T83">
+        <v>-1.375</v>
+      </c>
+      <c r="U83">
+        <v>-0.41470000000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>11</v>
       </c>
@@ -4077,7 +4857,7 @@
       <c r="P84" s="10"/>
       <c r="Q84" s="10"/>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -4127,8 +4907,20 @@
       <c r="Q85" s="11">
         <v>5.01</v>
       </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R85">
+        <v>-0.27079999999999999</v>
+      </c>
+      <c r="S85">
+        <v>-0.1205</v>
+      </c>
+      <c r="T85">
+        <v>-1.2043999999999999</v>
+      </c>
+      <c r="U85">
+        <v>-0.78010000000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>11</v>
       </c>
@@ -4175,8 +4967,20 @@
       <c r="Q86" s="11">
         <v>5.37</v>
       </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R86">
+        <v>-0.21740000000000001</v>
+      </c>
+      <c r="S86">
+        <v>-6.7100000000000007E-2</v>
+      </c>
+      <c r="T86">
+        <v>-1.3654999999999999</v>
+      </c>
+      <c r="U86">
+        <v>-0.60209999999999997</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>11</v>
       </c>
@@ -4226,8 +5030,20 @@
       <c r="Q87" s="11">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R87">
+        <v>-0.14019999999999999</v>
+      </c>
+      <c r="S87">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="T87">
+        <v>-1.3226</v>
+      </c>
+      <c r="U87">
+        <v>-0.4849</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -4274,8 +5090,20 @@
       <c r="Q88" s="11">
         <v>6.01</v>
       </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R88">
+        <v>-0.46279999999999999</v>
+      </c>
+      <c r="S88">
+        <v>-0.31209999999999999</v>
+      </c>
+      <c r="T88">
+        <v>-1.1081000000000001</v>
+      </c>
+      <c r="U88">
+        <v>-1.1059000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>11</v>
       </c>
@@ -4322,8 +5150,20 @@
       <c r="Q89" s="11">
         <v>6.26</v>
       </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R89">
+        <v>-0.222</v>
+      </c>
+      <c r="S89">
+        <v>-7.1400000000000005E-2</v>
+      </c>
+      <c r="T89">
+        <v>-1.3156000000000001</v>
+      </c>
+      <c r="U89">
+        <v>-0.66010000000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B90" s="2"/>
       <c r="M90" s="11"/>
       <c r="N90" s="11"/>
@@ -4331,7 +5171,7 @@
       <c r="P90" s="11"/>
       <c r="Q90" s="11"/>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B91" s="2"/>
       <c r="M91" s="11"/>
       <c r="N91" s="11"/>
@@ -4339,7 +5179,7 @@
       <c r="P91" s="11"/>
       <c r="Q91" s="11"/>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>20</v>
       </c>
@@ -4389,8 +5229,20 @@
       <c r="Q92" s="11">
         <v>5.53</v>
       </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R92">
+        <v>-0.2283</v>
+      </c>
+      <c r="S92">
+        <v>-7.6899999999999996E-2</v>
+      </c>
+      <c r="T92">
+        <v>-1.4065000000000001</v>
+      </c>
+      <c r="U92">
+        <v>-0.67259999999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>20</v>
       </c>
@@ -4440,8 +5292,20 @@
       <c r="Q93" s="11">
         <v>4.4400000000000004</v>
       </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R93">
+        <v>-0.1464</v>
+      </c>
+      <c r="S93">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="T93">
+        <v>-1.4226000000000001</v>
+      </c>
+      <c r="U93">
+        <v>-0.4733</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>20</v>
       </c>
@@ -4457,7 +5321,7 @@
       <c r="P94" s="10"/>
       <c r="Q94" s="10"/>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>20</v>
       </c>
@@ -4507,8 +5371,20 @@
       <c r="Q95" s="11">
         <v>4.6900000000000004</v>
       </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R95">
+        <v>-0.3276</v>
+      </c>
+      <c r="S95">
+        <v>-0.17630000000000001</v>
+      </c>
+      <c r="T95">
+        <v>-1.2895000000000001</v>
+      </c>
+      <c r="U95">
+        <v>-0.8448</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>20</v>
       </c>
@@ -4555,8 +5431,20 @@
       <c r="Q96" s="11">
         <v>4.63</v>
       </c>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R96">
+        <v>-0.1731</v>
+      </c>
+      <c r="S96">
+        <v>-2.1899999999999999E-2</v>
+      </c>
+      <c r="T96">
+        <v>-1.4355</v>
+      </c>
+      <c r="U96">
+        <v>-0.52449999999999997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>20</v>
       </c>
@@ -4606,8 +5494,20 @@
       <c r="Q97" s="11">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R97">
+        <v>-0.14779999999999999</v>
+      </c>
+      <c r="S97">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="T97">
+        <v>-1.4679</v>
+      </c>
+      <c r="U97">
+        <v>-0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>20</v>
       </c>
@@ -4657,8 +5557,20 @@
       <c r="Q98" s="11">
         <v>5.93</v>
       </c>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R98">
+        <v>-0.2167</v>
+      </c>
+      <c r="S98">
+        <v>-6.4899999999999999E-2</v>
+      </c>
+      <c r="T98">
+        <v>-1.2745</v>
+      </c>
+      <c r="U98">
+        <v>-0.75980000000000003</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>20</v>
       </c>
@@ -4705,8 +5617,20 @@
       <c r="Q99" s="11">
         <v>5.63</v>
       </c>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R99">
+        <v>-0.25130000000000002</v>
+      </c>
+      <c r="S99">
+        <v>-9.98E-2</v>
+      </c>
+      <c r="T99">
+        <v>-1.3691</v>
+      </c>
+      <c r="U99">
+        <v>-0.70299999999999996</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B100" s="2"/>
       <c r="M100" s="11"/>
       <c r="N100" s="11"/>
@@ -4714,7 +5638,7 @@
       <c r="P100" s="11"/>
       <c r="Q100" s="11"/>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B101" s="2"/>
       <c r="M101" s="11"/>
       <c r="N101" s="11"/>
@@ -4722,7 +5646,7 @@
       <c r="P101" s="11"/>
       <c r="Q101" s="11"/>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>4</v>
       </c>
@@ -4766,8 +5690,20 @@
       <c r="Q102" s="11">
         <v>4.6900000000000004</v>
       </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R102">
+        <v>-0.38890000000000002</v>
+      </c>
+      <c r="S102">
+        <v>-0.23369999999999999</v>
+      </c>
+      <c r="T102">
+        <v>-1.4669000000000001</v>
+      </c>
+      <c r="U102">
+        <v>-1.0932999999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>4</v>
       </c>
@@ -4811,8 +5747,20 @@
       <c r="Q103" s="11">
         <v>5.52</v>
       </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R103">
+        <v>-0.30430000000000001</v>
+      </c>
+      <c r="S103">
+        <v>-0.1522</v>
+      </c>
+      <c r="T103">
+        <v>-1.3225</v>
+      </c>
+      <c r="U103">
+        <v>-0.82720000000000005</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>4</v>
       </c>
@@ -4860,7 +5808,7 @@
         <v>5.81</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>4</v>
       </c>
@@ -4907,8 +5855,20 @@
       <c r="Q105" s="11">
         <v>6.33</v>
       </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R105">
+        <v>-0.42370000000000002</v>
+      </c>
+      <c r="S105">
+        <v>-0.27160000000000001</v>
+      </c>
+      <c r="T105">
+        <v>-1.1162000000000001</v>
+      </c>
+      <c r="U105">
+        <v>-1.1718</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>4</v>
       </c>
@@ -4952,8 +5912,20 @@
       <c r="Q106" s="11">
         <v>6.25</v>
       </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R106">
+        <v>-0.3014</v>
+      </c>
+      <c r="S106">
+        <v>-0.14910000000000001</v>
+      </c>
+      <c r="T106">
+        <v>-1.2757000000000001</v>
+      </c>
+      <c r="U106">
+        <v>-0.80979999999999996</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>4</v>
       </c>
@@ -4997,8 +5969,20 @@
       <c r="Q107" s="11">
         <v>6.97</v>
       </c>
-    </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R107">
+        <v>-0.29089999999999999</v>
+      </c>
+      <c r="S107">
+        <v>-0.1389</v>
+      </c>
+      <c r="T107">
+        <v>-1.3053999999999999</v>
+      </c>
+      <c r="U107">
+        <v>-0.81459999999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>4</v>
       </c>
@@ -5045,8 +6029,20 @@
       <c r="Q108" s="11">
         <v>6.33</v>
       </c>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R108">
+        <v>-0.52629999999999999</v>
+      </c>
+      <c r="S108">
+        <v>-0.37390000000000001</v>
+      </c>
+      <c r="T108">
+        <v>-1.1046</v>
+      </c>
+      <c r="U108">
+        <v>-1.2865</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>4</v>
       </c>
@@ -5089,6 +6085,18 @@
       </c>
       <c r="Q109" s="11">
         <v>6.37</v>
+      </c>
+      <c r="R109">
+        <v>-0.29809999999999998</v>
+      </c>
+      <c r="S109">
+        <v>-0.14610000000000001</v>
+      </c>
+      <c r="T109">
+        <v>-1.2383999999999999</v>
+      </c>
+      <c r="U109">
+        <v>-0.80259999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -5105,16 +6113,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J51" sqref="J51"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P1" sqref="P1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5160,8 +6168,20 @@
       <c r="O1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5220,8 +6240,24 @@
         <f>AVERAGE(MasterData!Q3,MasterData!Q4,MasterData!Q6,MasterData!Q9)</f>
         <v>5.7638249999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="6">
+        <f>AVERAGE(MasterData!R3,MasterData!R4,MasterData!R6,MasterData!R9)</f>
+        <v>-0.201575</v>
+      </c>
+      <c r="Q3" s="6">
+        <f>AVERAGE(MasterData!S3,MasterData!S4,MasterData!S6,MasterData!S9)</f>
+        <v>-4.99E-2</v>
+      </c>
+      <c r="R3" s="6">
+        <f>AVERAGE(MasterData!T3,MasterData!T4,MasterData!T6,MasterData!T9)</f>
+        <v>-1.3772249999999999</v>
+      </c>
+      <c r="S3" s="6">
+        <f>AVERAGE(MasterData!U3,MasterData!U4,MasterData!U6,MasterData!U9)</f>
+        <v>-0.62054999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>44</v>
       </c>
@@ -5277,8 +6313,24 @@
         <f>STDEV(MasterData!Q3,MasterData!Q4,MasterData!Q6,MasterData!Q9)</f>
         <v>0.3923661587089281</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4" s="6">
+        <f>STDEV(MasterData!R3,MasterData!R4,MasterData!R6,MasterData!R9)</f>
+        <v>2.8636384199126771E-2</v>
+      </c>
+      <c r="Q4" s="6">
+        <f>STDEV(MasterData!S3,MasterData!S4,MasterData!S6,MasterData!S9)</f>
+        <v>2.8711089611275057E-2</v>
+      </c>
+      <c r="R4" s="6">
+        <f>STDEV(MasterData!T3,MasterData!T4,MasterData!T6,MasterData!T9)</f>
+        <v>4.8737075209741416E-2</v>
+      </c>
+      <c r="S4" s="6">
+        <f>STDEV(MasterData!U3,MasterData!U4,MasterData!U6,MasterData!U9)</f>
+        <v>5.9211738701037964E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>45</v>
       </c>
@@ -5334,8 +6386,24 @@
         <f>AVERAGE(MasterData!Q2,MasterData!Q8,MasterData!Q7,MasterData!Q5)</f>
         <v>6.1349999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" s="6">
+        <f>AVERAGE(MasterData!R2,MasterData!R8,MasterData!R7,MasterData!R5)</f>
+        <v>-0.10742500000000001</v>
+      </c>
+      <c r="Q5" s="6">
+        <f>AVERAGE(MasterData!S2,MasterData!S8,MasterData!S7,MasterData!S5)</f>
+        <v>4.3024999999999994E-2</v>
+      </c>
+      <c r="R5" s="6">
+        <f>AVERAGE(MasterData!T2,MasterData!T8,MasterData!T7,MasterData!T5)</f>
+        <v>-1.4495750000000001</v>
+      </c>
+      <c r="S5" s="6">
+        <f>AVERAGE(MasterData!U2,MasterData!U8,MasterData!U7,MasterData!U5)</f>
+        <v>-0.40182499999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>46</v>
       </c>
@@ -5391,8 +6459,24 @@
         <f>STDEV(MasterData!Q2,MasterData!Q8,MasterData!Q7,MasterData!Q5)</f>
         <v>0.832334760377901</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6" s="6">
+        <f>STDEV(MasterData!R2,MasterData!R8,MasterData!R7,MasterData!R5)</f>
+        <v>9.764860043373208E-2</v>
+      </c>
+      <c r="Q6" s="6">
+        <f>STDEV(MasterData!S2,MasterData!S8,MasterData!S7,MasterData!S5)</f>
+        <v>9.7427626985367971E-2</v>
+      </c>
+      <c r="R6" s="6">
+        <f>STDEV(MasterData!T2,MasterData!T8,MasterData!T7,MasterData!T5)</f>
+        <v>0.13310312731111912</v>
+      </c>
+      <c r="S6" s="6">
+        <f>STDEV(MasterData!U2,MasterData!U8,MasterData!U7,MasterData!U5)</f>
+        <v>0.20621727013031674</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -5451,8 +6535,24 @@
         <f>AVERAGE(MasterData!Q13,MasterData!Q14,MasterData!Q16,MasterData!Q19)</f>
         <v>5.7025000000000006</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7" s="6">
+        <f>AVERAGE(MasterData!R13,MasterData!R14,MasterData!R16,MasterData!R19)</f>
+        <v>-0.25445000000000001</v>
+      </c>
+      <c r="Q7" s="6">
+        <f>AVERAGE(MasterData!S13,MasterData!S14,MasterData!S16,MasterData!S19)</f>
+        <v>-0.1028</v>
+      </c>
+      <c r="R7" s="6">
+        <f>AVERAGE(MasterData!T13,MasterData!T14,MasterData!T16,MasterData!T19)</f>
+        <v>-1.3653500000000003</v>
+      </c>
+      <c r="S7" s="6">
+        <f>AVERAGE(MasterData!U13,MasterData!U14,MasterData!U16,MasterData!U19)</f>
+        <v>-0.71079999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>44</v>
       </c>
@@ -5508,8 +6608,24 @@
         <f>STDEV(MasterData!Q13,MasterData!Q14,MasterData!Q16,MasterData!Q19)</f>
         <v>0.37546484078628006</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P8" s="6">
+        <f>STDEV(MasterData!R13,MasterData!R14,MasterData!R16,MasterData!R19)</f>
+        <v>5.6629115008682999E-2</v>
+      </c>
+      <c r="Q8" s="6">
+        <f>STDEV(MasterData!S13,MasterData!S14,MasterData!S16,MasterData!S19)</f>
+        <v>5.6734410487228409E-2</v>
+      </c>
+      <c r="R8" s="6">
+        <f>STDEV(MasterData!T13,MasterData!T14,MasterData!T16,MasterData!T19)</f>
+        <v>5.7132506800711379E-2</v>
+      </c>
+      <c r="S8" s="6">
+        <f>STDEV(MasterData!U13,MasterData!U14,MasterData!U16,MasterData!U19)</f>
+        <v>9.190781613479182E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>45</v>
       </c>
@@ -5565,8 +6681,24 @@
         <f>AVERAGE(MasterData!Q12,MasterData!Q15,MasterData!Q17,MasterData!Q18)</f>
         <v>6.3059749999999992</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9" s="6">
+        <f>AVERAGE(MasterData!R12,MasterData!R15,MasterData!R17,MasterData!R18)</f>
+        <v>-8.4099999999999994E-2</v>
+      </c>
+      <c r="Q9" s="6">
+        <f>AVERAGE(MasterData!S12,MasterData!S15,MasterData!S17,MasterData!S18)</f>
+        <v>6.6824999999999996E-2</v>
+      </c>
+      <c r="R9" s="6">
+        <f>AVERAGE(MasterData!T12,MasterData!T15,MasterData!T17,MasterData!T18)</f>
+        <v>-1.4924249999999999</v>
+      </c>
+      <c r="S9" s="6">
+        <f>AVERAGE(MasterData!U12,MasterData!U15,MasterData!U17,MasterData!U18)</f>
+        <v>-0.38439999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>46</v>
       </c>
@@ -5622,8 +6754,24 @@
         <f>STDEV(MasterData!Q12,MasterData!Q15,MasterData!Q17,MasterData!Q18)</f>
         <v>0.33006512867412519</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10" s="6">
+        <f>STDEV(MasterData!R12,MasterData!R15,MasterData!R17,MasterData!R18)</f>
+        <v>0.13885740887687628</v>
+      </c>
+      <c r="Q10" s="6">
+        <f>STDEV(MasterData!S12,MasterData!S15,MasterData!S17,MasterData!S18)</f>
+        <v>0.13866769330549444</v>
+      </c>
+      <c r="R10" s="6">
+        <f>STDEV(MasterData!T12,MasterData!T15,MasterData!T17,MasterData!T18)</f>
+        <v>0.1160582145591886</v>
+      </c>
+      <c r="S10" s="6">
+        <f>STDEV(MasterData!U12,MasterData!U15,MasterData!U17,MasterData!U18)</f>
+        <v>0.27144314321787538</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -5682,8 +6830,24 @@
         <f>AVERAGE(MasterData!Q23,MasterData!Q24,MasterData!Q26,MasterData!Q29)</f>
         <v>5.6808249999999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P11" s="6">
+        <f>AVERAGE(MasterData!R23,MasterData!R24,MasterData!R26,MasterData!R29)</f>
+        <v>2.5149999999999999E-2</v>
+      </c>
+      <c r="Q11" s="6">
+        <f>AVERAGE(MasterData!S23,MasterData!S24,MasterData!S26,MasterData!S29)</f>
+        <v>0.16895000000000002</v>
+      </c>
+      <c r="R11" s="6">
+        <f>AVERAGE(MasterData!T23,MasterData!T24,MasterData!T26,MasterData!T29)</f>
+        <v>-1.4147750000000001</v>
+      </c>
+      <c r="S11" s="6">
+        <f>AVERAGE(MasterData!U23,MasterData!U24,MasterData!U26,MasterData!U29)</f>
+        <v>-3.9524999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>44</v>
       </c>
@@ -5739,8 +6903,24 @@
         <f>STDEV(MasterData!Q23,MasterData!Q24,MasterData!Q26,MasterData!Q29)</f>
         <v>0.31572285710730541</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P12" s="6">
+        <f>STDEV(MasterData!R23,MasterData!R24,MasterData!R26,MasterData!R29)</f>
+        <v>3.0049902939388452E-2</v>
+      </c>
+      <c r="Q12" s="6">
+        <f>STDEV(MasterData!S23,MasterData!S24,MasterData!S26,MasterData!S29)</f>
+        <v>3.0049902939388345E-2</v>
+      </c>
+      <c r="R12" s="6">
+        <f>STDEV(MasterData!T23,MasterData!T24,MasterData!T26,MasterData!T29)</f>
+        <v>1.7623729268612012E-2</v>
+      </c>
+      <c r="S12" s="6">
+        <f>STDEV(MasterData!U23,MasterData!U24,MasterData!U26,MasterData!U29)</f>
+        <v>5.3704585465302684E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>45</v>
       </c>
@@ -5796,8 +6976,24 @@
         <f>AVERAGE(MasterData!Q22,MasterData!Q25,MasterData!Q27,MasterData!Q28)</f>
         <v>5.8804499999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P13" s="6">
+        <f>AVERAGE(MasterData!R22,MasterData!R25,MasterData!R27,MasterData!R28)</f>
+        <v>1.6424999999999999E-2</v>
+      </c>
+      <c r="Q13" s="6">
+        <f>AVERAGE(MasterData!S22,MasterData!S25,MasterData!S27,MasterData!S28)</f>
+        <v>0.16019999999999998</v>
+      </c>
+      <c r="R13" s="6">
+        <f>AVERAGE(MasterData!T22,MasterData!T25,MasterData!T27,MasterData!T28)</f>
+        <v>-1.393</v>
+      </c>
+      <c r="S13" s="6">
+        <f>AVERAGE(MasterData!U22,MasterData!U25,MasterData!U27,MasterData!U28)</f>
+        <v>-4.6075000000000005E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>46</v>
       </c>
@@ -5853,8 +7049,24 @@
         <f>STDEV(MasterData!Q22,MasterData!Q25,MasterData!Q27,MasterData!Q28)</f>
         <v>0.41082992831584231</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P14" s="6">
+        <f>STDEV(MasterData!R22,MasterData!R25,MasterData!R27,MasterData!R28)</f>
+        <v>3.2114314046335579E-2</v>
+      </c>
+      <c r="Q14" s="6">
+        <f>STDEV(MasterData!S22,MasterData!S25,MasterData!S27,MasterData!S28)</f>
+        <v>3.211925694449784E-2</v>
+      </c>
+      <c r="R14" s="6">
+        <f>STDEV(MasterData!T22,MasterData!T25,MasterData!T27,MasterData!T28)</f>
+        <v>2.3762856169520782E-2</v>
+      </c>
+      <c r="S14" s="6">
+        <f>STDEV(MasterData!U22,MasterData!U25,MasterData!U27,MasterData!U28)</f>
+        <v>6.2383297711273114E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -5913,8 +7125,24 @@
         <f>AVERAGE(MasterData!Q33,MasterData!Q34,MasterData!Q36,MasterData!Q39)</f>
         <v>5.7444000000000006</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P15" s="6">
+        <f>AVERAGE(MasterData!R33,MasterData!R34,MasterData!R36,MasterData!R39)</f>
+        <v>-0.34775</v>
+      </c>
+      <c r="Q15" s="6">
+        <f>AVERAGE(MasterData!S33,MasterData!S34,MasterData!S36,MasterData!S39)</f>
+        <v>-0.1956</v>
+      </c>
+      <c r="R15" s="6">
+        <f>AVERAGE(MasterData!T33,MasterData!T34,MasterData!T36,MasterData!T39)</f>
+        <v>-1.2932250000000001</v>
+      </c>
+      <c r="S15" s="6">
+        <f>AVERAGE(MasterData!U33,MasterData!U34,MasterData!U36,MasterData!U39)</f>
+        <v>-0.90712499999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>44</v>
       </c>
@@ -5970,8 +7198,24 @@
         <f>STDEV(MasterData!Q33,MasterData!Q34,MasterData!Q36,MasterData!Q39)</f>
         <v>0.28834031976121555</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16" s="6">
+        <f>STDEV(MasterData!R33,MasterData!R34,MasterData!R36,MasterData!R39)</f>
+        <v>8.3532129547059006E-2</v>
+      </c>
+      <c r="Q16" s="6">
+        <f>STDEV(MasterData!S33,MasterData!S34,MasterData!S36,MasterData!S39)</f>
+        <v>8.3468117665769115E-2</v>
+      </c>
+      <c r="R16" s="6">
+        <f>STDEV(MasterData!T33,MasterData!T34,MasterData!T36,MasterData!T39)</f>
+        <v>0.10066761726924242</v>
+      </c>
+      <c r="S16" s="6">
+        <f>STDEV(MasterData!U33,MasterData!U34,MasterData!U36,MasterData!U39)</f>
+        <v>0.16161873602195187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>45</v>
       </c>
@@ -6027,8 +7271,24 @@
         <f>AVERAGE(MasterData!Q32,MasterData!Q35,MasterData!Q37,MasterData!Q38)</f>
         <v>6.0555999999999992</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P17" s="6">
+        <f>AVERAGE(MasterData!R32,MasterData!R35,MasterData!R37,MasterData!R38)</f>
+        <v>-0.61417500000000003</v>
+      </c>
+      <c r="Q17" s="6">
+        <f>AVERAGE(MasterData!S32,MasterData!S35,MasterData!S37,MasterData!S38)</f>
+        <v>-0.46234999999999998</v>
+      </c>
+      <c r="R17" s="6">
+        <f>AVERAGE(MasterData!T32,MasterData!T35,MasterData!T37,MasterData!T38)</f>
+        <v>-1.0234749999999999</v>
+      </c>
+      <c r="S17" s="6">
+        <f>AVERAGE(MasterData!U32,MasterData!U35,MasterData!U37,MasterData!U38)</f>
+        <v>-1.4529749999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>46</v>
       </c>
@@ -6084,8 +7344,24 @@
         <f>STDEV(MasterData!Q32,MasterData!Q35,MasterData!Q37,MasterData!Q38)</f>
         <v>0.6889268514629594</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P18" s="6">
+        <f>STDEV(MasterData!R32,MasterData!R35,MasterData!R37,MasterData!R38)</f>
+        <v>0.16731804794064084</v>
+      </c>
+      <c r="Q18" s="6">
+        <f>STDEV(MasterData!S32,MasterData!S35,MasterData!S37,MasterData!S38)</f>
+        <v>0.16717714157942368</v>
+      </c>
+      <c r="R18" s="6">
+        <f>STDEV(MasterData!T32,MasterData!T35,MasterData!T37,MasterData!T38)</f>
+        <v>0.17916641007733622</v>
+      </c>
+      <c r="S18" s="6">
+        <f>STDEV(MasterData!U32,MasterData!U35,MasterData!U37,MasterData!U38)</f>
+        <v>0.3480037487824903</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -6144,8 +7420,24 @@
         <f>AVERAGE(MasterData!Q43,MasterData!Q44,MasterData!Q46,MasterData!Q49)</f>
         <v>5.785425</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P19" s="6">
+        <f>AVERAGE(MasterData!R43,MasterData!R44,MasterData!R46,MasterData!R49)</f>
+        <v>-0.2349</v>
+      </c>
+      <c r="Q19" s="6">
+        <f>AVERAGE(MasterData!S43,MasterData!S44,MasterData!S46,MasterData!S49)</f>
+        <v>-8.3475000000000008E-2</v>
+      </c>
+      <c r="R19" s="6">
+        <f>AVERAGE(MasterData!T43,MasterData!T44,MasterData!T46,MasterData!T49)</f>
+        <v>-1.3826749999999999</v>
+      </c>
+      <c r="S19" s="6">
+        <f>AVERAGE(MasterData!U43,MasterData!U44,MasterData!U46,MasterData!U49)</f>
+        <v>-0.65444999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>44</v>
       </c>
@@ -6201,8 +7493,24 @@
         <f>STDEV(MasterData!Q43,MasterData!Q44,MasterData!Q46,MasterData!Q49)</f>
         <v>0.33181282248681515</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P20" s="6">
+        <f>STDEV(MasterData!R43,MasterData!R44,MasterData!R46,MasterData!R49)</f>
+        <v>0.15305517523647044</v>
+      </c>
+      <c r="Q20" s="6">
+        <f>STDEV(MasterData!S43,MasterData!S44,MasterData!S46,MasterData!S49)</f>
+        <v>0.15282925930593266</v>
+      </c>
+      <c r="R20" s="6">
+        <f>STDEV(MasterData!T43,MasterData!T44,MasterData!T46,MasterData!T49)</f>
+        <v>0.11264816539414514</v>
+      </c>
+      <c r="S20" s="6">
+        <f>STDEV(MasterData!U43,MasterData!U44,MasterData!U46,MasterData!U49)</f>
+        <v>0.25953236792354045</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>45</v>
       </c>
@@ -6258,8 +7566,24 @@
         <f>AVERAGE(MasterData!Q42,MasterData!Q45,MasterData!Q47,MasterData!Q48)</f>
         <v>5.8929749999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P21" s="6">
+        <f>AVERAGE(MasterData!R42,MasterData!R45,MasterData!R47,MasterData!R48)</f>
+        <v>-0.48699999999999999</v>
+      </c>
+      <c r="Q21" s="6">
+        <f>AVERAGE(MasterData!S42,MasterData!S45,MasterData!S47,MasterData!S48)</f>
+        <v>-0.33545000000000003</v>
+      </c>
+      <c r="R21" s="6">
+        <f>AVERAGE(MasterData!T42,MasterData!T45,MasterData!T47,MasterData!T48)</f>
+        <v>-1.1219250000000001</v>
+      </c>
+      <c r="S21" s="6">
+        <f>AVERAGE(MasterData!U42,MasterData!U45,MasterData!U47,MasterData!U48)</f>
+        <v>-1.195225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>46</v>
       </c>
@@ -6315,8 +7639,24 @@
         <f>STDEV(MasterData!Q42,MasterData!Q45,MasterData!Q47,MasterData!Q48)</f>
         <v>0.30888355276166224</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P22" s="6">
+        <f>STDEV(MasterData!R42,MasterData!R45,MasterData!R47,MasterData!R48)</f>
+        <v>0.10359276036480537</v>
+      </c>
+      <c r="Q22" s="6">
+        <f>STDEV(MasterData!S42,MasterData!S45,MasterData!S47,MasterData!S48)</f>
+        <v>0.10324425730599579</v>
+      </c>
+      <c r="R22" s="6">
+        <f>STDEV(MasterData!T42,MasterData!T45,MasterData!T47,MasterData!T48)</f>
+        <v>6.3582721709596501E-2</v>
+      </c>
+      <c r="S22" s="6">
+        <f>STDEV(MasterData!U42,MasterData!U45,MasterData!U47,MasterData!U48)</f>
+        <v>0.20119299813860378</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -6375,8 +7715,24 @@
         <f>AVERAGE(MasterData!Q53,MasterData!Q54,MasterData!Q56,MasterData!Q59)</f>
         <v>5.4066666666666663</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P23" s="6">
+        <f>AVERAGE(MasterData!R53,MasterData!R54,MasterData!R56,MasterData!R59)</f>
+        <v>-0.4709666666666667</v>
+      </c>
+      <c r="Q23" s="6">
+        <f>AVERAGE(MasterData!S53,MasterData!S54,MasterData!S56,MasterData!S59)</f>
+        <v>-0.31770000000000004</v>
+      </c>
+      <c r="R23" s="6">
+        <f>AVERAGE(MasterData!T53,MasterData!T54,MasterData!T56,MasterData!T59)</f>
+        <v>-1.1907000000000001</v>
+      </c>
+      <c r="S23" s="6">
+        <f>AVERAGE(MasterData!U53,MasterData!U54,MasterData!U56,MasterData!U59)</f>
+        <v>-1.1978666666666666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>44</v>
       </c>
@@ -6432,8 +7788,24 @@
         <f>STDEV(MasterData!Q53,MasterData!Q54,MasterData!Q56,MasterData!Q59)</f>
         <v>7.0237691685685194E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P24" s="6">
+        <f>STDEV(MasterData!R53,MasterData!R54,MasterData!R56,MasterData!R59)</f>
+        <v>4.8445880457819473E-2</v>
+      </c>
+      <c r="Q24" s="6">
+        <f>STDEV(MasterData!S53,MasterData!S54,MasterData!S56,MasterData!S59)</f>
+        <v>4.859660481967825E-2</v>
+      </c>
+      <c r="R24" s="6">
+        <f>STDEV(MasterData!T53,MasterData!T54,MasterData!T56,MasterData!T59)</f>
+        <v>6.2816956309582575E-2</v>
+      </c>
+      <c r="S24" s="6">
+        <f>STDEV(MasterData!U53,MasterData!U54,MasterData!U56,MasterData!U59)</f>
+        <v>0.10420299099993879</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>45</v>
       </c>
@@ -6489,8 +7861,24 @@
         <f>AVERAGE(MasterData!Q52,MasterData!Q55,MasterData!Q57,MasterData!Q58)</f>
         <v>5.6924999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P25" s="6">
+        <f>AVERAGE(MasterData!R52,MasterData!R55,MasterData!R57,MasterData!R58)</f>
+        <v>-0.62565000000000004</v>
+      </c>
+      <c r="Q25" s="6">
+        <f>AVERAGE(MasterData!S52,MasterData!S55,MasterData!S57,MasterData!S58)</f>
+        <v>-0.47245000000000004</v>
+      </c>
+      <c r="R25" s="6">
+        <f>AVERAGE(MasterData!T52,MasterData!T55,MasterData!T57,MasterData!T58)</f>
+        <v>-0.98504999999999998</v>
+      </c>
+      <c r="S25" s="6">
+        <f>AVERAGE(MasterData!U52,MasterData!U55,MasterData!U57,MasterData!U58)</f>
+        <v>-1.5402</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>46</v>
       </c>
@@ -6546,8 +7934,24 @@
         <f>STDEV(MasterData!Q52,MasterData!Q55,MasterData!Q57,MasterData!Q58)</f>
         <v>0.25591339680967579</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P26" s="6">
+        <f>STDEV(MasterData!R52,MasterData!R55,MasterData!R57,MasterData!R58)</f>
+        <v>7.6565723401532615E-2</v>
+      </c>
+      <c r="Q26" s="6">
+        <f>STDEV(MasterData!S52,MasterData!S55,MasterData!S57,MasterData!S58)</f>
+        <v>7.6376457978445972E-2</v>
+      </c>
+      <c r="R26" s="6">
+        <f>STDEV(MasterData!T52,MasterData!T55,MasterData!T57,MasterData!T58)</f>
+        <v>0.1006783161029888</v>
+      </c>
+      <c r="S26" s="6">
+        <f>STDEV(MasterData!U52,MasterData!U55,MasterData!U57,MasterData!U58)</f>
+        <v>0.21451142937692849</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -6606,8 +8010,24 @@
         <f>AVERAGE(MasterData!Q63,MasterData!Q64,MasterData!Q66,MasterData!Q69)</f>
         <v>5.0366666666666662</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P27" s="6">
+        <f>AVERAGE(MasterData!R63,MasterData!R64,MasterData!R66,MasterData!R69)</f>
+        <v>-0.42699999999999999</v>
+      </c>
+      <c r="Q27" s="6">
+        <f>AVERAGE(MasterData!S63,MasterData!S64,MasterData!S66,MasterData!S69)</f>
+        <v>-0.27573333333333333</v>
+      </c>
+      <c r="R27" s="6">
+        <f>AVERAGE(MasterData!T63,MasterData!T64,MasterData!T66,MasterData!T69)</f>
+        <v>-1.1372333333333333</v>
+      </c>
+      <c r="S27" s="6">
+        <f>AVERAGE(MasterData!U63,MasterData!U64,MasterData!U66,MasterData!U69)</f>
+        <v>-1.0742999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>44</v>
       </c>
@@ -6663,8 +8083,24 @@
         <f>STDEV(MasterData!Q63,MasterData!Q64,MasterData!Q66,MasterData!Q69)</f>
         <v>0.49571497186723495</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P28" s="6">
+        <f>STDEV(MasterData!R63,MasterData!R64,MasterData!R66,MasterData!R69)</f>
+        <v>7.3018696235963965E-2</v>
+      </c>
+      <c r="Q28" s="6">
+        <f>STDEV(MasterData!S63,MasterData!S64,MasterData!S66,MasterData!S69)</f>
+        <v>7.2919224717034214E-2</v>
+      </c>
+      <c r="R28" s="6">
+        <f>STDEV(MasterData!T63,MasterData!T64,MasterData!T66,MasterData!T69)</f>
+        <v>5.5410588639116035E-2</v>
+      </c>
+      <c r="S28" s="6">
+        <f>STDEV(MasterData!U63,MasterData!U64,MasterData!U66,MasterData!U69)</f>
+        <v>0.12176908474649875</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>45</v>
       </c>
@@ -6720,8 +8156,24 @@
         <f>AVERAGE(MasterData!Q62,MasterData!Q65,MasterData!Q67,MasterData!Q68)</f>
         <v>5.3325000000000005</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P29" s="6">
+        <f>AVERAGE(MasterData!R62,MasterData!R65,MasterData!R67,MasterData!R68)</f>
+        <v>-0.57667500000000005</v>
+      </c>
+      <c r="Q29" s="6">
+        <f>AVERAGE(MasterData!S62,MasterData!S65,MasterData!S67,MasterData!S68)</f>
+        <v>-0.42549999999999999</v>
+      </c>
+      <c r="R29" s="6">
+        <f>AVERAGE(MasterData!T62,MasterData!T65,MasterData!T67,MasterData!T68)</f>
+        <v>-0.97560000000000002</v>
+      </c>
+      <c r="S29" s="6">
+        <f>AVERAGE(MasterData!U62,MasterData!U65,MasterData!U67,MasterData!U68)</f>
+        <v>-1.3858000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>46</v>
       </c>
@@ -6777,8 +8229,24 @@
         <f>STDEV(MasterData!Q62,MasterData!Q65,MasterData!Q67,MasterData!Q68)</f>
         <v>0.59623121913119137</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P30" s="6">
+        <f>STDEV(MasterData!R62,MasterData!R65,MasterData!R67,MasterData!R68)</f>
+        <v>0.14663633872043175</v>
+      </c>
+      <c r="Q30" s="6">
+        <f>STDEV(MasterData!S62,MasterData!S65,MasterData!S67,MasterData!S68)</f>
+        <v>0.14655667845581105</v>
+      </c>
+      <c r="R30" s="6">
+        <f>STDEV(MasterData!T62,MasterData!T65,MasterData!T67,MasterData!T68)</f>
+        <v>0.12954260560397296</v>
+      </c>
+      <c r="S30" s="6">
+        <f>STDEV(MasterData!U62,MasterData!U65,MasterData!U67,MasterData!U68)</f>
+        <v>0.28750627819232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -6837,8 +8305,24 @@
         <f>AVERAGE(MasterData!Q73,MasterData!Q74,MasterData!Q76,MasterData!Q79)</f>
         <v>5.3466666666666667</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P31" s="6">
+        <f>AVERAGE(MasterData!R73,MasterData!R74,MasterData!R76,MasterData!R79)</f>
+        <v>7.3866666666666678E-2</v>
+      </c>
+      <c r="Q31" s="6">
+        <f>AVERAGE(MasterData!S73,MasterData!S74,MasterData!S76,MasterData!S79)</f>
+        <v>0.22543333333333335</v>
+      </c>
+      <c r="R31" s="6">
+        <f>AVERAGE(MasterData!T73,MasterData!T74,MasterData!T76,MasterData!T79)</f>
+        <v>-1.6487333333333334</v>
+      </c>
+      <c r="S31" s="6">
+        <f>AVERAGE(MasterData!U73,MasterData!U74,MasterData!U76,MasterData!U79)</f>
+        <v>-4.3500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>44</v>
       </c>
@@ -6894,8 +8378,24 @@
         <f>STDEV(MasterData!Q73,MasterData!Q74,MasterData!Q76,MasterData!Q79)</f>
         <v>0.71514567280613273</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P32" s="6">
+        <f>STDEV(MasterData!R73,MasterData!R74,MasterData!R76,MasterData!R79)</f>
+        <v>6.6453316947563526E-2</v>
+      </c>
+      <c r="Q32" s="6">
+        <f>STDEV(MasterData!S73,MasterData!S74,MasterData!S76,MasterData!S79)</f>
+        <v>6.667603267541744E-2</v>
+      </c>
+      <c r="R32" s="6">
+        <f>STDEV(MasterData!T73,MasterData!T74,MasterData!T76,MasterData!T79)</f>
+        <v>2.5106639228166996E-2</v>
+      </c>
+      <c r="S32" s="6">
+        <f>STDEV(MasterData!U73,MasterData!U74,MasterData!U76,MasterData!U79)</f>
+        <v>7.3500816321997398E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>45</v>
       </c>
@@ -6951,8 +8451,24 @@
         <f>AVERAGE(MasterData!Q72,MasterData!Q75,MasterData!Q77,MasterData!Q78)</f>
         <v>5.7100000000000009</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P33" s="6">
+        <f>AVERAGE(MasterData!R72,MasterData!R75,MasterData!R77,MasterData!R78)</f>
+        <v>0.1082</v>
+      </c>
+      <c r="Q33" s="6">
+        <f>AVERAGE(MasterData!S72,MasterData!S75,MasterData!S77,MasterData!S78)</f>
+        <v>0.26005</v>
+      </c>
+      <c r="R33" s="6">
+        <f>AVERAGE(MasterData!T72,MasterData!T75,MasterData!T77,MasterData!T78)</f>
+        <v>-1.6701250000000001</v>
+      </c>
+      <c r="S33" s="6">
+        <f>AVERAGE(MasterData!U72,MasterData!U75,MasterData!U77,MasterData!U78)</f>
+        <v>-3.1899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>46</v>
       </c>
@@ -7008,8 +8524,24 @@
         <f>STDEV(MasterData!Q72,MasterData!Q75,MasterData!Q77,MasterData!Q78)</f>
         <v>0.20493901531919215</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P34" s="6">
+        <f>STDEV(MasterData!R72,MasterData!R75,MasterData!R77,MasterData!R78)</f>
+        <v>5.7993160516276974E-2</v>
+      </c>
+      <c r="Q34" s="6">
+        <f>STDEV(MasterData!S72,MasterData!S75,MasterData!S77,MasterData!S78)</f>
+        <v>5.7883820422175512E-2</v>
+      </c>
+      <c r="R34" s="6">
+        <f>STDEV(MasterData!T72,MasterData!T75,MasterData!T77,MasterData!T78)</f>
+        <v>3.7854843371313319E-2</v>
+      </c>
+      <c r="S34" s="6">
+        <f>STDEV(MasterData!U72,MasterData!U75,MasterData!U77,MasterData!U78)</f>
+        <v>0.12397817012146399</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -7068,8 +8600,24 @@
         <f>AVERAGE(MasterData!Q83,MasterData!Q84,MasterData!Q86,MasterData!Q89)</f>
         <v>5.9266666666666667</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P35" s="6">
+        <f>AVERAGE(MasterData!R83,MasterData!R84,MasterData!R86,MasterData!R89)</f>
+        <v>-0.18296666666666669</v>
+      </c>
+      <c r="Q35" s="6">
+        <f>AVERAGE(MasterData!S83,MasterData!S84,MasterData!S86,MasterData!S89)</f>
+        <v>-3.2900000000000006E-2</v>
+      </c>
+      <c r="R35" s="6">
+        <f>AVERAGE(MasterData!T83,MasterData!T84,MasterData!T86,MasterData!T89)</f>
+        <v>-1.3520333333333332</v>
+      </c>
+      <c r="S35" s="6">
+        <f>AVERAGE(MasterData!U83,MasterData!U84,MasterData!U86,MasterData!U89)</f>
+        <v>-0.55896666666666661</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>44</v>
       </c>
@@ -7125,8 +8673,24 @@
         <f>STDEV(MasterData!Q83,MasterData!Q84,MasterData!Q86,MasterData!Q89)</f>
         <v>0.48521472909767821</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P36" s="6">
+        <f>STDEV(MasterData!R83,MasterData!R84,MasterData!R86,MasterData!R89)</f>
+        <v>6.3665558454578247E-2</v>
+      </c>
+      <c r="Q36" s="6">
+        <f>STDEV(MasterData!S83,MasterData!S84,MasterData!S86,MasterData!S89)</f>
+        <v>6.2996745947707503E-2</v>
+      </c>
+      <c r="R36" s="6">
+        <f>STDEV(MasterData!T83,MasterData!T84,MasterData!T86,MasterData!T89)</f>
+        <v>3.1907731560443603E-2</v>
+      </c>
+      <c r="S36" s="6">
+        <f>STDEV(MasterData!U83,MasterData!U84,MasterData!U86,MasterData!U89)</f>
+        <v>0.12826010031702531</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>45</v>
       </c>
@@ -7182,8 +8746,24 @@
         <f>AVERAGE(MasterData!Q82,MasterData!Q85,MasterData!Q87,MasterData!Q88)</f>
         <v>5.6549999999999994</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P37" s="6">
+        <f>AVERAGE(MasterData!R82,MasterData!R85,MasterData!R87,MasterData!R88)</f>
+        <v>-0.26965</v>
+      </c>
+      <c r="Q37" s="6">
+        <f>AVERAGE(MasterData!S82,MasterData!S85,MasterData!S87,MasterData!S88)</f>
+        <v>-0.11945</v>
+      </c>
+      <c r="R37" s="6">
+        <f>AVERAGE(MasterData!T82,MasterData!T85,MasterData!T87,MasterData!T88)</f>
+        <v>-1.23865</v>
+      </c>
+      <c r="S37" s="6">
+        <f>AVERAGE(MasterData!U82,MasterData!U85,MasterData!U87,MasterData!U88)</f>
+        <v>-0.73597500000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>46</v>
       </c>
@@ -7239,8 +8819,24 @@
         <f>STDEV(MasterData!Q82,MasterData!Q85,MasterData!Q87,MasterData!Q88)</f>
         <v>0.44124822945820413</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P38" s="6">
+        <f>STDEV(MasterData!R82,MasterData!R85,MasterData!R87,MasterData!R88)</f>
+        <v>0.13936889896960511</v>
+      </c>
+      <c r="Q38" s="6">
+        <f>STDEV(MasterData!S82,MasterData!S85,MasterData!S87,MasterData!S88)</f>
+        <v>0.13892138064387355</v>
+      </c>
+      <c r="R38" s="6">
+        <f>STDEV(MasterData!T82,MasterData!T85,MasterData!T87,MasterData!T88)</f>
+        <v>0.10295741838255264</v>
+      </c>
+      <c r="S38" s="6">
+        <f>STDEV(MasterData!U82,MasterData!U85,MasterData!U87,MasterData!U88)</f>
+        <v>0.27591727474009298</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -7299,8 +8895,24 @@
         <f>AVERAGE(MasterData!Q93,MasterData!Q94,MasterData!Q96,MasterData!Q99)</f>
         <v>4.8999999999999995</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P39" s="6">
+        <f>AVERAGE(MasterData!R93,MasterData!R94,MasterData!R96,MasterData!R99)</f>
+        <v>-0.19026666666666667</v>
+      </c>
+      <c r="Q39" s="6">
+        <f>AVERAGE(MasterData!S93,MasterData!S94,MasterData!S96,MasterData!S99)</f>
+        <v>-3.903333333333333E-2</v>
+      </c>
+      <c r="R39" s="6">
+        <f>AVERAGE(MasterData!T93,MasterData!T94,MasterData!T96,MasterData!T99)</f>
+        <v>-1.4090666666666667</v>
+      </c>
+      <c r="S39" s="6">
+        <f>AVERAGE(MasterData!U93,MasterData!U94,MasterData!U96,MasterData!U99)</f>
+        <v>-0.5669333333333334</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>44</v>
       </c>
@@ -7356,8 +8968,24 @@
         <f>STDEV(MasterData!Q93,MasterData!Q94,MasterData!Q96,MasterData!Q99)</f>
         <v>0.63929648833698682</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P40" s="6">
+        <f>STDEV(MasterData!R93,MasterData!R94,MasterData!R96,MasterData!R99)</f>
+        <v>5.4516266685580593E-2</v>
+      </c>
+      <c r="Q40" s="6">
+        <f>STDEV(MasterData!S93,MasterData!S94,MasterData!S96,MasterData!S99)</f>
+        <v>5.4267884916710481E-2</v>
+      </c>
+      <c r="R40" s="6">
+        <f>STDEV(MasterData!T93,MasterData!T94,MasterData!T96,MasterData!T99)</f>
+        <v>3.5208000984624718E-2</v>
+      </c>
+      <c r="S40" s="6">
+        <f>STDEV(MasterData!U93,MasterData!U94,MasterData!U96,MasterData!U99)</f>
+        <v>0.12058591681176212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>45</v>
       </c>
@@ -7413,8 +9041,24 @@
         <f>AVERAGE(MasterData!Q92,MasterData!Q95,MasterData!Q97,MasterData!Q98)</f>
         <v>5.2374999999999998</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P41" s="6">
+        <f>AVERAGE(MasterData!R92,MasterData!R95,MasterData!R97,MasterData!R98)</f>
+        <v>-0.2301</v>
+      </c>
+      <c r="Q41" s="6">
+        <f>AVERAGE(MasterData!S92,MasterData!S95,MasterData!S97,MasterData!S98)</f>
+        <v>-7.8774999999999998E-2</v>
+      </c>
+      <c r="R41" s="6">
+        <f>AVERAGE(MasterData!T92,MasterData!T95,MasterData!T97,MasterData!T98)</f>
+        <v>-1.3595999999999999</v>
+      </c>
+      <c r="S41" s="6">
+        <f>AVERAGE(MasterData!U92,MasterData!U95,MasterData!U97,MasterData!U98)</f>
+        <v>-0.68805000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>46</v>
       </c>
@@ -7470,8 +9114,24 @@
         <f>STDEV(MasterData!Q92,MasterData!Q95,MasterData!Q97,MasterData!Q98)</f>
         <v>0.59337312600645009</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P42" s="6">
+        <f>STDEV(MasterData!R92,MasterData!R95,MasterData!R97,MasterData!R98)</f>
+        <v>7.4077301966706866E-2</v>
+      </c>
+      <c r="Q42" s="6">
+        <f>STDEV(MasterData!S92,MasterData!S95,MasterData!S97,MasterData!S98)</f>
+        <v>7.392407704304918E-2</v>
+      </c>
+      <c r="R42" s="6">
+        <f>STDEV(MasterData!T92,MasterData!T95,MasterData!T97,MasterData!T98)</f>
+        <v>9.3246125924887624E-2</v>
+      </c>
+      <c r="S42" s="6">
+        <f>STDEV(MasterData!U92,MasterData!U95,MasterData!U97,MasterData!U98)</f>
+        <v>0.15847989357223369</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -7530,8 +9190,24 @@
         <f>AVERAGE(MasterData!Q103,MasterData!Q104,MasterData!Q106,MasterData!Q109)</f>
         <v>5.9874999999999998</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P43" s="6">
+        <f>AVERAGE(MasterData!R103,MasterData!R104,MasterData!R106,MasterData!R109)</f>
+        <v>-0.30126666666666663</v>
+      </c>
+      <c r="Q43" s="6">
+        <f>AVERAGE(MasterData!S103,MasterData!S104,MasterData!S106,MasterData!S109)</f>
+        <v>-0.14913333333333334</v>
+      </c>
+      <c r="R43" s="6">
+        <f>AVERAGE(MasterData!T103,MasterData!T104,MasterData!T106,MasterData!T109)</f>
+        <v>-1.2788666666666668</v>
+      </c>
+      <c r="S43" s="6">
+        <f>AVERAGE(MasterData!U103,MasterData!U104,MasterData!U106,MasterData!U109)</f>
+        <v>-0.81320000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>44</v>
       </c>
@@ -7587,8 +9263,24 @@
         <f>STDEV(MasterData!Q103,MasterData!Q104,MasterData!Q106,MasterData!Q109)</f>
         <v>0.39381679327660329</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P44" s="6">
+        <f>STDEV(MasterData!R103,MasterData!R104,MasterData!R106,MasterData!R109)</f>
+        <v>3.1021497922140147E-3</v>
+      </c>
+      <c r="Q44" s="6">
+        <f>STDEV(MasterData!S103,MasterData!S104,MasterData!S106,MasterData!S109)</f>
+        <v>3.0501366089625095E-3</v>
+      </c>
+      <c r="R44" s="6">
+        <f>STDEV(MasterData!T103,MasterData!T104,MasterData!T106,MasterData!T109)</f>
+        <v>4.2139332378827929E-2</v>
+      </c>
+      <c r="S44" s="6">
+        <f>STDEV(MasterData!U103,MasterData!U104,MasterData!U106,MasterData!U109)</f>
+        <v>1.2647529403009941E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
         <v>45</v>
       </c>
@@ -7644,8 +9336,24 @@
         <f>AVERAGE(MasterData!Q102,MasterData!Q105,MasterData!Q107,MasterData!Q108)</f>
         <v>6.08</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P45" s="6">
+        <f>AVERAGE(MasterData!R102,MasterData!R105,MasterData!R107,MasterData!R108)</f>
+        <v>-0.40744999999999998</v>
+      </c>
+      <c r="Q45" s="6">
+        <f>AVERAGE(MasterData!S102,MasterData!S105,MasterData!S107,MasterData!S108)</f>
+        <v>-0.254525</v>
+      </c>
+      <c r="R45" s="6">
+        <f>AVERAGE(MasterData!T102,MasterData!T105,MasterData!T107,MasterData!T108)</f>
+        <v>-1.248275</v>
+      </c>
+      <c r="S45" s="6">
+        <f>AVERAGE(MasterData!U102,MasterData!U105,MasterData!U107,MasterData!U108)</f>
+        <v>-1.09155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
@@ -7701,25 +9409,41 @@
         <f>STDEV(MasterData!Q102,MasterData!Q105,MasterData!Q107,MasterData!Q108)</f>
         <v>0.97454262776613942</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P46" s="6">
+        <f>STDEV(MasterData!R102,MasterData!R105,MasterData!R107,MasterData!R108)</f>
+        <v>9.7155185142122166E-2</v>
+      </c>
+      <c r="Q46" s="6">
+        <f>STDEV(MasterData!S102,MasterData!S105,MasterData!S107,MasterData!S108)</f>
+        <v>9.7202139036820207E-2</v>
+      </c>
+      <c r="R46" s="6">
+        <f>STDEV(MasterData!T102,MasterData!T105,MasterData!T107,MasterData!T108)</f>
+        <v>0.17238181216899498</v>
+      </c>
+      <c r="S46" s="6">
+        <f>STDEV(MasterData!U102,MasterData!U105,MasterData!U107,MasterData!U108)</f>
+        <v>0.20095599020681087</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>52</v>
       </c>
       <c r="C50" s="6">
-        <f>AVERAGE(C3,C7,C15,C19,C23,C27,C31,C35,C39,C43)</f>
+        <f t="shared" ref="C50:F53" si="0">AVERAGE(C3,C7,C15,C19,C23,C27,C31,C35,C39,C43)</f>
         <v>14.445000000000002</v>
       </c>
       <c r="D50" s="6">
-        <f>AVERAGE(D3,D7,D15,D19,D23,D27,D31,D35,D39,D43)</f>
+        <f t="shared" si="0"/>
         <v>638.83916666666664</v>
       </c>
       <c r="E50" s="6">
-        <f>AVERAGE(E3,E7,E15,E19,E23,E27,E31,E35,E39,E43)</f>
+        <f t="shared" si="0"/>
         <v>31.772500000000001</v>
       </c>
       <c r="F50" s="6">
-        <f>AVERAGE(F3,F7,F15,F19,F23,F27,F31,F35,F39,F43)</f>
+        <f t="shared" si="0"/>
         <v>6.8778333333333332</v>
       </c>
       <c r="G50" s="6">
@@ -7727,11 +9451,11 @@
         <v>339.82291666666669</v>
       </c>
       <c r="H50" s="6">
-        <f>AVERAGE(H3,H7,H11,H15,H19,H23,H27,H35,H39,H43)</f>
+        <f t="shared" ref="H50:I53" si="1">AVERAGE(H3,H7,H11,H15,H19,H23,H27,H35,H39,H43)</f>
         <v>2.2681804146595281</v>
       </c>
       <c r="I50" s="6">
-        <f>AVERAGE(I3,I7,I11,I15,I19,I23,I27,I35,I39,I43)</f>
+        <f t="shared" si="1"/>
         <v>41.558382751948457</v>
       </c>
       <c r="J50" s="6">
@@ -7739,44 +9463,60 @@
         <v>0.83965206511880164</v>
       </c>
       <c r="K50" s="6">
-        <f>AVERAGE(K3,K7,K11,K15,K19,K23,K27,K31,K35,K39,K43)</f>
+        <f t="shared" ref="K50:O53" si="2">AVERAGE(K3,K7,K11,K15,K19,K23,K27,K31,K35,K39,K43)</f>
         <v>116.07990151515151</v>
       </c>
       <c r="L50" s="6">
-        <f>AVERAGE(L3,L7,L11,L15,L19,L23,L27,L31,L35,L39,L43)</f>
+        <f t="shared" si="2"/>
         <v>1.1139378787878789</v>
       </c>
       <c r="M50" s="6" t="e">
-        <f>AVERAGE(M3,M7,M11,M15,M19,M23,M27,M31,M35,M39,M43)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N50" s="6">
-        <f>AVERAGE(N3,N7,N11,N15,N19,N23,N27,N31,N35,N39,N43)</f>
+        <f t="shared" si="2"/>
         <v>22.509100757575755</v>
       </c>
       <c r="O50" s="6">
-        <f>AVERAGE(O3,O7,O11,O15,O19,O23,O27,O31,O35,O39,O43)</f>
+        <f t="shared" si="2"/>
         <v>5.5710128787878785</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P50" s="6">
+        <f t="shared" ref="P50:S50" si="3">AVERAGE(P3,P7,P11,P15,P19,P23,P27,P31,P35,P39,P43)</f>
+        <v>-0.22837500000000002</v>
+      </c>
+      <c r="Q50" s="6">
+        <f t="shared" si="3"/>
+        <v>-7.7444696969696969E-2</v>
+      </c>
+      <c r="R50" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.3499893939393939</v>
+      </c>
+      <c r="S50" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.65338333333333332</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>44</v>
       </c>
       <c r="C51" s="6">
-        <f>AVERAGE(C4,C8,C16,C20,C24,C28,C32,C36,C40,C44)</f>
+        <f t="shared" si="0"/>
         <v>0.30000969249146625</v>
       </c>
       <c r="D51" s="6">
-        <f>AVERAGE(D4,D8,D16,D20,D24,D28,D32,D36,D40,D44)</f>
+        <f t="shared" si="0"/>
         <v>7.5870957282340425</v>
       </c>
       <c r="E51" s="6">
-        <f>AVERAGE(E4,E8,E16,E20,E24,E28,E32,E36,E40,E44)</f>
+        <f t="shared" si="0"/>
         <v>3.2815243088606332</v>
       </c>
       <c r="F51" s="6">
-        <f>AVERAGE(F4,F8,F16,F20,F24,F28,F32,F36,F40,F44)</f>
+        <f t="shared" si="0"/>
         <v>5.247865207987943E-2</v>
       </c>
       <c r="G51" s="6">
@@ -7784,11 +9524,11 @@
         <v>6.9148050649372719</v>
       </c>
       <c r="H51" s="6">
-        <f>AVERAGE(H4,H8,H12,H16,H20,H24,H28,H36,H40,H44)</f>
+        <f t="shared" si="1"/>
         <v>0.15055190029363763</v>
       </c>
       <c r="I51" s="6">
-        <f>AVERAGE(I4,I8,I12,I16,I20,I24,I28,I36,I40,I44)</f>
+        <f t="shared" si="1"/>
         <v>1.3455148551585014</v>
       </c>
       <c r="J51" s="6">
@@ -7796,44 +9536,60 @@
         <v>0.11796722679571951</v>
       </c>
       <c r="K51" s="6">
-        <f>AVERAGE(K4,K8,K12,K16,K20,K24,K28,K32,K36,K40,K44)</f>
+        <f t="shared" si="2"/>
         <v>8.6571466910815893</v>
       </c>
       <c r="L51" s="6">
-        <f>AVERAGE(L4,L8,L12,L16,L20,L24,L28,L32,L36,L40,L44)</f>
+        <f t="shared" si="2"/>
         <v>0.22824962348669156</v>
       </c>
       <c r="M51" s="6" t="e">
-        <f>AVERAGE(M4,M8,M12,M16,M20,M24,M28,M32,M36,M40,M44)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N51" s="6">
-        <f>AVERAGE(N4,N8,N12,N16,N20,N24,N28,N32,N36,N40,N44)</f>
+        <f t="shared" si="2"/>
         <v>0.87129466991843896</v>
       </c>
       <c r="O51" s="6">
-        <f>AVERAGE(O4,O8,O12,O16,O20,O24,O28,O32,O36,O40,O44)</f>
+        <f t="shared" si="2"/>
         <v>0.40937575872007875</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P51" s="6">
+        <f t="shared" ref="P51:S51" si="4">AVERAGE(P4,P8,P12,P16,P20,P24,P28,P32,P36,P40,P44)</f>
+        <v>6.0100415954949776E-2</v>
+      </c>
+      <c r="Q51" s="6">
+        <f t="shared" si="4"/>
+        <v>6.0027219063191278E-2</v>
+      </c>
+      <c r="R51" s="6">
+        <f t="shared" si="4"/>
+        <v>5.3581667549383101E-2</v>
+      </c>
+      <c r="S51" s="6">
+        <f t="shared" si="4"/>
+        <v>0.10790378934971429</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
       <c r="C52" s="6">
-        <f>AVERAGE(C5,C9,C17,C21,C25,C29,C33,C37,C41,C45)</f>
+        <f t="shared" si="0"/>
         <v>14.584999999999999</v>
       </c>
       <c r="D52" s="6">
-        <f>AVERAGE(D5,D9,D17,D21,D25,D29,D33,D37,D41,D45)</f>
+        <f t="shared" si="0"/>
         <v>633.79250000000002</v>
       </c>
       <c r="E52" s="6">
-        <f>AVERAGE(E5,E9,E17,E21,E25,E29,E33,E37,E41,E45)</f>
+        <f t="shared" si="0"/>
         <v>28.2925</v>
       </c>
       <c r="F52" s="6">
-        <f>AVERAGE(F5,F9,F17,F21,F25,F29,F33,F37,F41,F45)</f>
+        <f t="shared" si="0"/>
         <v>6.7896666666666663</v>
       </c>
       <c r="G52" s="6">
@@ -7841,11 +9597,11 @@
         <v>342.72974999999997</v>
       </c>
       <c r="H52" s="6">
-        <f>AVERAGE(H5,H9,H13,H17,H21,H25,H29,H37,H41,H45)</f>
+        <f t="shared" si="1"/>
         <v>2.3770038280002606</v>
       </c>
       <c r="I52" s="6">
-        <f>AVERAGE(I5,I9,I13,I17,I21,I25,I29,I37,I41,I45)</f>
+        <f t="shared" si="1"/>
         <v>41.412580632368282</v>
       </c>
       <c r="J52" s="6">
@@ -7853,44 +9609,60 @@
         <v>1.3358224223994233</v>
       </c>
       <c r="K52" s="6">
-        <f>AVERAGE(K5,K9,K13,K17,K21,K25,K29,K33,K37,K41,K45)</f>
+        <f t="shared" si="2"/>
         <v>118.43713636363636</v>
       </c>
       <c r="L52" s="6">
-        <f>AVERAGE(L5,L9,L13,L17,L21,L25,L29,L33,L37,L41,L45)</f>
+        <f t="shared" si="2"/>
         <v>1.227211363636364</v>
       </c>
       <c r="M52" s="6" t="e">
-        <f>AVERAGE(M5,M9,M13,M17,M21,M25,M29,M33,M37,M41,M45)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N52" s="6">
-        <f>AVERAGE(N5,N9,N13,N17,N21,N25,N29,N33,N37,N41,N45)</f>
+        <f t="shared" si="2"/>
         <v>21.807679545454548</v>
       </c>
       <c r="O52" s="6">
-        <f>AVERAGE(O5,O9,O13,O17,O21,O25,O29,O33,O37,O41,O45)</f>
+        <f t="shared" si="2"/>
         <v>5.8161363636363639</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P52" s="6">
+        <f t="shared" ref="P52:S52" si="5">AVERAGE(P5,P9,P13,P17,P21,P25,P29,P33,P37,P41,P45)</f>
+        <v>-0.29796363636363637</v>
+      </c>
+      <c r="Q52" s="6">
+        <f t="shared" si="5"/>
+        <v>-0.14712727272727272</v>
+      </c>
+      <c r="R52" s="6">
+        <f t="shared" si="5"/>
+        <v>-1.2688818181818182</v>
+      </c>
+      <c r="S52" s="6">
+        <f t="shared" si="5"/>
+        <v>-0.81399772727272723</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>46</v>
       </c>
       <c r="C53" s="6">
-        <f>AVERAGE(C6,C10,C18,C22,C26,C30,C34,C38,C42,C46)</f>
+        <f t="shared" si="0"/>
         <v>0.75966375550034204</v>
       </c>
       <c r="D53" s="6">
-        <f>AVERAGE(D6,D10,D18,D22,D26,D30,D34,D38,D42,D46)</f>
+        <f t="shared" si="0"/>
         <v>19.253439105781748</v>
       </c>
       <c r="E53" s="6">
-        <f>AVERAGE(E6,E10,E18,E22,E26,E30,E34,E38,E42,E46)</f>
+        <f t="shared" si="0"/>
         <v>3.5463388830997515</v>
       </c>
       <c r="F53" s="6">
-        <f>AVERAGE(F6,F10,F18,F22,F26,F30,F34,F38,F42,F46)</f>
+        <f t="shared" si="0"/>
         <v>0.11370416870136835</v>
       </c>
       <c r="G53" s="6">
@@ -7898,11 +9670,11 @@
         <v>13.156755877405407</v>
       </c>
       <c r="H53" s="6">
-        <f>AVERAGE(H6,H10,H14,H18,H22,H26,H30,H38,H42,H46)</f>
+        <f t="shared" si="1"/>
         <v>0.25134488622937445</v>
       </c>
       <c r="I53" s="6">
-        <f>AVERAGE(I6,I10,I14,I18,I22,I26,I30,I38,I42,I46)</f>
+        <f t="shared" si="1"/>
         <v>1.6536224169239564</v>
       </c>
       <c r="J53" s="6">
@@ -7910,24 +9682,40 @@
         <v>0.38887673083033336</v>
       </c>
       <c r="K53" s="6">
-        <f>AVERAGE(K6,K10,K14,K18,K22,K26,K30,K34,K38,K42,K46)</f>
+        <f t="shared" si="2"/>
         <v>9.7081405781464589</v>
       </c>
       <c r="L53" s="6">
-        <f>AVERAGE(L6,L10,L14,L18,L22,L26,L30,L34,L38,L42,L46)</f>
+        <f t="shared" si="2"/>
         <v>0.15946162531564642</v>
       </c>
       <c r="M53" s="6" t="e">
-        <f>AVERAGE(M6,M10,M14,M18,M22,M26,M30,M34,M38,M42,M46)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N53" s="6">
-        <f>AVERAGE(N6,N10,N14,N18,N22,N26,N30,N34,N38,N42,N46)</f>
+        <f t="shared" si="2"/>
         <v>0.92474577139431036</v>
       </c>
       <c r="O53" s="6">
-        <f>AVERAGE(O6,O10,O14,O18,O22,O26,O30,O34,O38,O42,O46)</f>
+        <f t="shared" si="2"/>
         <v>0.51248071237121295</v>
+      </c>
+      <c r="P53" s="6">
+        <f t="shared" ref="P53:S53" si="6">AVERAGE(P6,P10,P14,P18,P22,P26,P30,P34,P38,P42,P46)</f>
+        <v>0.10284797639809687</v>
+      </c>
+      <c r="Q53" s="6">
+        <f t="shared" si="6"/>
+        <v>0.10268186633645048</v>
+      </c>
+      <c r="R53" s="6">
+        <f t="shared" si="6"/>
+        <v>0.10475767739831561</v>
+      </c>
+      <c r="S53" s="6">
+        <f t="shared" si="6"/>
+        <v>0.21368995401730995</v>
       </c>
     </row>
   </sheetData>
@@ -7943,15 +9731,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7994,8 +9782,20 @@
       <c r="N1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -8051,8 +9851,24 @@
         <f>AVERAGE(MasterData!Q2:Q9)</f>
         <v>5.9494125000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <f>AVERAGE(MasterData!R2:R9)</f>
+        <v>-0.1545</v>
+      </c>
+      <c r="P2">
+        <f>AVERAGE(MasterData!S2:S9)</f>
+        <v>-3.4375000000000031E-3</v>
+      </c>
+      <c r="Q2">
+        <f>AVERAGE(MasterData!T2:T9)</f>
+        <v>-1.4134000000000002</v>
+      </c>
+      <c r="R2">
+        <f>AVERAGE(MasterData!U2:U9)</f>
+        <v>-0.51118750000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -8108,8 +9924,24 @@
         <f>STDEV(MasterData!Q2:Q9)</f>
         <v>0.63423056068526285</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3">
+        <f>STDEV(MasterData!R2:R9)</f>
+        <v>8.3490221839788797E-2</v>
+      </c>
+      <c r="P3">
+        <f>STDEV(MasterData!S2:S9)</f>
+        <v>8.2997004033708521E-2</v>
+      </c>
+      <c r="Q3">
+        <f>STDEV(MasterData!T2:T9)</f>
+        <v>0.10053022288986384</v>
+      </c>
+      <c r="R3">
+        <f>STDEV(MasterData!U2:U9)</f>
+        <v>0.18274729966736639</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -8165,8 +9997,24 @@
         <f>AVERAGE(MasterData!Q12:Q19)</f>
         <v>6.0042375000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <f>AVERAGE(MasterData!R12:R19)</f>
+        <v>-0.16927500000000001</v>
+      </c>
+      <c r="P4">
+        <f>AVERAGE(MasterData!S12:S19)</f>
+        <v>-1.79875E-2</v>
+      </c>
+      <c r="Q4">
+        <f>AVERAGE(MasterData!T12:T19)</f>
+        <v>-1.4288875000000001</v>
+      </c>
+      <c r="R4">
+        <f>AVERAGE(MasterData!U12:U19)</f>
+        <v>-0.54759999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -8222,13 +10070,29 @@
         <f>STDEV(MasterData!Q12:Q19)</f>
         <v>0.45952065999722563</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <f>STDEV(MasterData!R12:R19)</f>
+        <v>0.13389919182515089</v>
+      </c>
+      <c r="P5">
+        <f>STDEV(MasterData!S12:S19)</f>
+        <v>0.13357066013911889</v>
+      </c>
+      <c r="Q5">
+        <f>STDEV(MasterData!T12:T19)</f>
+        <v>0.10856006155251438</v>
+      </c>
+      <c r="R5">
+        <f>STDEV(MasterData!U12:U19)</f>
+        <v>0.25619724544075134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -8284,8 +10148,24 @@
         <f>AVERAGE(MasterData!Q32:Q39)</f>
         <v>5.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <f>AVERAGE(MasterData!R32:R39)</f>
+        <v>-0.48096250000000002</v>
+      </c>
+      <c r="P7">
+        <f>AVERAGE(MasterData!S32:S39)</f>
+        <v>-0.32897500000000002</v>
+      </c>
+      <c r="Q7">
+        <f>AVERAGE(MasterData!T32:T39)</f>
+        <v>-1.15835</v>
+      </c>
+      <c r="R7">
+        <f>AVERAGE(MasterData!U32:U39)</f>
+        <v>-1.1800499999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -8341,8 +10221,24 @@
         <f>STDEV(MasterData!Q32:Q39)</f>
         <v>0.51644000066388573</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <f>STDEV(MasterData!R32:R39)</f>
+        <v>0.18780057764630456</v>
+      </c>
+      <c r="P8">
+        <f>STDEV(MasterData!S32:S39)</f>
+        <v>0.18786640199886723</v>
+      </c>
+      <c r="Q8">
+        <f>STDEV(MasterData!T32:T39)</f>
+        <v>0.19720686745503715</v>
+      </c>
+      <c r="R8">
+        <f>STDEV(MasterData!U32:U39)</f>
+        <v>0.38500206307425011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -8398,8 +10294,24 @@
         <f>AVERAGE(MasterData!Q42:Q49)</f>
         <v>5.8391999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <f>AVERAGE(MasterData!R42:R49)</f>
+        <v>-0.36094999999999999</v>
+      </c>
+      <c r="P9">
+        <f>AVERAGE(MasterData!S42:S49)</f>
+        <v>-0.2094625</v>
+      </c>
+      <c r="Q9">
+        <f>AVERAGE(MasterData!T42:T49)</f>
+        <v>-1.2523</v>
+      </c>
+      <c r="R9">
+        <f>AVERAGE(MasterData!U42:U49)</f>
+        <v>-0.92483749999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -8455,8 +10367,24 @@
         <f>STDEV(MasterData!Q42:Q49)</f>
         <v>0.30229134480308423</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <f>STDEV(MasterData!R42:R49)</f>
+        <v>0.18110015382181682</v>
+      </c>
+      <c r="P10">
+        <f>STDEV(MasterData!S42:S49)</f>
+        <v>0.18088326099211852</v>
+      </c>
+      <c r="Q10">
+        <f>STDEV(MasterData!T42:T49)</f>
+        <v>0.16308553408739759</v>
+      </c>
+      <c r="R10">
+        <f>STDEV(MasterData!U42:U49)</f>
+        <v>0.36023449084291903</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -8512,8 +10440,24 @@
         <f>AVERAGE(MasterData!Q52:Q59)</f>
         <v>5.5699999999999994</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <f>AVERAGE(MasterData!R52:R59)</f>
+        <v>-0.55935714285714289</v>
+      </c>
+      <c r="P11">
+        <f>AVERAGE(MasterData!S52:S59)</f>
+        <v>-0.40612857142857145</v>
+      </c>
+      <c r="Q11">
+        <f>AVERAGE(MasterData!T52:T59)</f>
+        <v>-1.0731857142857142</v>
+      </c>
+      <c r="R11">
+        <f>AVERAGE(MasterData!U52:U59)</f>
+        <v>-1.393485714285714</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -8569,8 +10513,24 @@
         <f>STDEV(MasterData!Q52:Q59)</f>
         <v>0.24027761721253449</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <f>STDEV(MasterData!R52:R59)</f>
+        <v>0.10271200606782128</v>
+      </c>
+      <c r="P12">
+        <f>STDEV(MasterData!S52:S59)</f>
+        <v>0.10269397441404424</v>
+      </c>
+      <c r="Q12">
+        <f>STDEV(MasterData!T52:T59)</f>
+        <v>0.13589257311778066</v>
+      </c>
+      <c r="R12">
+        <f>STDEV(MasterData!U52:U59)</f>
+        <v>0.24517434224493936</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -8626,8 +10586,24 @@
         <f>AVERAGE(MasterData!Q62:Q69)</f>
         <v>5.2057142857142864</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13">
+        <f>AVERAGE(MasterData!R62:R69)</f>
+        <v>-0.51252857142857144</v>
+      </c>
+      <c r="P13">
+        <f>AVERAGE(MasterData!S62:S69)</f>
+        <v>-0.36131428571428564</v>
+      </c>
+      <c r="Q13">
+        <f>AVERAGE(MasterData!T62:T69)</f>
+        <v>-1.0448714285714287</v>
+      </c>
+      <c r="R13">
+        <f>AVERAGE(MasterData!U62:U69)</f>
+        <v>-1.2523</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -8683,8 +10659,24 @@
         <f>STDEV(MasterData!Q62:Q69)</f>
         <v>0.53353716343091306</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14">
+        <f>STDEV(MasterData!R62:R69)</f>
+        <v>0.13758305024342807</v>
+      </c>
+      <c r="P14">
+        <f>STDEV(MasterData!S62:S69)</f>
+        <v>0.13755152281444019</v>
+      </c>
+      <c r="Q14">
+        <f>STDEV(MasterData!T62:T69)</f>
+        <v>0.12991716225202499</v>
+      </c>
+      <c r="R14">
+        <f>STDEV(MasterData!U62:U69)</f>
+        <v>0.27202205792913225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -8740,8 +10732,24 @@
         <f>AVERAGE(MasterData!Q72:Q79)</f>
         <v>5.5542857142857143</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15">
+        <f>AVERAGE(MasterData!R72:R79)</f>
+        <v>9.3485714285714269E-2</v>
+      </c>
+      <c r="P15">
+        <f>AVERAGE(MasterData!S72:S79)</f>
+        <v>0.24521428571428569</v>
+      </c>
+      <c r="Q15">
+        <f>AVERAGE(MasterData!T72:T79)</f>
+        <v>-1.6609571428571428</v>
+      </c>
+      <c r="R15">
+        <f>AVERAGE(MasterData!U72:U79)</f>
+        <v>-3.6871428571428576E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -8797,13 +10805,29 @@
         <f>STDEV(MasterData!Q72:Q79)</f>
         <v>0.47874339483196876</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16">
+        <f>STDEV(MasterData!R72:R79)</f>
+        <v>5.9079704032530773E-2</v>
+      </c>
+      <c r="P16">
+        <f>STDEV(MasterData!S72:S79)</f>
+        <v>5.9156922068101567E-2</v>
+      </c>
+      <c r="Q16">
+        <f>STDEV(MasterData!T72:T79)</f>
+        <v>3.2516962606351424E-2</v>
+      </c>
+      <c r="R16">
+        <f>STDEV(MasterData!U72:U79)</f>
+        <v>9.7593693687753461E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -8859,8 +10883,24 @@
         <f>AVERAGE(MasterData!Q82:Q89)</f>
         <v>5.7714285714285714</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18">
+        <f>AVERAGE(MasterData!R82:R89)</f>
+        <v>-0.23249999999999998</v>
+      </c>
+      <c r="P18">
+        <f>AVERAGE(MasterData!S82:S89)</f>
+        <v>-8.2357142857142865E-2</v>
+      </c>
+      <c r="Q18">
+        <f>AVERAGE(MasterData!T82:T89)</f>
+        <v>-1.2872428571428571</v>
+      </c>
+      <c r="R18">
+        <f>AVERAGE(MasterData!U82:U89)</f>
+        <v>-0.66011428571428576</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -8916,8 +10956,24 @@
         <f>STDEV(MasterData!Q82:Q89)</f>
         <v>0.44375025150898306</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19">
+        <f>STDEV(MasterData!R82:R89)</f>
+        <v>0.11493390854457759</v>
+      </c>
+      <c r="P19">
+        <f>STDEV(MasterData!S82:S89)</f>
+        <v>0.11451068155624694</v>
+      </c>
+      <c r="Q19">
+        <f>STDEV(MasterData!T82:T89)</f>
+        <v>9.6501621007850702E-2</v>
+      </c>
+      <c r="R19">
+        <f>STDEV(MasterData!U82:U89)</f>
+        <v>0.22913032993307136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -8973,8 +11029,24 @@
         <f>AVERAGE(MasterData!Q92:Q99)</f>
         <v>5.0928571428571425</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20">
+        <f>AVERAGE(MasterData!R92:R99)</f>
+        <v>-0.21302857142857143</v>
+      </c>
+      <c r="P20">
+        <f>AVERAGE(MasterData!S92:S99)</f>
+        <v>-6.1742857142857148E-2</v>
+      </c>
+      <c r="Q20">
+        <f>AVERAGE(MasterData!T92:T99)</f>
+        <v>-1.3808000000000002</v>
+      </c>
+      <c r="R20">
+        <f>AVERAGE(MasterData!U92:U99)</f>
+        <v>-0.63614285714285723</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -9030,8 +11102,24 @@
         <f>STDEV(MasterData!Q92:Q99)</f>
         <v>0.58721700377612707</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21">
+        <f>STDEV(MasterData!R92:R99)</f>
+        <v>6.4712742544409618E-2</v>
+      </c>
+      <c r="P21">
+        <f>STDEV(MasterData!S92:S99)</f>
+        <v>6.4539209197274211E-2</v>
+      </c>
+      <c r="Q21">
+        <f>STDEV(MasterData!T92:T99)</f>
+        <v>7.3890121125898822E-2</v>
+      </c>
+      <c r="R21">
+        <f>STDEV(MasterData!U92:U99)</f>
+        <v>0.14695625037339996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -9087,8 +11175,24 @@
         <f>AVERAGE(MasterData!Q102:Q109)</f>
         <v>6.0337499999999995</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22">
+        <f>AVERAGE(MasterData!R102:R109)</f>
+        <v>-0.36194285714285712</v>
+      </c>
+      <c r="P22">
+        <f>AVERAGE(MasterData!S102:S109)</f>
+        <v>-0.20935714285714285</v>
+      </c>
+      <c r="Q22">
+        <f>AVERAGE(MasterData!T102:T109)</f>
+        <v>-1.2613857142857143</v>
+      </c>
+      <c r="R22">
+        <f>AVERAGE(MasterData!U102:U109)</f>
+        <v>-0.97225714285714282</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -9144,8 +11248,24 @@
         <f>STDEV(MasterData!Q102:Q109)</f>
         <v>0.68988482475596835</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23">
+        <f>STDEV(MasterData!R102:R109)</f>
+        <v>8.9130089516071306E-2</v>
+      </c>
+      <c r="P23">
+        <f>STDEV(MasterData!S102:S109)</f>
+        <v>8.8886291727931013E-2</v>
+      </c>
+      <c r="Q23">
+        <f>STDEV(MasterData!T102:T109)</f>
+        <v>0.1253676118271306</v>
+      </c>
+      <c r="R23">
+        <f>STDEV(MasterData!U102:U109)</f>
+        <v>0.20586829007193636</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -9201,8 +11321,24 @@
         <f>AVERAGE(MasterData!Q2:Q109)</f>
         <v>5.7158783132530111</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25">
+        <f>AVERAGE(MasterData!R2:R109)</f>
+        <v>-0.26415000000000011</v>
+      </c>
+      <c r="P25">
+        <f>AVERAGE(MasterData!S2:S109)</f>
+        <v>-0.11331829268292684</v>
+      </c>
+      <c r="Q25">
+        <f>AVERAGE(MasterData!T2:T109)</f>
+        <v>-1.3074841463414637</v>
+      </c>
+      <c r="R25">
+        <f>AVERAGE(MasterData!U2:U109)</f>
+        <v>-0.73548780487804899</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -9257,6 +11393,22 @@
       <c r="N26">
         <f>STDEV(MasterData!Q2:Q109)</f>
         <v>0.5513366828142604</v>
+      </c>
+      <c r="O26">
+        <f>STDEV(MasterData!R2:R109)</f>
+        <v>0.23053248251347816</v>
+      </c>
+      <c r="P26">
+        <f>STDEV(MasterData!S2:S109)</f>
+        <v>0.22926391936581519</v>
+      </c>
+      <c r="Q26">
+        <f>STDEV(MasterData!T2:T109)</f>
+        <v>0.2017783385145816</v>
+      </c>
+      <c r="R26">
+        <f>STDEV(MasterData!U2:U109)</f>
+        <v>0.48976858692481623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>